<commit_message>
fixes for new input_samples folder fix for new weighting function in omega2.py
Signed-off-by: kevinanewman <newman.kevin@epa.gov>
</commit_message>
<xml_diff>
--- a/input_samples/multiple_session_batch.xlsx
+++ b/input_samples/multiple_session_batch.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\GitHub\EPA_OMEGA_Model\sample_inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7930B9E3-A0EC-4C70-BD48-2382FDB6B32E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6A81933-1631-42CB-9114-2F31928A68D9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2520" yWindow="3300" windowWidth="14160" windowHeight="16785" tabRatio="151" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="255" yWindow="3255" windowWidth="19815" windowHeight="15180" tabRatio="151" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sessions" sheetId="5" r:id="rId1"/>
@@ -150,30 +150,6 @@
     <t>Demanded Shares File</t>
   </si>
   <si>
-    <t>sample_inputs/manufacturers.csv</t>
-  </si>
-  <si>
-    <t>sample_inputs/market_classes.csv</t>
-  </si>
-  <si>
-    <t>sample_inputs/vehicles.csv</t>
-  </si>
-  <si>
-    <t>sample_inputs/demanded_shares-gcam.csv</t>
-  </si>
-  <si>
-    <t>sample_inputs/fuels.csv</t>
-  </si>
-  <si>
-    <t>sample_inputs/cost_curves.csv</t>
-  </si>
-  <si>
-    <t>sample_inputs/ghg_standards-footprint.csv</t>
-  </si>
-  <si>
-    <t>sample_inputs/ghg_standards-flat.csv</t>
-  </si>
-  <si>
     <t>ReferencePolicy</t>
   </si>
   <si>
@@ -192,22 +168,46 @@
     <t>Num Tech Options per BEV Vehicle</t>
   </si>
   <si>
-    <t>sample_inputs/fuels_context.csv</t>
-  </si>
-  <si>
     <t>GHG Standards Fuels File</t>
   </si>
   <si>
-    <t>sample_inputs/ghg_standards-fuels.csv</t>
-  </si>
-  <si>
     <t>ZEV Requirement File</t>
   </si>
   <si>
-    <t>sample_inputs/required_zev_share.csv</t>
-  </si>
-  <si>
     <t>Iterate Producer-Consumer</t>
+  </si>
+  <si>
+    <t>input_samples/market_classes.csv</t>
+  </si>
+  <si>
+    <t>input_samples/vehicles.csv</t>
+  </si>
+  <si>
+    <t>input_samples/demanded_shares-gcam.csv</t>
+  </si>
+  <si>
+    <t>input_samples/fuels.csv</t>
+  </si>
+  <si>
+    <t>input_samples/fuels_context.csv</t>
+  </si>
+  <si>
+    <t>input_samples/cost_curves.csv</t>
+  </si>
+  <si>
+    <t>input_samples/ghg_standards-footprint.csv</t>
+  </si>
+  <si>
+    <t>input_samples/ghg_standards-fuels.csv</t>
+  </si>
+  <si>
+    <t>input_samples/required_zev_share.csv</t>
+  </si>
+  <si>
+    <t>input_samples/ghg_standards-flat.csv</t>
+  </si>
+  <si>
+    <t>input_samples/manufacturers.csv</t>
   </si>
 </sst>
 </file>
@@ -703,8 +703,8 @@
   <dimension ref="A1:AG39"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="9" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A33" sqref="A33:XFD33"/>
+      <pane ySplit="9" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C21" sqref="C21:C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -788,7 +788,7 @@
         <v>3</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="D3" s="14"/>
       <c r="E3" s="14"/>
@@ -807,7 +807,7 @@
     </row>
     <row r="4" spans="1:33" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="B4" s="6" t="s">
         <v>3</v>
@@ -830,7 +830,7 @@
     </row>
     <row r="5" spans="1:33" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="B5" s="6" t="s">
         <v>3</v>
@@ -926,7 +926,7 @@
         <v>3</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="D9" s="9" t="s">
         <v>33</v>
@@ -997,10 +997,10 @@
         <v>3</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>39</v>
+        <v>58</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>39</v>
+        <v>58</v>
       </c>
       <c r="E12" s="8"/>
       <c r="F12" s="8"/>
@@ -1026,10 +1026,10 @@
         <v>3</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="E13" s="8"/>
       <c r="F13" s="8"/>
@@ -1055,10 +1055,10 @@
         <v>3</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="E14" s="8"/>
       <c r="F14" s="8"/>
@@ -1084,10 +1084,10 @@
         <v>3</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="E15" s="8"/>
       <c r="F15" s="8"/>
@@ -1113,10 +1113,10 @@
         <v>3</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="E16" s="8"/>
       <c r="F16" s="8"/>
@@ -1142,10 +1142,10 @@
         <v>3</v>
       </c>
       <c r="C17" s="8" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E17" s="8"/>
       <c r="F17" s="8"/>
@@ -1200,10 +1200,10 @@
         <v>3</v>
       </c>
       <c r="C19" s="8" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="D19" s="8" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="E19" s="8"/>
       <c r="F19" s="8"/>
@@ -1258,10 +1258,10 @@
         <v>3</v>
       </c>
       <c r="C21" s="10" t="s">
-        <v>45</v>
+        <v>54</v>
       </c>
       <c r="D21" s="10" t="s">
-        <v>46</v>
+        <v>57</v>
       </c>
       <c r="E21" s="10"/>
       <c r="F21" s="10"/>
@@ -1281,7 +1281,7 @@
     </row>
     <row r="22" spans="1:19" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="8" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>3</v>
@@ -1310,16 +1310,16 @@
     </row>
     <row r="23" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="8" t="s">
-        <v>56</v>
+        <v>46</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>3</v>
       </c>
       <c r="C23" s="8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D23" s="8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E23" s="8"/>
       <c r="F23" s="8"/>
@@ -1456,7 +1456,7 @@
     </row>
     <row r="29" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="8" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="B29" s="3" t="s">
         <v>13</v>
@@ -1485,7 +1485,7 @@
     </row>
     <row r="30" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="8" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="B30" s="3" t="s">
         <v>13</v>
@@ -1572,7 +1572,7 @@
     </row>
     <row r="33" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="8" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
       <c r="B33" s="3" t="s">
         <v>11</v>

</xml_diff>

<commit_message>
added new iteration parameters to the batch defintion file fixed a weird pandas error in the partition function... not really sure what the issue was, but it seems to work now
Signed-off-by: kevinanewman <newman.kevin@epa.gov>
</commit_message>
<xml_diff>
--- a/input_samples/multiple_session_batch.xlsx
+++ b/input_samples/multiple_session_batch.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\GitHub\EPA_OMEGA_Model\sample_inputs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\GitHub\EPA_OMEGA_Model\input_samples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6A81933-1631-42CB-9114-2F31928A68D9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2E28C8A-F8B8-410D-B525-6B8BAA8B2DE5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="255" yWindow="3255" windowWidth="19815" windowHeight="15180" tabRatio="151" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6225" yWindow="1170" windowWidth="24735" windowHeight="19170" tabRatio="151" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sessions" sheetId="5" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="62">
   <si>
     <t>Parameter</t>
   </si>
@@ -162,12 +162,6 @@
     <t>Context Folder Name</t>
   </si>
   <si>
-    <t>Num Tech Options per ICE Vehicle</t>
-  </si>
-  <si>
-    <t>Num Tech Options per BEV Vehicle</t>
-  </si>
-  <si>
     <t>GHG Standards Fuels File</t>
   </si>
   <si>
@@ -208,6 +202,21 @@
   </si>
   <si>
     <t>input_samples/manufacturers.csv</t>
+  </si>
+  <si>
+    <t>Iteration Num Tech Options per ICE Vehicle</t>
+  </si>
+  <si>
+    <t>Iteration Num Tech Options per BEV Vehicle</t>
+  </si>
+  <si>
+    <t>First Pass Num Tech Options per ICE Vehicle</t>
+  </si>
+  <si>
+    <t>First Pass Num Tech Options per BEV Vehicle</t>
+  </si>
+  <si>
+    <t>First Pass Num Market Share Options</t>
   </si>
 </sst>
 </file>
@@ -700,16 +709,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AG39"/>
+  <dimension ref="A1:AG42"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="9" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C21" sqref="C21:C23"/>
+      <pane ySplit="9" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A29" sqref="A29:XFD29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="32.42578125" style="11" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="42" style="11" customWidth="1"/>
     <col min="2" max="2" width="17.28515625" style="1" customWidth="1"/>
     <col min="3" max="4" width="48" style="11" bestFit="1" customWidth="1"/>
     <col min="5" max="17" width="21.28515625" style="11" customWidth="1"/>
@@ -997,10 +1006,10 @@
         <v>3</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E12" s="8"/>
       <c r="F12" s="8"/>
@@ -1026,10 +1035,10 @@
         <v>3</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="E13" s="8"/>
       <c r="F13" s="8"/>
@@ -1055,10 +1064,10 @@
         <v>3</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E14" s="8"/>
       <c r="F14" s="8"/>
@@ -1084,10 +1093,10 @@
         <v>3</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E15" s="8"/>
       <c r="F15" s="8"/>
@@ -1113,10 +1122,10 @@
         <v>3</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E16" s="8"/>
       <c r="F16" s="8"/>
@@ -1142,10 +1151,10 @@
         <v>3</v>
       </c>
       <c r="C17" s="8" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E17" s="8"/>
       <c r="F17" s="8"/>
@@ -1200,10 +1209,10 @@
         <v>3</v>
       </c>
       <c r="C19" s="8" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D19" s="8" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E19" s="8"/>
       <c r="F19" s="8"/>
@@ -1258,10 +1267,10 @@
         <v>3</v>
       </c>
       <c r="C21" s="10" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D21" s="10" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E21" s="10"/>
       <c r="F21" s="10"/>
@@ -1281,16 +1290,16 @@
     </row>
     <row r="22" spans="1:19" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="8" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>3</v>
       </c>
       <c r="C22" s="8" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D22" s="8" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E22" s="10"/>
       <c r="F22" s="10"/>
@@ -1310,16 +1319,16 @@
     </row>
     <row r="23" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="8" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>3</v>
       </c>
       <c r="C23" s="8" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D23" s="8" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E23" s="8"/>
       <c r="F23" s="8"/>
@@ -1456,7 +1465,7 @@
     </row>
     <row r="29" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="8" t="s">
-        <v>43</v>
+        <v>61</v>
       </c>
       <c r="B29" s="3" t="s">
         <v>13</v>
@@ -1465,7 +1474,7 @@
         <v>15</v>
       </c>
       <c r="D29" s="8">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="E29" s="8"/>
       <c r="F29" s="8"/>
@@ -1485,13 +1494,13 @@
     </row>
     <row r="30" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="8" t="s">
-        <v>44</v>
+        <v>59</v>
       </c>
       <c r="B30" s="3" t="s">
         <v>13</v>
       </c>
       <c r="C30" s="8">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="D30" s="8">
         <v>5</v>
@@ -1512,47 +1521,47 @@
       <c r="R30" s="8"/>
       <c r="S30" s="8"/>
     </row>
-    <row r="31" spans="1:19" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="10" t="s">
-        <v>29</v>
+    <row r="31" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="8" t="s">
+        <v>60</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C31" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="D31" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="E31" s="10"/>
-      <c r="F31" s="10"/>
-      <c r="G31" s="10"/>
-      <c r="H31" s="10"/>
-      <c r="I31" s="10"/>
-      <c r="J31" s="10"/>
-      <c r="K31" s="10"/>
-      <c r="L31" s="10"/>
-      <c r="M31" s="10"/>
-      <c r="N31" s="10"/>
-      <c r="O31" s="10"/>
-      <c r="P31" s="10"/>
-      <c r="Q31" s="10"/>
-      <c r="R31" s="10"/>
-      <c r="S31" s="10"/>
+        <v>13</v>
+      </c>
+      <c r="C31" s="8">
+        <v>2</v>
+      </c>
+      <c r="D31" s="8">
+        <v>5</v>
+      </c>
+      <c r="E31" s="8"/>
+      <c r="F31" s="8"/>
+      <c r="G31" s="8"/>
+      <c r="H31" s="8"/>
+      <c r="I31" s="8"/>
+      <c r="J31" s="8"/>
+      <c r="K31" s="8"/>
+      <c r="L31" s="8"/>
+      <c r="M31" s="8"/>
+      <c r="N31" s="8"/>
+      <c r="O31" s="8"/>
+      <c r="P31" s="8"/>
+      <c r="Q31" s="8"/>
+      <c r="R31" s="8"/>
+      <c r="S31" s="8"/>
     </row>
     <row r="32" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="B32" s="4" t="s">
+      <c r="A32" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="B32" s="3" t="s">
         <v>13</v>
       </c>
       <c r="C32" s="8">
-        <v>0.75</v>
+        <v>15</v>
       </c>
       <c r="D32" s="8">
-        <v>0.75</v>
+        <v>5</v>
       </c>
       <c r="E32" s="8"/>
       <c r="F32" s="8"/>
@@ -1572,16 +1581,16 @@
     </row>
     <row r="33" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="8" t="s">
-        <v>47</v>
+        <v>58</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C33" s="8" t="b">
-        <v>1</v>
-      </c>
-      <c r="D33" s="8" t="b">
-        <v>1</v>
+        <v>13</v>
+      </c>
+      <c r="C33" s="8">
+        <v>2</v>
+      </c>
+      <c r="D33" s="8">
+        <v>5</v>
       </c>
       <c r="E33" s="8"/>
       <c r="F33" s="8"/>
@@ -1599,82 +1608,98 @@
       <c r="R33" s="8"/>
       <c r="S33" s="8"/>
     </row>
-    <row r="34" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="8"/>
-      <c r="B34" s="3"/>
-      <c r="C34" s="8"/>
-      <c r="D34" s="8"/>
-      <c r="E34" s="8"/>
-      <c r="F34" s="8"/>
-      <c r="G34" s="8"/>
-      <c r="H34" s="8"/>
-      <c r="I34" s="8"/>
-      <c r="J34" s="8"/>
-      <c r="K34" s="8"/>
-      <c r="L34" s="8"/>
-      <c r="M34" s="8"/>
-      <c r="N34" s="8"/>
-      <c r="O34" s="8"/>
-      <c r="P34" s="8"/>
-      <c r="Q34" s="8"/>
-      <c r="R34" s="8"/>
-      <c r="S34" s="8"/>
-    </row>
-    <row r="35" spans="1:19" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="15"/>
-      <c r="C35" s="15"/>
-      <c r="D35" s="15"/>
-      <c r="E35" s="14"/>
-      <c r="F35" s="14"/>
-      <c r="G35" s="14"/>
-      <c r="H35" s="14"/>
-      <c r="I35" s="14"/>
-      <c r="J35" s="14"/>
-      <c r="K35" s="14"/>
-      <c r="L35" s="14"/>
-      <c r="M35" s="14"/>
-      <c r="N35" s="14"/>
-      <c r="O35" s="14"/>
-      <c r="P35" s="14"/>
-      <c r="Q35" s="14"/>
-      <c r="R35" s="14"/>
-      <c r="S35" s="14"/>
-    </row>
-    <row r="36" spans="1:19" s="12" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A36" s="20" t="s">
-        <v>7</v>
-      </c>
-      <c r="C36" s="14"/>
-      <c r="D36" s="14"/>
-      <c r="E36" s="14"/>
-      <c r="F36" s="14"/>
-      <c r="G36" s="14"/>
-      <c r="H36" s="14"/>
-      <c r="I36" s="14"/>
-      <c r="J36" s="14"/>
-      <c r="K36" s="14"/>
-      <c r="L36" s="14"/>
-      <c r="M36" s="14"/>
-      <c r="N36" s="14"/>
-      <c r="O36" s="14"/>
-      <c r="P36" s="14"/>
-      <c r="Q36" s="14"/>
-      <c r="R36" s="14"/>
-      <c r="S36" s="14"/>
-    </row>
-    <row r="37" spans="1:19" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A37" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="B37" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="C37" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="D37" s="8" t="s">
-        <v>31</v>
-      </c>
+    <row r="34" spans="1:19" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C34" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="D34" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="E34" s="10"/>
+      <c r="F34" s="10"/>
+      <c r="G34" s="10"/>
+      <c r="H34" s="10"/>
+      <c r="I34" s="10"/>
+      <c r="J34" s="10"/>
+      <c r="K34" s="10"/>
+      <c r="L34" s="10"/>
+      <c r="M34" s="10"/>
+      <c r="N34" s="10"/>
+      <c r="O34" s="10"/>
+      <c r="P34" s="10"/>
+      <c r="Q34" s="10"/>
+      <c r="R34" s="10"/>
+      <c r="S34" s="10"/>
+    </row>
+    <row r="35" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="B35" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C35" s="8">
+        <v>0.75</v>
+      </c>
+      <c r="D35" s="8">
+        <v>0.75</v>
+      </c>
+      <c r="E35" s="8"/>
+      <c r="F35" s="8"/>
+      <c r="G35" s="8"/>
+      <c r="H35" s="8"/>
+      <c r="I35" s="8"/>
+      <c r="J35" s="8"/>
+      <c r="K35" s="8"/>
+      <c r="L35" s="8"/>
+      <c r="M35" s="8"/>
+      <c r="N35" s="8"/>
+      <c r="O35" s="8"/>
+      <c r="P35" s="8"/>
+      <c r="Q35" s="8"/>
+      <c r="R35" s="8"/>
+      <c r="S35" s="8"/>
+    </row>
+    <row r="36" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="B36" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C36" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="D36" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="E36" s="8"/>
+      <c r="F36" s="8"/>
+      <c r="G36" s="8"/>
+      <c r="H36" s="8"/>
+      <c r="I36" s="8"/>
+      <c r="J36" s="8"/>
+      <c r="K36" s="8"/>
+      <c r="L36" s="8"/>
+      <c r="M36" s="8"/>
+      <c r="N36" s="8"/>
+      <c r="O36" s="8"/>
+      <c r="P36" s="8"/>
+      <c r="Q36" s="8"/>
+      <c r="R36" s="8"/>
+      <c r="S36" s="8"/>
+    </row>
+    <row r="37" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="8"/>
+      <c r="B37" s="3"/>
+      <c r="C37" s="8"/>
+      <c r="D37" s="8"/>
       <c r="E37" s="8"/>
       <c r="F37" s="8"/>
       <c r="G37" s="8"/>
@@ -1691,55 +1716,126 @@
       <c r="R37" s="8"/>
       <c r="S37" s="8"/>
     </row>
-    <row r="38" spans="1:19" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A38" s="10" t="s">
+    <row r="38" spans="1:19" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="15"/>
+      <c r="C38" s="15"/>
+      <c r="D38" s="15"/>
+      <c r="E38" s="14"/>
+      <c r="F38" s="14"/>
+      <c r="G38" s="14"/>
+      <c r="H38" s="14"/>
+      <c r="I38" s="14"/>
+      <c r="J38" s="14"/>
+      <c r="K38" s="14"/>
+      <c r="L38" s="14"/>
+      <c r="M38" s="14"/>
+      <c r="N38" s="14"/>
+      <c r="O38" s="14"/>
+      <c r="P38" s="14"/>
+      <c r="Q38" s="14"/>
+      <c r="R38" s="14"/>
+      <c r="S38" s="14"/>
+    </row>
+    <row r="39" spans="1:19" s="12" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A39" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="C39" s="14"/>
+      <c r="D39" s="14"/>
+      <c r="E39" s="14"/>
+      <c r="F39" s="14"/>
+      <c r="G39" s="14"/>
+      <c r="H39" s="14"/>
+      <c r="I39" s="14"/>
+      <c r="J39" s="14"/>
+      <c r="K39" s="14"/>
+      <c r="L39" s="14"/>
+      <c r="M39" s="14"/>
+      <c r="N39" s="14"/>
+      <c r="O39" s="14"/>
+      <c r="P39" s="14"/>
+      <c r="Q39" s="14"/>
+      <c r="R39" s="14"/>
+      <c r="S39" s="14"/>
+    </row>
+    <row r="40" spans="1:19" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A40" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="B40" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C40" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="D40" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="E40" s="8"/>
+      <c r="F40" s="8"/>
+      <c r="G40" s="8"/>
+      <c r="H40" s="8"/>
+      <c r="I40" s="8"/>
+      <c r="J40" s="8"/>
+      <c r="K40" s="8"/>
+      <c r="L40" s="8"/>
+      <c r="M40" s="8"/>
+      <c r="N40" s="8"/>
+      <c r="O40" s="8"/>
+      <c r="P40" s="8"/>
+      <c r="Q40" s="8"/>
+      <c r="R40" s="8"/>
+      <c r="S40" s="8"/>
+    </row>
+    <row r="41" spans="1:19" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A41" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="B38" s="3" t="s">
+      <c r="B41" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="C38" s="8" t="s">
+      <c r="C41" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="D38" s="8" t="s">
+      <c r="D41" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="E38" s="8"/>
-      <c r="F38" s="8"/>
-      <c r="G38" s="8"/>
-      <c r="H38" s="8"/>
-      <c r="I38" s="8"/>
-      <c r="J38" s="8"/>
-      <c r="K38" s="8"/>
-      <c r="L38" s="8"/>
-      <c r="M38" s="8"/>
-      <c r="N38" s="8"/>
-      <c r="O38" s="8"/>
-      <c r="P38" s="8"/>
-      <c r="Q38" s="8"/>
-      <c r="R38" s="8"/>
-      <c r="S38" s="8"/>
-    </row>
-    <row r="39" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="8"/>
-      <c r="B39" s="3"/>
-      <c r="C39" s="8"/>
-      <c r="D39" s="8"/>
-      <c r="E39" s="8"/>
-      <c r="F39" s="8"/>
-      <c r="G39" s="8"/>
-      <c r="H39" s="8"/>
-      <c r="I39" s="8"/>
-      <c r="J39" s="8"/>
-      <c r="K39" s="8"/>
-      <c r="L39" s="8"/>
-      <c r="M39" s="8"/>
-      <c r="N39" s="8"/>
-      <c r="O39" s="8"/>
-      <c r="P39" s="8"/>
-      <c r="Q39" s="8"/>
-      <c r="R39" s="8"/>
-      <c r="S39" s="8"/>
+      <c r="E41" s="8"/>
+      <c r="F41" s="8"/>
+      <c r="G41" s="8"/>
+      <c r="H41" s="8"/>
+      <c r="I41" s="8"/>
+      <c r="J41" s="8"/>
+      <c r="K41" s="8"/>
+      <c r="L41" s="8"/>
+      <c r="M41" s="8"/>
+      <c r="N41" s="8"/>
+      <c r="O41" s="8"/>
+      <c r="P41" s="8"/>
+      <c r="Q41" s="8"/>
+      <c r="R41" s="8"/>
+      <c r="S41" s="8"/>
+    </row>
+    <row r="42" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="8"/>
+      <c r="B42" s="3"/>
+      <c r="C42" s="8"/>
+      <c r="D42" s="8"/>
+      <c r="E42" s="8"/>
+      <c r="F42" s="8"/>
+      <c r="G42" s="8"/>
+      <c r="H42" s="8"/>
+      <c r="I42" s="8"/>
+      <c r="J42" s="8"/>
+      <c r="K42" s="8"/>
+      <c r="L42" s="8"/>
+      <c r="M42" s="8"/>
+      <c r="N42" s="8"/>
+      <c r="O42" s="8"/>
+      <c r="P42" s="8"/>
+      <c r="Q42" s="8"/>
+      <c r="R42" s="8"/>
+      <c r="S42" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
fuels_context.py updates for latest file format and default file name
Signed-off-by: kevinanewman <newman.kevin@epa.gov>
</commit_message>
<xml_diff>
--- a/input_samples/multiple_session_batch.xlsx
+++ b/input_samples/multiple_session_batch.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\GitHub\EPA_OMEGA_Model\input_samples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2E28C8A-F8B8-410D-B525-6B8BAA8B2DE5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53C7D8E1-C525-4497-85AE-CAC84689FD74}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6225" yWindow="1170" windowWidth="24735" windowHeight="19170" tabRatio="151" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5355" yWindow="3510" windowWidth="15975" windowHeight="12885" tabRatio="151" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sessions" sheetId="5" r:id="rId1"/>
@@ -183,9 +183,6 @@
     <t>input_samples/fuels.csv</t>
   </si>
   <si>
-    <t>input_samples/fuels_context.csv</t>
-  </si>
-  <si>
     <t>input_samples/cost_curves.csv</t>
   </si>
   <si>
@@ -217,6 +214,9 @@
   </si>
   <si>
     <t>First Pass Num Market Share Options</t>
+  </si>
+  <si>
+    <t>input_samples/context_fuel_prices.csv</t>
   </si>
 </sst>
 </file>
@@ -712,8 +712,8 @@
   <dimension ref="A1:AG42"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="9" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A29" sqref="A29:XFD29"/>
+      <pane ySplit="9" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1006,10 +1006,10 @@
         <v>3</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E12" s="8"/>
       <c r="F12" s="8"/>
@@ -1151,10 +1151,10 @@
         <v>3</v>
       </c>
       <c r="C17" s="8" t="s">
-        <v>50</v>
+        <v>61</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>50</v>
+        <v>61</v>
       </c>
       <c r="E17" s="8"/>
       <c r="F17" s="8"/>
@@ -1209,10 +1209,10 @@
         <v>3</v>
       </c>
       <c r="C19" s="8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D19" s="8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E19" s="8"/>
       <c r="F19" s="8"/>
@@ -1267,10 +1267,10 @@
         <v>3</v>
       </c>
       <c r="C21" s="10" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D21" s="10" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E21" s="10"/>
       <c r="F21" s="10"/>
@@ -1296,10 +1296,10 @@
         <v>3</v>
       </c>
       <c r="C22" s="8" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D22" s="8" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E22" s="10"/>
       <c r="F22" s="10"/>
@@ -1325,10 +1325,10 @@
         <v>3</v>
       </c>
       <c r="C23" s="8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D23" s="8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E23" s="8"/>
       <c r="F23" s="8"/>
@@ -1465,7 +1465,7 @@
     </row>
     <row r="29" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B29" s="3" t="s">
         <v>13</v>
@@ -1494,7 +1494,7 @@
     </row>
     <row r="30" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="8" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B30" s="3" t="s">
         <v>13</v>
@@ -1523,7 +1523,7 @@
     </row>
     <row r="31" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="8" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B31" s="3" t="s">
         <v>13</v>
@@ -1552,7 +1552,7 @@
     </row>
     <row r="32" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B32" s="3" t="s">
         <v>13</v>
@@ -1581,7 +1581,7 @@
     </row>
     <row r="33" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="8" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B33" s="3" t="s">
         <v>13</v>

</xml_diff>

<commit_message>
added Context New Vehicle Market File to batch definition renamed Fuel Scenario Annual Data to Context Fuel Prices in batch definition refactor of options.fuels_context_file to options.context_fuel_prices_file slightly better init fail handling
Signed-off-by: kevinanewman <newman.kevin@epa.gov>
</commit_message>
<xml_diff>
--- a/input_samples/multiple_session_batch.xlsx
+++ b/input_samples/multiple_session_batch.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\GitHub\EPA_OMEGA_Model\input_samples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53C7D8E1-C525-4497-85AE-CAC84689FD74}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42847E73-E4ED-440D-8B86-712912D9773D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5355" yWindow="3510" windowWidth="15975" windowHeight="12885" tabRatio="151" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3030" yWindow="465" windowWidth="20115" windowHeight="19695" tabRatio="151" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sessions" sheetId="5" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="65">
   <si>
     <t>Parameter</t>
   </si>
@@ -217,6 +217,15 @@
   </si>
   <si>
     <t>input_samples/context_fuel_prices.csv</t>
+  </si>
+  <si>
+    <t>Context Fuel Prices File</t>
+  </si>
+  <si>
+    <t>Context New Vehicle Market File</t>
+  </si>
+  <si>
+    <t>input_samples/context_new_vehicle_market.csv</t>
   </si>
 </sst>
 </file>
@@ -709,7 +718,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AG42"/>
+  <dimension ref="A1:AG44"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane ySplit="9" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
@@ -1145,7 +1154,7 @@
     </row>
     <row r="17" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="8" t="s">
-        <v>18</v>
+        <v>62</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>3</v>
@@ -1172,18 +1181,18 @@
       <c r="R17" s="8"/>
       <c r="S17" s="8"/>
     </row>
-    <row r="18" spans="1:19" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>36</v>
+        <v>63</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>3</v>
       </c>
       <c r="C18" s="8" t="s">
-        <v>37</v>
+        <v>64</v>
       </c>
       <c r="D18" s="8" t="s">
-        <v>37</v>
+        <v>64</v>
       </c>
       <c r="E18" s="8"/>
       <c r="F18" s="8"/>
@@ -1203,16 +1212,16 @@
     </row>
     <row r="19" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="8" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>3</v>
       </c>
       <c r="C19" s="8" t="s">
-        <v>50</v>
+        <v>61</v>
       </c>
       <c r="D19" s="8" t="s">
-        <v>50</v>
+        <v>61</v>
       </c>
       <c r="E19" s="8"/>
       <c r="F19" s="8"/>
@@ -1230,76 +1239,76 @@
       <c r="R19" s="8"/>
       <c r="S19" s="8"/>
     </row>
-    <row r="20" spans="1:19" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A20" s="10" t="s">
-        <v>23</v>
+    <row r="20" spans="1:19" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A20" s="8" t="s">
+        <v>21</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C20" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="D20" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="E20" s="10"/>
-      <c r="F20" s="10"/>
-      <c r="G20" s="10"/>
-      <c r="H20" s="10"/>
-      <c r="I20" s="10"/>
-      <c r="J20" s="10"/>
-      <c r="K20" s="10"/>
-      <c r="L20" s="10"/>
-      <c r="M20" s="10"/>
-      <c r="N20" s="10"/>
-      <c r="O20" s="10"/>
-      <c r="P20" s="10"/>
-      <c r="Q20" s="10"/>
-      <c r="R20" s="10"/>
-      <c r="S20" s="10"/>
-    </row>
-    <row r="21" spans="1:19" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="10" t="s">
-        <v>22</v>
+        <v>36</v>
+      </c>
+      <c r="C20" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="D20" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="E20" s="8"/>
+      <c r="F20" s="8"/>
+      <c r="G20" s="8"/>
+      <c r="H20" s="8"/>
+      <c r="I20" s="8"/>
+      <c r="J20" s="8"/>
+      <c r="K20" s="8"/>
+      <c r="L20" s="8"/>
+      <c r="M20" s="8"/>
+      <c r="N20" s="8"/>
+      <c r="O20" s="8"/>
+      <c r="P20" s="8"/>
+      <c r="Q20" s="8"/>
+      <c r="R20" s="8"/>
+      <c r="S20" s="8"/>
+    </row>
+    <row r="21" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="8" t="s">
+        <v>20</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C21" s="10" t="s">
-        <v>51</v>
-      </c>
-      <c r="D21" s="10" t="s">
-        <v>54</v>
-      </c>
-      <c r="E21" s="10"/>
-      <c r="F21" s="10"/>
-      <c r="G21" s="10"/>
-      <c r="H21" s="10"/>
-      <c r="I21" s="10"/>
-      <c r="J21" s="10"/>
-      <c r="K21" s="10"/>
-      <c r="L21" s="10"/>
-      <c r="M21" s="10"/>
-      <c r="N21" s="10"/>
-      <c r="O21" s="10"/>
-      <c r="P21" s="10"/>
-      <c r="Q21" s="10"/>
-      <c r="R21" s="10"/>
-      <c r="S21" s="10"/>
-    </row>
-    <row r="22" spans="1:19" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C22" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="D22" s="8" t="s">
-        <v>52</v>
+      <c r="C21" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="D21" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="E21" s="8"/>
+      <c r="F21" s="8"/>
+      <c r="G21" s="8"/>
+      <c r="H21" s="8"/>
+      <c r="I21" s="8"/>
+      <c r="J21" s="8"/>
+      <c r="K21" s="8"/>
+      <c r="L21" s="8"/>
+      <c r="M21" s="8"/>
+      <c r="N21" s="8"/>
+      <c r="O21" s="8"/>
+      <c r="P21" s="8"/>
+      <c r="Q21" s="8"/>
+      <c r="R21" s="8"/>
+      <c r="S21" s="8"/>
+    </row>
+    <row r="22" spans="1:19" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A22" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C22" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="D22" s="10" t="s">
+        <v>35</v>
       </c>
       <c r="E22" s="10"/>
       <c r="F22" s="10"/>
@@ -1317,47 +1326,47 @@
       <c r="R22" s="10"/>
       <c r="S22" s="10"/>
     </row>
-    <row r="23" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="8" t="s">
-        <v>44</v>
+    <row r="23" spans="1:19" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="10" t="s">
+        <v>22</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C23" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="D23" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="E23" s="8"/>
-      <c r="F23" s="8"/>
-      <c r="G23" s="8"/>
-      <c r="H23" s="8"/>
-      <c r="I23" s="8"/>
-      <c r="J23" s="8"/>
-      <c r="K23" s="8"/>
-      <c r="L23" s="8"/>
-      <c r="M23" s="8"/>
-      <c r="N23" s="8"/>
-      <c r="O23" s="8"/>
-      <c r="P23" s="8"/>
-      <c r="Q23" s="8"/>
-      <c r="R23" s="8"/>
-      <c r="S23" s="8"/>
+      <c r="C23" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="D23" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="E23" s="10"/>
+      <c r="F23" s="10"/>
+      <c r="G23" s="10"/>
+      <c r="H23" s="10"/>
+      <c r="I23" s="10"/>
+      <c r="J23" s="10"/>
+      <c r="K23" s="10"/>
+      <c r="L23" s="10"/>
+      <c r="M23" s="10"/>
+      <c r="N23" s="10"/>
+      <c r="O23" s="10"/>
+      <c r="P23" s="10"/>
+      <c r="Q23" s="10"/>
+      <c r="R23" s="10"/>
+      <c r="S23" s="10"/>
     </row>
     <row r="24" spans="1:19" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="B24" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C24" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="D24" s="10" t="b">
-        <v>0</v>
+      <c r="A24" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C24" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="D24" s="8" t="s">
+        <v>52</v>
       </c>
       <c r="E24" s="10"/>
       <c r="F24" s="10"/>
@@ -1376,17 +1385,17 @@
       <c r="S24" s="10"/>
     </row>
     <row r="25" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="B25" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C25" s="8" t="b">
-        <v>1</v>
-      </c>
-      <c r="D25" s="8" t="b">
-        <v>1</v>
+      <c r="A25" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C25" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="D25" s="8" t="s">
+        <v>53</v>
       </c>
       <c r="E25" s="8"/>
       <c r="F25" s="8"/>
@@ -1404,135 +1413,135 @@
       <c r="R25" s="8"/>
       <c r="S25" s="8"/>
     </row>
-    <row r="26" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="E26" s="8"/>
-      <c r="F26" s="8"/>
-      <c r="G26" s="8"/>
-      <c r="H26" s="8"/>
-      <c r="I26" s="8"/>
-      <c r="J26" s="8"/>
-      <c r="K26" s="8"/>
-      <c r="L26" s="8"/>
-      <c r="M26" s="8"/>
-      <c r="N26" s="8"/>
-      <c r="O26" s="8"/>
-      <c r="P26" s="8"/>
-      <c r="Q26" s="8"/>
-      <c r="R26" s="8"/>
-      <c r="S26" s="8"/>
-    </row>
-    <row r="27" spans="1:19" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="15"/>
-      <c r="C27" s="15"/>
-      <c r="D27" s="15"/>
-      <c r="E27" s="14"/>
-      <c r="F27" s="14"/>
-      <c r="G27" s="14"/>
-      <c r="H27" s="14"/>
-      <c r="I27" s="14"/>
-      <c r="J27" s="14"/>
-      <c r="K27" s="14"/>
-      <c r="L27" s="14"/>
-      <c r="M27" s="14"/>
-      <c r="N27" s="14"/>
-      <c r="O27" s="14"/>
-      <c r="P27" s="14"/>
-      <c r="Q27" s="14"/>
-      <c r="R27" s="14"/>
-      <c r="S27" s="14"/>
-    </row>
-    <row r="28" spans="1:19" s="12" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A28" s="20" t="s">
+    <row r="26" spans="1:19" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C26" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="D26" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="E26" s="10"/>
+      <c r="F26" s="10"/>
+      <c r="G26" s="10"/>
+      <c r="H26" s="10"/>
+      <c r="I26" s="10"/>
+      <c r="J26" s="10"/>
+      <c r="K26" s="10"/>
+      <c r="L26" s="10"/>
+      <c r="M26" s="10"/>
+      <c r="N26" s="10"/>
+      <c r="O26" s="10"/>
+      <c r="P26" s="10"/>
+      <c r="Q26" s="10"/>
+      <c r="R26" s="10"/>
+      <c r="S26" s="10"/>
+    </row>
+    <row r="27" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C27" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="D27" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="E27" s="8"/>
+      <c r="F27" s="8"/>
+      <c r="G27" s="8"/>
+      <c r="H27" s="8"/>
+      <c r="I27" s="8"/>
+      <c r="J27" s="8"/>
+      <c r="K27" s="8"/>
+      <c r="L27" s="8"/>
+      <c r="M27" s="8"/>
+      <c r="N27" s="8"/>
+      <c r="O27" s="8"/>
+      <c r="P27" s="8"/>
+      <c r="Q27" s="8"/>
+      <c r="R27" s="8"/>
+      <c r="S27" s="8"/>
+    </row>
+    <row r="28" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E28" s="8"/>
+      <c r="F28" s="8"/>
+      <c r="G28" s="8"/>
+      <c r="H28" s="8"/>
+      <c r="I28" s="8"/>
+      <c r="J28" s="8"/>
+      <c r="K28" s="8"/>
+      <c r="L28" s="8"/>
+      <c r="M28" s="8"/>
+      <c r="N28" s="8"/>
+      <c r="O28" s="8"/>
+      <c r="P28" s="8"/>
+      <c r="Q28" s="8"/>
+      <c r="R28" s="8"/>
+      <c r="S28" s="8"/>
+    </row>
+    <row r="29" spans="1:19" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="15"/>
+      <c r="C29" s="15"/>
+      <c r="D29" s="15"/>
+      <c r="E29" s="14"/>
+      <c r="F29" s="14"/>
+      <c r="G29" s="14"/>
+      <c r="H29" s="14"/>
+      <c r="I29" s="14"/>
+      <c r="J29" s="14"/>
+      <c r="K29" s="14"/>
+      <c r="L29" s="14"/>
+      <c r="M29" s="14"/>
+      <c r="N29" s="14"/>
+      <c r="O29" s="14"/>
+      <c r="P29" s="14"/>
+      <c r="Q29" s="14"/>
+      <c r="R29" s="14"/>
+      <c r="S29" s="14"/>
+    </row>
+    <row r="30" spans="1:19" s="12" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A30" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="C28" s="14"/>
-      <c r="D28" s="14"/>
-      <c r="E28" s="14"/>
-      <c r="F28" s="14"/>
-      <c r="G28" s="14"/>
-      <c r="H28" s="14"/>
-      <c r="I28" s="14"/>
-      <c r="J28" s="14"/>
-      <c r="K28" s="14"/>
-      <c r="L28" s="14"/>
-      <c r="M28" s="14"/>
-      <c r="N28" s="14"/>
-      <c r="O28" s="14"/>
-      <c r="P28" s="14"/>
-      <c r="Q28" s="14"/>
-      <c r="R28" s="14"/>
-      <c r="S28" s="14"/>
-    </row>
-    <row r="29" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="8" t="s">
-        <v>60</v>
-      </c>
-      <c r="B29" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C29" s="8">
-        <v>15</v>
-      </c>
-      <c r="D29" s="8">
-        <v>15</v>
-      </c>
-      <c r="E29" s="8"/>
-      <c r="F29" s="8"/>
-      <c r="G29" s="8"/>
-      <c r="H29" s="8"/>
-      <c r="I29" s="8"/>
-      <c r="J29" s="8"/>
-      <c r="K29" s="8"/>
-      <c r="L29" s="8"/>
-      <c r="M29" s="8"/>
-      <c r="N29" s="8"/>
-      <c r="O29" s="8"/>
-      <c r="P29" s="8"/>
-      <c r="Q29" s="8"/>
-      <c r="R29" s="8"/>
-      <c r="S29" s="8"/>
-    </row>
-    <row r="30" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="B30" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C30" s="8">
-        <v>15</v>
-      </c>
-      <c r="D30" s="8">
-        <v>5</v>
-      </c>
-      <c r="E30" s="8"/>
-      <c r="F30" s="8"/>
-      <c r="G30" s="8"/>
-      <c r="H30" s="8"/>
-      <c r="I30" s="8"/>
-      <c r="J30" s="8"/>
-      <c r="K30" s="8"/>
-      <c r="L30" s="8"/>
-      <c r="M30" s="8"/>
-      <c r="N30" s="8"/>
-      <c r="O30" s="8"/>
-      <c r="P30" s="8"/>
-      <c r="Q30" s="8"/>
-      <c r="R30" s="8"/>
-      <c r="S30" s="8"/>
+      <c r="C30" s="14"/>
+      <c r="D30" s="14"/>
+      <c r="E30" s="14"/>
+      <c r="F30" s="14"/>
+      <c r="G30" s="14"/>
+      <c r="H30" s="14"/>
+      <c r="I30" s="14"/>
+      <c r="J30" s="14"/>
+      <c r="K30" s="14"/>
+      <c r="L30" s="14"/>
+      <c r="M30" s="14"/>
+      <c r="N30" s="14"/>
+      <c r="O30" s="14"/>
+      <c r="P30" s="14"/>
+      <c r="Q30" s="14"/>
+      <c r="R30" s="14"/>
+      <c r="S30" s="14"/>
     </row>
     <row r="31" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="8" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B31" s="3" t="s">
         <v>13</v>
       </c>
       <c r="C31" s="8">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="D31" s="8">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="E31" s="8"/>
       <c r="F31" s="8"/>
@@ -1552,7 +1561,7 @@
     </row>
     <row r="32" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="8" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="B32" s="3" t="s">
         <v>13</v>
@@ -1581,7 +1590,7 @@
     </row>
     <row r="33" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="8" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="B33" s="3" t="s">
         <v>13</v>
@@ -1608,47 +1617,47 @@
       <c r="R33" s="8"/>
       <c r="S33" s="8"/>
     </row>
-    <row r="34" spans="1:19" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="10" t="s">
-        <v>29</v>
+    <row r="34" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="8" t="s">
+        <v>56</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C34" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="D34" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="E34" s="10"/>
-      <c r="F34" s="10"/>
-      <c r="G34" s="10"/>
-      <c r="H34" s="10"/>
-      <c r="I34" s="10"/>
-      <c r="J34" s="10"/>
-      <c r="K34" s="10"/>
-      <c r="L34" s="10"/>
-      <c r="M34" s="10"/>
-      <c r="N34" s="10"/>
-      <c r="O34" s="10"/>
-      <c r="P34" s="10"/>
-      <c r="Q34" s="10"/>
-      <c r="R34" s="10"/>
-      <c r="S34" s="10"/>
+        <v>13</v>
+      </c>
+      <c r="C34" s="8">
+        <v>15</v>
+      </c>
+      <c r="D34" s="8">
+        <v>5</v>
+      </c>
+      <c r="E34" s="8"/>
+      <c r="F34" s="8"/>
+      <c r="G34" s="8"/>
+      <c r="H34" s="8"/>
+      <c r="I34" s="8"/>
+      <c r="J34" s="8"/>
+      <c r="K34" s="8"/>
+      <c r="L34" s="8"/>
+      <c r="M34" s="8"/>
+      <c r="N34" s="8"/>
+      <c r="O34" s="8"/>
+      <c r="P34" s="8"/>
+      <c r="Q34" s="8"/>
+      <c r="R34" s="8"/>
+      <c r="S34" s="8"/>
     </row>
     <row r="35" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="B35" s="4" t="s">
+      <c r="A35" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="B35" s="3" t="s">
         <v>13</v>
       </c>
       <c r="C35" s="8">
-        <v>0.75</v>
+        <v>2</v>
       </c>
       <c r="D35" s="8">
-        <v>0.75</v>
+        <v>5</v>
       </c>
       <c r="E35" s="8"/>
       <c r="F35" s="8"/>
@@ -1666,40 +1675,48 @@
       <c r="R35" s="8"/>
       <c r="S35" s="8"/>
     </row>
-    <row r="36" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="8" t="s">
-        <v>45</v>
+    <row r="36" spans="1:19" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="10" t="s">
+        <v>29</v>
       </c>
       <c r="B36" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C36" s="8" t="b">
-        <v>1</v>
-      </c>
-      <c r="D36" s="8" t="b">
-        <v>1</v>
-      </c>
-      <c r="E36" s="8"/>
-      <c r="F36" s="8"/>
-      <c r="G36" s="8"/>
-      <c r="H36" s="8"/>
-      <c r="I36" s="8"/>
-      <c r="J36" s="8"/>
-      <c r="K36" s="8"/>
-      <c r="L36" s="8"/>
-      <c r="M36" s="8"/>
-      <c r="N36" s="8"/>
-      <c r="O36" s="8"/>
-      <c r="P36" s="8"/>
-      <c r="Q36" s="8"/>
-      <c r="R36" s="8"/>
-      <c r="S36" s="8"/>
+      <c r="C36" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="D36" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="E36" s="10"/>
+      <c r="F36" s="10"/>
+      <c r="G36" s="10"/>
+      <c r="H36" s="10"/>
+      <c r="I36" s="10"/>
+      <c r="J36" s="10"/>
+      <c r="K36" s="10"/>
+      <c r="L36" s="10"/>
+      <c r="M36" s="10"/>
+      <c r="N36" s="10"/>
+      <c r="O36" s="10"/>
+      <c r="P36" s="10"/>
+      <c r="Q36" s="10"/>
+      <c r="R36" s="10"/>
+      <c r="S36" s="10"/>
     </row>
     <row r="37" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="8"/>
-      <c r="B37" s="3"/>
-      <c r="C37" s="8"/>
-      <c r="D37" s="8"/>
+      <c r="A37" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="B37" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C37" s="8">
+        <v>0.75</v>
+      </c>
+      <c r="D37" s="8">
+        <v>0.75</v>
+      </c>
       <c r="E37" s="8"/>
       <c r="F37" s="8"/>
       <c r="G37" s="8"/>
@@ -1716,111 +1733,111 @@
       <c r="R37" s="8"/>
       <c r="S37" s="8"/>
     </row>
-    <row r="38" spans="1:19" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="15"/>
-      <c r="C38" s="15"/>
-      <c r="D38" s="15"/>
-      <c r="E38" s="14"/>
-      <c r="F38" s="14"/>
-      <c r="G38" s="14"/>
-      <c r="H38" s="14"/>
-      <c r="I38" s="14"/>
-      <c r="J38" s="14"/>
-      <c r="K38" s="14"/>
-      <c r="L38" s="14"/>
-      <c r="M38" s="14"/>
-      <c r="N38" s="14"/>
-      <c r="O38" s="14"/>
-      <c r="P38" s="14"/>
-      <c r="Q38" s="14"/>
-      <c r="R38" s="14"/>
-      <c r="S38" s="14"/>
-    </row>
-    <row r="39" spans="1:19" s="12" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A39" s="20" t="s">
+    <row r="38" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C38" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="D38" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="E38" s="8"/>
+      <c r="F38" s="8"/>
+      <c r="G38" s="8"/>
+      <c r="H38" s="8"/>
+      <c r="I38" s="8"/>
+      <c r="J38" s="8"/>
+      <c r="K38" s="8"/>
+      <c r="L38" s="8"/>
+      <c r="M38" s="8"/>
+      <c r="N38" s="8"/>
+      <c r="O38" s="8"/>
+      <c r="P38" s="8"/>
+      <c r="Q38" s="8"/>
+      <c r="R38" s="8"/>
+      <c r="S38" s="8"/>
+    </row>
+    <row r="39" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="8"/>
+      <c r="B39" s="3"/>
+      <c r="C39" s="8"/>
+      <c r="D39" s="8"/>
+      <c r="E39" s="8"/>
+      <c r="F39" s="8"/>
+      <c r="G39" s="8"/>
+      <c r="H39" s="8"/>
+      <c r="I39" s="8"/>
+      <c r="J39" s="8"/>
+      <c r="K39" s="8"/>
+      <c r="L39" s="8"/>
+      <c r="M39" s="8"/>
+      <c r="N39" s="8"/>
+      <c r="O39" s="8"/>
+      <c r="P39" s="8"/>
+      <c r="Q39" s="8"/>
+      <c r="R39" s="8"/>
+      <c r="S39" s="8"/>
+    </row>
+    <row r="40" spans="1:19" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="15"/>
+      <c r="C40" s="15"/>
+      <c r="D40" s="15"/>
+      <c r="E40" s="14"/>
+      <c r="F40" s="14"/>
+      <c r="G40" s="14"/>
+      <c r="H40" s="14"/>
+      <c r="I40" s="14"/>
+      <c r="J40" s="14"/>
+      <c r="K40" s="14"/>
+      <c r="L40" s="14"/>
+      <c r="M40" s="14"/>
+      <c r="N40" s="14"/>
+      <c r="O40" s="14"/>
+      <c r="P40" s="14"/>
+      <c r="Q40" s="14"/>
+      <c r="R40" s="14"/>
+      <c r="S40" s="14"/>
+    </row>
+    <row r="41" spans="1:19" s="12" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A41" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="C39" s="14"/>
-      <c r="D39" s="14"/>
-      <c r="E39" s="14"/>
-      <c r="F39" s="14"/>
-      <c r="G39" s="14"/>
-      <c r="H39" s="14"/>
-      <c r="I39" s="14"/>
-      <c r="J39" s="14"/>
-      <c r="K39" s="14"/>
-      <c r="L39" s="14"/>
-      <c r="M39" s="14"/>
-      <c r="N39" s="14"/>
-      <c r="O39" s="14"/>
-      <c r="P39" s="14"/>
-      <c r="Q39" s="14"/>
-      <c r="R39" s="14"/>
-      <c r="S39" s="14"/>
-    </row>
-    <row r="40" spans="1:19" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A40" s="10" t="s">
+      <c r="C41" s="14"/>
+      <c r="D41" s="14"/>
+      <c r="E41" s="14"/>
+      <c r="F41" s="14"/>
+      <c r="G41" s="14"/>
+      <c r="H41" s="14"/>
+      <c r="I41" s="14"/>
+      <c r="J41" s="14"/>
+      <c r="K41" s="14"/>
+      <c r="L41" s="14"/>
+      <c r="M41" s="14"/>
+      <c r="N41" s="14"/>
+      <c r="O41" s="14"/>
+      <c r="P41" s="14"/>
+      <c r="Q41" s="14"/>
+      <c r="R41" s="14"/>
+      <c r="S41" s="14"/>
+    </row>
+    <row r="42" spans="1:19" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A42" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="B40" s="3" t="s">
+      <c r="B42" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="C40" s="8" t="s">
+      <c r="C42" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="D40" s="8" t="s">
+      <c r="D42" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="E40" s="8"/>
-      <c r="F40" s="8"/>
-      <c r="G40" s="8"/>
-      <c r="H40" s="8"/>
-      <c r="I40" s="8"/>
-      <c r="J40" s="8"/>
-      <c r="K40" s="8"/>
-      <c r="L40" s="8"/>
-      <c r="M40" s="8"/>
-      <c r="N40" s="8"/>
-      <c r="O40" s="8"/>
-      <c r="P40" s="8"/>
-      <c r="Q40" s="8"/>
-      <c r="R40" s="8"/>
-      <c r="S40" s="8"/>
-    </row>
-    <row r="41" spans="1:19" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A41" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="B41" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="C41" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="D41" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="E41" s="8"/>
-      <c r="F41" s="8"/>
-      <c r="G41" s="8"/>
-      <c r="H41" s="8"/>
-      <c r="I41" s="8"/>
-      <c r="J41" s="8"/>
-      <c r="K41" s="8"/>
-      <c r="L41" s="8"/>
-      <c r="M41" s="8"/>
-      <c r="N41" s="8"/>
-      <c r="O41" s="8"/>
-      <c r="P41" s="8"/>
-      <c r="Q41" s="8"/>
-      <c r="R41" s="8"/>
-      <c r="S41" s="8"/>
-    </row>
-    <row r="42" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="8"/>
-      <c r="B42" s="3"/>
-      <c r="C42" s="8"/>
-      <c r="D42" s="8"/>
       <c r="E42" s="8"/>
       <c r="F42" s="8"/>
       <c r="G42" s="8"/>
@@ -1837,6 +1854,56 @@
       <c r="R42" s="8"/>
       <c r="S42" s="8"/>
     </row>
+    <row r="43" spans="1:19" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A43" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="B43" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C43" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="D43" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="E43" s="8"/>
+      <c r="F43" s="8"/>
+      <c r="G43" s="8"/>
+      <c r="H43" s="8"/>
+      <c r="I43" s="8"/>
+      <c r="J43" s="8"/>
+      <c r="K43" s="8"/>
+      <c r="L43" s="8"/>
+      <c r="M43" s="8"/>
+      <c r="N43" s="8"/>
+      <c r="O43" s="8"/>
+      <c r="P43" s="8"/>
+      <c r="Q43" s="8"/>
+      <c r="R43" s="8"/>
+      <c r="S43" s="8"/>
+    </row>
+    <row r="44" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="8"/>
+      <c r="B44" s="3"/>
+      <c r="C44" s="8"/>
+      <c r="D44" s="8"/>
+      <c r="E44" s="8"/>
+      <c r="F44" s="8"/>
+      <c r="G44" s="8"/>
+      <c r="H44" s="8"/>
+      <c r="I44" s="8"/>
+      <c r="J44" s="8"/>
+      <c r="K44" s="8"/>
+      <c r="L44" s="8"/>
+      <c r="M44" s="8"/>
+      <c r="N44" s="8"/>
+      <c r="O44" s="8"/>
+      <c r="P44" s="8"/>
+      <c r="Q44" s="8"/>
+      <c r="R44" s="8"/>
+      <c r="S44" s="8"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
updates to batch definition -     ghg standards and cost file types no longer have to be specified - correct module is imported based on input file template name     context reference name and case added to batch definition and used to load correct context data
vehicles input file aeo_size_class column is now context_size_class
hauling / non hauling sales split now comes from context (default ice/bev split comes from initial fleet)
added hauling / non hauling to market share plot in postproc
added cert_fuel_ID and size classes and electrification classes to Vehicle classes

Signed-off-by: kevinanewman <newman.kevin@epa.gov>
</commit_message>
<xml_diff>
--- a/input_samples/multiple_session_batch.xlsx
+++ b/input_samples/multiple_session_batch.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\GitHub\EPA_OMEGA_Model\input_samples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42847E73-E4ED-440D-8B86-712912D9773D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49042595-0D08-459A-8A92-55C254113FA7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3030" yWindow="465" windowWidth="20115" windowHeight="19695" tabRatio="151" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,17 +18,25 @@
   <definedNames>
     <definedName name="LOCAL_MYSQL_DATE_FORMAT" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="62">
   <si>
     <t>Parameter</t>
   </si>
@@ -93,17 +101,7 @@
     <t>Cost File</t>
   </si>
   <si>
-    <t>Cost File Type</t>
-  </si>
-  <si>
     <t>GHG Standards File</t>
-  </si>
-  <si>
-    <t>GHG Standard Type</t>
-  </si>
-  <si>
-    <t>Flat
-Footprint</t>
   </si>
   <si>
     <t>Fixed
@@ -122,9 +120,6 @@
     <t>Allow Backsliding</t>
   </si>
   <si>
-    <t>Footprint</t>
-  </si>
-  <si>
     <t>Fixed</t>
   </si>
   <si>
@@ -137,16 +132,6 @@
     <t>FALSE, TRUE</t>
   </si>
   <si>
-    <t>Flat</t>
-  </si>
-  <si>
-    <t>CostClouds
-CostCurves</t>
-  </si>
-  <si>
-    <t>CostCurves</t>
-  </si>
-  <si>
     <t>Demanded Shares File</t>
   </si>
   <si>
@@ -226,6 +211,18 @@
   </si>
   <si>
     <t>input_samples/context_new_vehicle_market.csv</t>
+  </si>
+  <si>
+    <t>AEO2020</t>
+  </si>
+  <si>
+    <t>Context Case</t>
+  </si>
+  <si>
+    <t>Reference case</t>
+  </si>
+  <si>
+    <t>New Vehicle Price Sales Response Elasticity</t>
   </si>
 </sst>
 </file>
@@ -721,8 +718,8 @@
   <dimension ref="A1:AG44"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="9" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A17" sqref="A17"/>
+      <pane ySplit="10" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A38" sqref="A38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -806,7 +803,7 @@
         <v>3</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="D3" s="14"/>
       <c r="E3" s="14"/>
@@ -825,7 +822,7 @@
     </row>
     <row r="4" spans="1:33" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="B4" s="6" t="s">
         <v>3</v>
@@ -846,51 +843,30 @@
       <c r="P4" s="14"/>
       <c r="Q4" s="14"/>
     </row>
-    <row r="5" spans="1:33" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="B5" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="7"/>
-      <c r="D5" s="14"/>
-      <c r="E5" s="14"/>
-      <c r="F5" s="14"/>
-      <c r="G5" s="14"/>
-      <c r="H5" s="14"/>
-      <c r="I5" s="14"/>
-      <c r="J5" s="14"/>
-      <c r="K5" s="14"/>
-      <c r="L5" s="14"/>
-      <c r="M5" s="14"/>
-      <c r="N5" s="14"/>
-      <c r="O5" s="14"/>
-      <c r="P5" s="14"/>
-      <c r="Q5" s="14"/>
-    </row>
-    <row r="6" spans="1:33" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="14"/>
-      <c r="C6" s="14"/>
-      <c r="D6" s="14"/>
-      <c r="E6" s="14"/>
-      <c r="F6" s="14"/>
-      <c r="G6" s="14"/>
-      <c r="H6" s="14"/>
-      <c r="I6" s="14"/>
-      <c r="J6" s="14"/>
-      <c r="K6" s="14"/>
-      <c r="L6" s="14"/>
-      <c r="M6" s="14"/>
-      <c r="N6" s="14"/>
-      <c r="O6" s="14"/>
-      <c r="P6" s="14"/>
-      <c r="Q6" s="14"/>
-    </row>
-    <row r="7" spans="1:33" s="12" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="20" t="s">
-        <v>9</v>
-      </c>
+      <c r="C5" s="7" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="6" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A6" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="7" spans="1:33" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="14"/>
       <c r="C7" s="14"/>
       <c r="D7" s="14"/>
       <c r="E7" s="14"/>
@@ -907,90 +883,88 @@
       <c r="P7" s="14"/>
       <c r="Q7" s="14"/>
     </row>
-    <row r="8" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="8" t="s">
+    <row r="8" spans="1:33" s="12" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="14"/>
+      <c r="D8" s="14"/>
+      <c r="E8" s="14"/>
+      <c r="F8" s="14"/>
+      <c r="G8" s="14"/>
+      <c r="H8" s="14"/>
+      <c r="I8" s="14"/>
+      <c r="J8" s="14"/>
+      <c r="K8" s="14"/>
+      <c r="L8" s="14"/>
+      <c r="M8" s="14"/>
+      <c r="N8" s="14"/>
+      <c r="O8" s="14"/>
+      <c r="P8" s="14"/>
+      <c r="Q8" s="14"/>
+    </row>
+    <row r="9" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B9" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C8" s="8" t="b">
+      <c r="C9" s="8" t="b">
         <v>1</v>
       </c>
-      <c r="D8" s="8" t="b">
+      <c r="D9" s="8" t="b">
         <v>1</v>
       </c>
-      <c r="E8" s="8"/>
-      <c r="F8" s="8"/>
-      <c r="G8" s="8"/>
-      <c r="H8" s="8"/>
-      <c r="I8" s="8"/>
-      <c r="J8" s="8"/>
-      <c r="K8" s="8"/>
-      <c r="L8" s="8"/>
-      <c r="M8" s="8"/>
-      <c r="N8" s="8"/>
-      <c r="O8" s="8"/>
-      <c r="P8" s="8"/>
-      <c r="Q8" s="8"/>
-      <c r="R8" s="8"/>
-      <c r="S8" s="8"/>
-    </row>
-    <row r="9" spans="1:33" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="9" t="s">
+      <c r="E9" s="8"/>
+      <c r="F9" s="8"/>
+      <c r="G9" s="8"/>
+      <c r="H9" s="8"/>
+      <c r="I9" s="8"/>
+      <c r="J9" s="8"/>
+      <c r="K9" s="8"/>
+      <c r="L9" s="8"/>
+      <c r="M9" s="8"/>
+      <c r="N9" s="8"/>
+      <c r="O9" s="8"/>
+      <c r="P9" s="8"/>
+      <c r="Q9" s="8"/>
+      <c r="R9" s="8"/>
+      <c r="S9" s="8"/>
+    </row>
+    <row r="10" spans="1:33" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="B10" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C9" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="D9" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="E9" s="9"/>
-      <c r="F9" s="9"/>
-      <c r="G9" s="9"/>
-      <c r="H9" s="9"/>
-      <c r="I9" s="9"/>
-      <c r="J9" s="9"/>
-      <c r="K9" s="9"/>
-      <c r="L9" s="9"/>
-      <c r="M9" s="9"/>
-      <c r="N9" s="9"/>
-      <c r="O9" s="9"/>
-      <c r="P9" s="9"/>
-      <c r="Q9" s="9"/>
-      <c r="R9" s="9"/>
-      <c r="S9" s="9"/>
-    </row>
-    <row r="10" spans="1:33" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="15"/>
-      <c r="C10" s="15"/>
-      <c r="D10" s="15"/>
-      <c r="E10" s="14"/>
-      <c r="F10" s="14"/>
-      <c r="G10" s="14"/>
-      <c r="H10" s="14"/>
-      <c r="I10" s="14"/>
-      <c r="J10" s="14"/>
-      <c r="K10" s="14"/>
-      <c r="L10" s="14"/>
-      <c r="M10" s="14"/>
-      <c r="N10" s="14"/>
-      <c r="O10" s="14"/>
-      <c r="P10" s="14"/>
-      <c r="Q10" s="14"/>
-      <c r="R10" s="14"/>
-      <c r="S10" s="14"/>
-    </row>
-    <row r="11" spans="1:33" s="12" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="C11" s="14"/>
-      <c r="D11" s="14"/>
+      <c r="C10" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="D10" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="E10" s="9"/>
+      <c r="F10" s="9"/>
+      <c r="G10" s="9"/>
+      <c r="H10" s="9"/>
+      <c r="I10" s="9"/>
+      <c r="J10" s="9"/>
+      <c r="K10" s="9"/>
+      <c r="L10" s="9"/>
+      <c r="M10" s="9"/>
+      <c r="N10" s="9"/>
+      <c r="O10" s="9"/>
+      <c r="P10" s="9"/>
+      <c r="Q10" s="9"/>
+      <c r="R10" s="9"/>
+      <c r="S10" s="9"/>
+    </row>
+    <row r="11" spans="1:33" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="15"/>
+      <c r="C11" s="15"/>
+      <c r="D11" s="15"/>
       <c r="E11" s="14"/>
       <c r="F11" s="14"/>
       <c r="G11" s="14"/>
@@ -1007,47 +981,40 @@
       <c r="R11" s="14"/>
       <c r="S11" s="14"/>
     </row>
-    <row r="12" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C12" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="D12" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="E12" s="8"/>
-      <c r="F12" s="8"/>
-      <c r="G12" s="8"/>
-      <c r="H12" s="8"/>
-      <c r="I12" s="8"/>
-      <c r="J12" s="8"/>
-      <c r="K12" s="8"/>
-      <c r="L12" s="8"/>
-      <c r="M12" s="8"/>
-      <c r="N12" s="8"/>
-      <c r="O12" s="8"/>
-      <c r="P12" s="8"/>
-      <c r="Q12" s="8"/>
-      <c r="R12" s="8"/>
-      <c r="S12" s="8"/>
+    <row r="12" spans="1:33" s="12" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A12" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12" s="14"/>
+      <c r="D12" s="14"/>
+      <c r="E12" s="14"/>
+      <c r="F12" s="14"/>
+      <c r="G12" s="14"/>
+      <c r="H12" s="14"/>
+      <c r="I12" s="14"/>
+      <c r="J12" s="14"/>
+      <c r="K12" s="14"/>
+      <c r="L12" s="14"/>
+      <c r="M12" s="14"/>
+      <c r="N12" s="14"/>
+      <c r="O12" s="14"/>
+      <c r="P12" s="14"/>
+      <c r="Q12" s="14"/>
+      <c r="R12" s="14"/>
+      <c r="S12" s="14"/>
     </row>
     <row r="13" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>3</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="E13" s="8"/>
       <c r="F13" s="8"/>
@@ -1067,16 +1034,16 @@
     </row>
     <row r="14" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>3</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="E14" s="8"/>
       <c r="F14" s="8"/>
@@ -1096,16 +1063,16 @@
     </row>
     <row r="15" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="8" t="s">
-        <v>38</v>
+        <v>17</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>3</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="E15" s="8"/>
       <c r="F15" s="8"/>
@@ -1125,16 +1092,16 @@
     </row>
     <row r="16" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="8" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>3</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="E16" s="8"/>
       <c r="F16" s="8"/>
@@ -1154,16 +1121,16 @@
     </row>
     <row r="17" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="8" t="s">
-        <v>62</v>
+        <v>19</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>3</v>
       </c>
       <c r="C17" s="8" t="s">
-        <v>61</v>
+        <v>42</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>61</v>
+        <v>42</v>
       </c>
       <c r="E17" s="8"/>
       <c r="F17" s="8"/>
@@ -1183,16 +1150,16 @@
     </row>
     <row r="18" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="8" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>3</v>
       </c>
       <c r="C18" s="8" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="D18" s="8" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="E18" s="8"/>
       <c r="F18" s="8"/>
@@ -1212,16 +1179,16 @@
     </row>
     <row r="19" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="8" t="s">
-        <v>18</v>
+        <v>56</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>3</v>
       </c>
       <c r="C19" s="8" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="D19" s="8" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="E19" s="8"/>
       <c r="F19" s="8"/>
@@ -1239,18 +1206,18 @@
       <c r="R19" s="8"/>
       <c r="S19" s="8"/>
     </row>
-    <row r="20" spans="1:19" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="B20" s="3" t="s">
-        <v>36</v>
+        <v>18</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>3</v>
       </c>
       <c r="C20" s="8" t="s">
-        <v>37</v>
+        <v>54</v>
       </c>
       <c r="D20" s="8" t="s">
-        <v>37</v>
+        <v>54</v>
       </c>
       <c r="E20" s="8"/>
       <c r="F20" s="8"/>
@@ -1276,10 +1243,10 @@
         <v>3</v>
       </c>
       <c r="C21" s="8" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="D21" s="8" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="E21" s="8"/>
       <c r="F21" s="8"/>
@@ -1297,18 +1264,18 @@
       <c r="R21" s="8"/>
       <c r="S21" s="8"/>
     </row>
-    <row r="22" spans="1:19" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:19" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="B22" s="3" t="s">
-        <v>24</v>
+        <v>21</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>3</v>
       </c>
       <c r="C22" s="10" t="s">
-        <v>30</v>
+        <v>44</v>
       </c>
       <c r="D22" s="10" t="s">
-        <v>35</v>
+        <v>47</v>
       </c>
       <c r="E22" s="10"/>
       <c r="F22" s="10"/>
@@ -1327,17 +1294,17 @@
       <c r="S22" s="10"/>
     </row>
     <row r="23" spans="1:19" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="10" t="s">
-        <v>22</v>
+      <c r="A23" s="8" t="s">
+        <v>36</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C23" s="10" t="s">
-        <v>51</v>
-      </c>
-      <c r="D23" s="10" t="s">
-        <v>54</v>
+      <c r="C23" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="D23" s="8" t="s">
+        <v>45</v>
       </c>
       <c r="E23" s="10"/>
       <c r="F23" s="10"/>
@@ -1355,106 +1322,94 @@
       <c r="R23" s="10"/>
       <c r="S23" s="10"/>
     </row>
-    <row r="24" spans="1:19" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="8" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>3</v>
       </c>
       <c r="C24" s="8" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="D24" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="E24" s="10"/>
-      <c r="F24" s="10"/>
-      <c r="G24" s="10"/>
-      <c r="H24" s="10"/>
-      <c r="I24" s="10"/>
-      <c r="J24" s="10"/>
-      <c r="K24" s="10"/>
-      <c r="L24" s="10"/>
-      <c r="M24" s="10"/>
-      <c r="N24" s="10"/>
-      <c r="O24" s="10"/>
-      <c r="P24" s="10"/>
-      <c r="Q24" s="10"/>
-      <c r="R24" s="10"/>
-      <c r="S24" s="10"/>
-    </row>
-    <row r="25" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C25" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="D25" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="E25" s="8"/>
-      <c r="F25" s="8"/>
-      <c r="G25" s="8"/>
-      <c r="H25" s="8"/>
-      <c r="I25" s="8"/>
-      <c r="J25" s="8"/>
-      <c r="K25" s="8"/>
-      <c r="L25" s="8"/>
-      <c r="M25" s="8"/>
-      <c r="N25" s="8"/>
-      <c r="O25" s="8"/>
-      <c r="P25" s="8"/>
-      <c r="Q25" s="8"/>
-      <c r="R25" s="8"/>
-      <c r="S25" s="8"/>
-    </row>
-    <row r="26" spans="1:19" s="4" customFormat="1" x14ac:dyDescent="0.25">
+        <v>46</v>
+      </c>
+      <c r="E24" s="8"/>
+      <c r="F24" s="8"/>
+      <c r="G24" s="8"/>
+      <c r="H24" s="8"/>
+      <c r="I24" s="8"/>
+      <c r="J24" s="8"/>
+      <c r="K24" s="8"/>
+      <c r="L24" s="8"/>
+      <c r="M24" s="8"/>
+      <c r="N24" s="8"/>
+      <c r="O24" s="8"/>
+      <c r="P24" s="8"/>
+      <c r="Q24" s="8"/>
+      <c r="R24" s="8"/>
+      <c r="S24" s="8"/>
+    </row>
+    <row r="25" spans="1:19" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C25" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="D25" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="E25" s="10"/>
+      <c r="F25" s="10"/>
+      <c r="G25" s="10"/>
+      <c r="H25" s="10"/>
+      <c r="I25" s="10"/>
+      <c r="J25" s="10"/>
+      <c r="K25" s="10"/>
+      <c r="L25" s="10"/>
+      <c r="M25" s="10"/>
+      <c r="N25" s="10"/>
+      <c r="O25" s="10"/>
+      <c r="P25" s="10"/>
+      <c r="Q25" s="10"/>
+      <c r="R25" s="10"/>
+      <c r="S25" s="10"/>
+    </row>
+    <row r="26" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="10" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="B26" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C26" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="D26" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="E26" s="10"/>
-      <c r="F26" s="10"/>
-      <c r="G26" s="10"/>
-      <c r="H26" s="10"/>
-      <c r="I26" s="10"/>
-      <c r="J26" s="10"/>
-      <c r="K26" s="10"/>
-      <c r="L26" s="10"/>
-      <c r="M26" s="10"/>
-      <c r="N26" s="10"/>
-      <c r="O26" s="10"/>
-      <c r="P26" s="10"/>
-      <c r="Q26" s="10"/>
-      <c r="R26" s="10"/>
-      <c r="S26" s="10"/>
+      <c r="C26" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="D26" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="E26" s="8"/>
+      <c r="F26" s="8"/>
+      <c r="G26" s="8"/>
+      <c r="H26" s="8"/>
+      <c r="I26" s="8"/>
+      <c r="J26" s="8"/>
+      <c r="K26" s="8"/>
+      <c r="L26" s="8"/>
+      <c r="M26" s="8"/>
+      <c r="N26" s="8"/>
+      <c r="O26" s="8"/>
+      <c r="P26" s="8"/>
+      <c r="Q26" s="8"/>
+      <c r="R26" s="8"/>
+      <c r="S26" s="8"/>
     </row>
     <row r="27" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="B27" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C27" s="8" t="b">
-        <v>1</v>
-      </c>
-      <c r="D27" s="8" t="b">
-        <v>1</v>
-      </c>
       <c r="E27" s="8"/>
       <c r="F27" s="8"/>
       <c r="G27" s="8"/>
@@ -1471,27 +1426,32 @@
       <c r="R27" s="8"/>
       <c r="S27" s="8"/>
     </row>
-    <row r="28" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="E28" s="8"/>
-      <c r="F28" s="8"/>
-      <c r="G28" s="8"/>
-      <c r="H28" s="8"/>
-      <c r="I28" s="8"/>
-      <c r="J28" s="8"/>
-      <c r="K28" s="8"/>
-      <c r="L28" s="8"/>
-      <c r="M28" s="8"/>
-      <c r="N28" s="8"/>
-      <c r="O28" s="8"/>
-      <c r="P28" s="8"/>
-      <c r="Q28" s="8"/>
-      <c r="R28" s="8"/>
-      <c r="S28" s="8"/>
-    </row>
-    <row r="29" spans="1:19" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="15"/>
-      <c r="C29" s="15"/>
-      <c r="D29" s="15"/>
+    <row r="28" spans="1:19" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="15"/>
+      <c r="C28" s="15"/>
+      <c r="D28" s="15"/>
+      <c r="E28" s="14"/>
+      <c r="F28" s="14"/>
+      <c r="G28" s="14"/>
+      <c r="H28" s="14"/>
+      <c r="I28" s="14"/>
+      <c r="J28" s="14"/>
+      <c r="K28" s="14"/>
+      <c r="L28" s="14"/>
+      <c r="M28" s="14"/>
+      <c r="N28" s="14"/>
+      <c r="O28" s="14"/>
+      <c r="P28" s="14"/>
+      <c r="Q28" s="14"/>
+      <c r="R28" s="14"/>
+      <c r="S28" s="14"/>
+    </row>
+    <row r="29" spans="1:19" s="12" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A29" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="C29" s="14"/>
+      <c r="D29" s="14"/>
       <c r="E29" s="14"/>
       <c r="F29" s="14"/>
       <c r="G29" s="14"/>
@@ -1508,31 +1468,38 @@
       <c r="R29" s="14"/>
       <c r="S29" s="14"/>
     </row>
-    <row r="30" spans="1:19" s="12" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A30" s="20" t="s">
-        <v>8</v>
-      </c>
-      <c r="C30" s="14"/>
-      <c r="D30" s="14"/>
-      <c r="E30" s="14"/>
-      <c r="F30" s="14"/>
-      <c r="G30" s="14"/>
-      <c r="H30" s="14"/>
-      <c r="I30" s="14"/>
-      <c r="J30" s="14"/>
-      <c r="K30" s="14"/>
-      <c r="L30" s="14"/>
-      <c r="M30" s="14"/>
-      <c r="N30" s="14"/>
-      <c r="O30" s="14"/>
-      <c r="P30" s="14"/>
-      <c r="Q30" s="14"/>
-      <c r="R30" s="14"/>
-      <c r="S30" s="14"/>
+    <row r="30" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C30" s="8">
+        <v>15</v>
+      </c>
+      <c r="D30" s="8">
+        <v>15</v>
+      </c>
+      <c r="E30" s="8"/>
+      <c r="F30" s="8"/>
+      <c r="G30" s="8"/>
+      <c r="H30" s="8"/>
+      <c r="I30" s="8"/>
+      <c r="J30" s="8"/>
+      <c r="K30" s="8"/>
+      <c r="L30" s="8"/>
+      <c r="M30" s="8"/>
+      <c r="N30" s="8"/>
+      <c r="O30" s="8"/>
+      <c r="P30" s="8"/>
+      <c r="Q30" s="8"/>
+      <c r="R30" s="8"/>
+      <c r="S30" s="8"/>
     </row>
     <row r="31" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="8" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="B31" s="3" t="s">
         <v>13</v>
@@ -1541,7 +1508,7 @@
         <v>15</v>
       </c>
       <c r="D31" s="8">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="E31" s="8"/>
       <c r="F31" s="8"/>
@@ -1561,13 +1528,13 @@
     </row>
     <row r="32" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="8" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="B32" s="3" t="s">
         <v>13</v>
       </c>
       <c r="C32" s="8">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="D32" s="8">
         <v>5</v>
@@ -1590,13 +1557,13 @@
     </row>
     <row r="33" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="8" t="s">
-        <v>59</v>
+        <v>49</v>
       </c>
       <c r="B33" s="3" t="s">
         <v>13</v>
       </c>
       <c r="C33" s="8">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="D33" s="8">
         <v>5</v>
@@ -1619,13 +1586,13 @@
     </row>
     <row r="34" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="8" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="B34" s="3" t="s">
         <v>13</v>
       </c>
       <c r="C34" s="8">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="D34" s="8">
         <v>5</v>
@@ -1646,76 +1613,76 @@
       <c r="R34" s="8"/>
       <c r="S34" s="8"/>
     </row>
-    <row r="35" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="8" t="s">
-        <v>57</v>
+    <row r="35" spans="1:19" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="10" t="s">
+        <v>26</v>
       </c>
       <c r="B35" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C35" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="D35" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="E35" s="10"/>
+      <c r="F35" s="10"/>
+      <c r="G35" s="10"/>
+      <c r="H35" s="10"/>
+      <c r="I35" s="10"/>
+      <c r="J35" s="10"/>
+      <c r="K35" s="10"/>
+      <c r="L35" s="10"/>
+      <c r="M35" s="10"/>
+      <c r="N35" s="10"/>
+      <c r="O35" s="10"/>
+      <c r="P35" s="10"/>
+      <c r="Q35" s="10"/>
+      <c r="R35" s="10"/>
+      <c r="S35" s="10"/>
+    </row>
+    <row r="36" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="B36" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C35" s="8">
-        <v>2</v>
-      </c>
-      <c r="D35" s="8">
-        <v>5</v>
-      </c>
-      <c r="E35" s="8"/>
-      <c r="F35" s="8"/>
-      <c r="G35" s="8"/>
-      <c r="H35" s="8"/>
-      <c r="I35" s="8"/>
-      <c r="J35" s="8"/>
-      <c r="K35" s="8"/>
-      <c r="L35" s="8"/>
-      <c r="M35" s="8"/>
-      <c r="N35" s="8"/>
-      <c r="O35" s="8"/>
-      <c r="P35" s="8"/>
-      <c r="Q35" s="8"/>
-      <c r="R35" s="8"/>
-      <c r="S35" s="8"/>
-    </row>
-    <row r="36" spans="1:19" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="B36" s="3" t="s">
+      <c r="C36" s="8">
+        <v>0.75</v>
+      </c>
+      <c r="D36" s="8">
+        <v>0.75</v>
+      </c>
+      <c r="E36" s="8"/>
+      <c r="F36" s="8"/>
+      <c r="G36" s="8"/>
+      <c r="H36" s="8"/>
+      <c r="I36" s="8"/>
+      <c r="J36" s="8"/>
+      <c r="K36" s="8"/>
+      <c r="L36" s="8"/>
+      <c r="M36" s="8"/>
+      <c r="N36" s="8"/>
+      <c r="O36" s="8"/>
+      <c r="P36" s="8"/>
+      <c r="Q36" s="8"/>
+      <c r="R36" s="8"/>
+      <c r="S36" s="8"/>
+    </row>
+    <row r="37" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="B37" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C36" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="D36" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="E36" s="10"/>
-      <c r="F36" s="10"/>
-      <c r="G36" s="10"/>
-      <c r="H36" s="10"/>
-      <c r="I36" s="10"/>
-      <c r="J36" s="10"/>
-      <c r="K36" s="10"/>
-      <c r="L36" s="10"/>
-      <c r="M36" s="10"/>
-      <c r="N36" s="10"/>
-      <c r="O36" s="10"/>
-      <c r="P36" s="10"/>
-      <c r="Q36" s="10"/>
-      <c r="R36" s="10"/>
-      <c r="S36" s="10"/>
-    </row>
-    <row r="37" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="B37" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C37" s="8">
-        <v>0.75</v>
-      </c>
-      <c r="D37" s="8">
-        <v>0.75</v>
+      <c r="C37" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="D37" s="8" t="b">
+        <v>1</v>
       </c>
       <c r="E37" s="8"/>
       <c r="F37" s="8"/>
@@ -1735,16 +1702,16 @@
     </row>
     <row r="38" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="8" t="s">
-        <v>45</v>
+        <v>61</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C38" s="8" t="b">
-        <v>1</v>
-      </c>
-      <c r="D38" s="8" t="b">
-        <v>1</v>
+        <v>13</v>
+      </c>
+      <c r="C38" s="8">
+        <v>-0.5</v>
+      </c>
+      <c r="D38" s="8">
+        <v>-0.5</v>
       </c>
       <c r="E38" s="8"/>
       <c r="F38" s="8"/>
@@ -1827,16 +1794,16 @@
     </row>
     <row r="42" spans="1:19" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A42" s="10" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C42" s="8" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="D42" s="8" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="E42" s="8"/>
       <c r="F42" s="8"/>
@@ -1856,16 +1823,16 @@
     </row>
     <row r="43" spans="1:19" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A43" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="B43" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C43" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="B43" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="C43" s="8" t="s">
-        <v>31</v>
-      </c>
       <c r="D43" s="8" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="E43" s="8"/>
       <c r="F43" s="8"/>

</xml_diff>

<commit_message>
added context_fuel_upstream module and batch definition input fixed a bug where some vehicle characterstics were not being inherited properly changed context fuels table names to be consistent with context_XXX modules
Signed-off-by: kevinanewman <newman.kevin@epa.gov>
</commit_message>
<xml_diff>
--- a/input_samples/multiple_session_batch.xlsx
+++ b/input_samples/multiple_session_batch.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\GitHub\EPA_OMEGA_Model\input_samples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49042595-0D08-459A-8A92-55C254113FA7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B668B380-DDB0-44B8-9189-8A2DBA1B7F76}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3030" yWindow="465" windowWidth="20115" windowHeight="19695" tabRatio="151" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="405" yWindow="735" windowWidth="17625" windowHeight="16530" tabRatio="151" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sessions" sheetId="5" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="64">
   <si>
     <t>Parameter</t>
   </si>
@@ -223,6 +223,12 @@
   </si>
   <si>
     <t>New Vehicle Price Sales Response Elasticity</t>
+  </si>
+  <si>
+    <t>Context Fuel Upstream File</t>
+  </si>
+  <si>
+    <t>input_samples/context_fuel_upstream.csv</t>
   </si>
 </sst>
 </file>
@@ -715,11 +721,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AG44"/>
+  <dimension ref="A1:AG45"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane ySplit="10" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A38" sqref="A38"/>
+      <selection pane="bottomLeft" activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1179,16 +1185,16 @@
     </row>
     <row r="19" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="8" t="s">
-        <v>56</v>
+        <v>62</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>3</v>
       </c>
       <c r="C19" s="8" t="s">
-        <v>57</v>
+        <v>63</v>
       </c>
       <c r="D19" s="8" t="s">
-        <v>57</v>
+        <v>63</v>
       </c>
       <c r="E19" s="8"/>
       <c r="F19" s="8"/>
@@ -1208,16 +1214,16 @@
     </row>
     <row r="20" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="8" t="s">
-        <v>18</v>
+        <v>56</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>3</v>
       </c>
       <c r="C20" s="8" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="D20" s="8" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="E20" s="8"/>
       <c r="F20" s="8"/>
@@ -1237,16 +1243,16 @@
     </row>
     <row r="21" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="8" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>3</v>
       </c>
       <c r="C21" s="8" t="s">
-        <v>43</v>
+        <v>54</v>
       </c>
       <c r="D21" s="8" t="s">
-        <v>43</v>
+        <v>54</v>
       </c>
       <c r="E21" s="8"/>
       <c r="F21" s="8"/>
@@ -1264,47 +1270,47 @@
       <c r="R21" s="8"/>
       <c r="S21" s="8"/>
     </row>
-    <row r="22" spans="1:19" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="10" t="s">
-        <v>21</v>
+    <row r="22" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="8" t="s">
+        <v>20</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C22" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="D22" s="10" t="s">
-        <v>47</v>
-      </c>
-      <c r="E22" s="10"/>
-      <c r="F22" s="10"/>
-      <c r="G22" s="10"/>
-      <c r="H22" s="10"/>
-      <c r="I22" s="10"/>
-      <c r="J22" s="10"/>
-      <c r="K22" s="10"/>
-      <c r="L22" s="10"/>
-      <c r="M22" s="10"/>
-      <c r="N22" s="10"/>
-      <c r="O22" s="10"/>
-      <c r="P22" s="10"/>
-      <c r="Q22" s="10"/>
-      <c r="R22" s="10"/>
-      <c r="S22" s="10"/>
+      <c r="C22" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="D22" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="E22" s="8"/>
+      <c r="F22" s="8"/>
+      <c r="G22" s="8"/>
+      <c r="H22" s="8"/>
+      <c r="I22" s="8"/>
+      <c r="J22" s="8"/>
+      <c r="K22" s="8"/>
+      <c r="L22" s="8"/>
+      <c r="M22" s="8"/>
+      <c r="N22" s="8"/>
+      <c r="O22" s="8"/>
+      <c r="P22" s="8"/>
+      <c r="Q22" s="8"/>
+      <c r="R22" s="8"/>
+      <c r="S22" s="8"/>
     </row>
     <row r="23" spans="1:19" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="8" t="s">
-        <v>36</v>
+      <c r="A23" s="10" t="s">
+        <v>21</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C23" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="D23" s="8" t="s">
-        <v>45</v>
+      <c r="C23" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="D23" s="10" t="s">
+        <v>47</v>
       </c>
       <c r="E23" s="10"/>
       <c r="F23" s="10"/>
@@ -1322,94 +1328,106 @@
       <c r="R23" s="10"/>
       <c r="S23" s="10"/>
     </row>
-    <row r="24" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:19" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>3</v>
       </c>
       <c r="C24" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="D24" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="E24" s="10"/>
+      <c r="F24" s="10"/>
+      <c r="G24" s="10"/>
+      <c r="H24" s="10"/>
+      <c r="I24" s="10"/>
+      <c r="J24" s="10"/>
+      <c r="K24" s="10"/>
+      <c r="L24" s="10"/>
+      <c r="M24" s="10"/>
+      <c r="N24" s="10"/>
+      <c r="O24" s="10"/>
+      <c r="P24" s="10"/>
+      <c r="Q24" s="10"/>
+      <c r="R24" s="10"/>
+      <c r="S24" s="10"/>
+    </row>
+    <row r="25" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C25" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="D24" s="8" t="s">
+      <c r="D25" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="E24" s="8"/>
-      <c r="F24" s="8"/>
-      <c r="G24" s="8"/>
-      <c r="H24" s="8"/>
-      <c r="I24" s="8"/>
-      <c r="J24" s="8"/>
-      <c r="K24" s="8"/>
-      <c r="L24" s="8"/>
-      <c r="M24" s="8"/>
-      <c r="N24" s="8"/>
-      <c r="O24" s="8"/>
-      <c r="P24" s="8"/>
-      <c r="Q24" s="8"/>
-      <c r="R24" s="8"/>
-      <c r="S24" s="8"/>
-    </row>
-    <row r="25" spans="1:19" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="10" t="s">
+      <c r="E25" s="8"/>
+      <c r="F25" s="8"/>
+      <c r="G25" s="8"/>
+      <c r="H25" s="8"/>
+      <c r="I25" s="8"/>
+      <c r="J25" s="8"/>
+      <c r="K25" s="8"/>
+      <c r="L25" s="8"/>
+      <c r="M25" s="8"/>
+      <c r="N25" s="8"/>
+      <c r="O25" s="8"/>
+      <c r="P25" s="8"/>
+      <c r="Q25" s="8"/>
+      <c r="R25" s="8"/>
+      <c r="S25" s="8"/>
+    </row>
+    <row r="26" spans="1:19" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="10" t="s">
         <v>15</v>
-      </c>
-      <c r="B25" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C25" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="D25" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="E25" s="10"/>
-      <c r="F25" s="10"/>
-      <c r="G25" s="10"/>
-      <c r="H25" s="10"/>
-      <c r="I25" s="10"/>
-      <c r="J25" s="10"/>
-      <c r="K25" s="10"/>
-      <c r="L25" s="10"/>
-      <c r="M25" s="10"/>
-      <c r="N25" s="10"/>
-      <c r="O25" s="10"/>
-      <c r="P25" s="10"/>
-      <c r="Q25" s="10"/>
-      <c r="R25" s="10"/>
-      <c r="S25" s="10"/>
-    </row>
-    <row r="26" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="10" t="s">
-        <v>25</v>
       </c>
       <c r="B26" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C26" s="8" t="b">
+      <c r="C26" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="D26" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="E26" s="10"/>
+      <c r="F26" s="10"/>
+      <c r="G26" s="10"/>
+      <c r="H26" s="10"/>
+      <c r="I26" s="10"/>
+      <c r="J26" s="10"/>
+      <c r="K26" s="10"/>
+      <c r="L26" s="10"/>
+      <c r="M26" s="10"/>
+      <c r="N26" s="10"/>
+      <c r="O26" s="10"/>
+      <c r="P26" s="10"/>
+      <c r="Q26" s="10"/>
+      <c r="R26" s="10"/>
+      <c r="S26" s="10"/>
+    </row>
+    <row r="27" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C27" s="8" t="b">
         <v>1</v>
       </c>
-      <c r="D26" s="8" t="b">
+      <c r="D27" s="8" t="b">
         <v>1</v>
       </c>
-      <c r="E26" s="8"/>
-      <c r="F26" s="8"/>
-      <c r="G26" s="8"/>
-      <c r="H26" s="8"/>
-      <c r="I26" s="8"/>
-      <c r="J26" s="8"/>
-      <c r="K26" s="8"/>
-      <c r="L26" s="8"/>
-      <c r="M26" s="8"/>
-      <c r="N26" s="8"/>
-      <c r="O26" s="8"/>
-      <c r="P26" s="8"/>
-      <c r="Q26" s="8"/>
-      <c r="R26" s="8"/>
-      <c r="S26" s="8"/>
-    </row>
-    <row r="27" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E27" s="8"/>
       <c r="F27" s="8"/>
       <c r="G27" s="8"/>
@@ -1426,32 +1444,27 @@
       <c r="R27" s="8"/>
       <c r="S27" s="8"/>
     </row>
-    <row r="28" spans="1:19" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="15"/>
-      <c r="C28" s="15"/>
-      <c r="D28" s="15"/>
-      <c r="E28" s="14"/>
-      <c r="F28" s="14"/>
-      <c r="G28" s="14"/>
-      <c r="H28" s="14"/>
-      <c r="I28" s="14"/>
-      <c r="J28" s="14"/>
-      <c r="K28" s="14"/>
-      <c r="L28" s="14"/>
-      <c r="M28" s="14"/>
-      <c r="N28" s="14"/>
-      <c r="O28" s="14"/>
-      <c r="P28" s="14"/>
-      <c r="Q28" s="14"/>
-      <c r="R28" s="14"/>
-      <c r="S28" s="14"/>
-    </row>
-    <row r="29" spans="1:19" s="12" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A29" s="20" t="s">
-        <v>8</v>
-      </c>
-      <c r="C29" s="14"/>
-      <c r="D29" s="14"/>
+    <row r="28" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E28" s="8"/>
+      <c r="F28" s="8"/>
+      <c r="G28" s="8"/>
+      <c r="H28" s="8"/>
+      <c r="I28" s="8"/>
+      <c r="J28" s="8"/>
+      <c r="K28" s="8"/>
+      <c r="L28" s="8"/>
+      <c r="M28" s="8"/>
+      <c r="N28" s="8"/>
+      <c r="O28" s="8"/>
+      <c r="P28" s="8"/>
+      <c r="Q28" s="8"/>
+      <c r="R28" s="8"/>
+      <c r="S28" s="8"/>
+    </row>
+    <row r="29" spans="1:19" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="15"/>
+      <c r="C29" s="15"/>
+      <c r="D29" s="15"/>
       <c r="E29" s="14"/>
       <c r="F29" s="14"/>
       <c r="G29" s="14"/>
@@ -1468,38 +1481,31 @@
       <c r="R29" s="14"/>
       <c r="S29" s="14"/>
     </row>
-    <row r="30" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="B30" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C30" s="8">
-        <v>15</v>
-      </c>
-      <c r="D30" s="8">
-        <v>15</v>
-      </c>
-      <c r="E30" s="8"/>
-      <c r="F30" s="8"/>
-      <c r="G30" s="8"/>
-      <c r="H30" s="8"/>
-      <c r="I30" s="8"/>
-      <c r="J30" s="8"/>
-      <c r="K30" s="8"/>
-      <c r="L30" s="8"/>
-      <c r="M30" s="8"/>
-      <c r="N30" s="8"/>
-      <c r="O30" s="8"/>
-      <c r="P30" s="8"/>
-      <c r="Q30" s="8"/>
-      <c r="R30" s="8"/>
-      <c r="S30" s="8"/>
+    <row r="30" spans="1:19" s="12" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A30" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="C30" s="14"/>
+      <c r="D30" s="14"/>
+      <c r="E30" s="14"/>
+      <c r="F30" s="14"/>
+      <c r="G30" s="14"/>
+      <c r="H30" s="14"/>
+      <c r="I30" s="14"/>
+      <c r="J30" s="14"/>
+      <c r="K30" s="14"/>
+      <c r="L30" s="14"/>
+      <c r="M30" s="14"/>
+      <c r="N30" s="14"/>
+      <c r="O30" s="14"/>
+      <c r="P30" s="14"/>
+      <c r="Q30" s="14"/>
+      <c r="R30" s="14"/>
+      <c r="S30" s="14"/>
     </row>
     <row r="31" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="8" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B31" s="3" t="s">
         <v>13</v>
@@ -1508,7 +1514,7 @@
         <v>15</v>
       </c>
       <c r="D31" s="8">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="E31" s="8"/>
       <c r="F31" s="8"/>
@@ -1528,13 +1534,13 @@
     </row>
     <row r="32" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B32" s="3" t="s">
         <v>13</v>
       </c>
       <c r="C32" s="8">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="D32" s="8">
         <v>5</v>
@@ -1557,13 +1563,13 @@
     </row>
     <row r="33" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="8" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="B33" s="3" t="s">
         <v>13</v>
       </c>
       <c r="C33" s="8">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="D33" s="8">
         <v>5</v>
@@ -1586,13 +1592,13 @@
     </row>
     <row r="34" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="8" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B34" s="3" t="s">
         <v>13</v>
       </c>
       <c r="C34" s="8">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="D34" s="8">
         <v>5</v>
@@ -1613,76 +1619,76 @@
       <c r="R34" s="8"/>
       <c r="S34" s="8"/>
     </row>
-    <row r="35" spans="1:19" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="10" t="s">
+    <row r="35" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C35" s="8">
+        <v>2</v>
+      </c>
+      <c r="D35" s="8">
+        <v>5</v>
+      </c>
+      <c r="E35" s="8"/>
+      <c r="F35" s="8"/>
+      <c r="G35" s="8"/>
+      <c r="H35" s="8"/>
+      <c r="I35" s="8"/>
+      <c r="J35" s="8"/>
+      <c r="K35" s="8"/>
+      <c r="L35" s="8"/>
+      <c r="M35" s="8"/>
+      <c r="N35" s="8"/>
+      <c r="O35" s="8"/>
+      <c r="P35" s="8"/>
+      <c r="Q35" s="8"/>
+      <c r="R35" s="8"/>
+      <c r="S35" s="8"/>
+    </row>
+    <row r="36" spans="1:19" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="B35" s="3" t="s">
+      <c r="B36" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C35" s="10" t="b">
+      <c r="C36" s="10" t="b">
         <v>0</v>
       </c>
-      <c r="D35" s="10" t="s">
+      <c r="D36" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="E35" s="10"/>
-      <c r="F35" s="10"/>
-      <c r="G35" s="10"/>
-      <c r="H35" s="10"/>
-      <c r="I35" s="10"/>
-      <c r="J35" s="10"/>
-      <c r="K35" s="10"/>
-      <c r="L35" s="10"/>
-      <c r="M35" s="10"/>
-      <c r="N35" s="10"/>
-      <c r="O35" s="10"/>
-      <c r="P35" s="10"/>
-      <c r="Q35" s="10"/>
-      <c r="R35" s="10"/>
-      <c r="S35" s="10"/>
-    </row>
-    <row r="36" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="10" t="s">
+      <c r="E36" s="10"/>
+      <c r="F36" s="10"/>
+      <c r="G36" s="10"/>
+      <c r="H36" s="10"/>
+      <c r="I36" s="10"/>
+      <c r="J36" s="10"/>
+      <c r="K36" s="10"/>
+      <c r="L36" s="10"/>
+      <c r="M36" s="10"/>
+      <c r="N36" s="10"/>
+      <c r="O36" s="10"/>
+      <c r="P36" s="10"/>
+      <c r="Q36" s="10"/>
+      <c r="R36" s="10"/>
+      <c r="S36" s="10"/>
+    </row>
+    <row r="37" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="B36" s="4" t="s">
+      <c r="B37" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C36" s="8">
+      <c r="C37" s="8">
         <v>0.75</v>
       </c>
-      <c r="D36" s="8">
+      <c r="D37" s="8">
         <v>0.75</v>
-      </c>
-      <c r="E36" s="8"/>
-      <c r="F36" s="8"/>
-      <c r="G36" s="8"/>
-      <c r="H36" s="8"/>
-      <c r="I36" s="8"/>
-      <c r="J36" s="8"/>
-      <c r="K36" s="8"/>
-      <c r="L36" s="8"/>
-      <c r="M36" s="8"/>
-      <c r="N36" s="8"/>
-      <c r="O36" s="8"/>
-      <c r="P36" s="8"/>
-      <c r="Q36" s="8"/>
-      <c r="R36" s="8"/>
-      <c r="S36" s="8"/>
-    </row>
-    <row r="37" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="B37" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C37" s="8" t="b">
-        <v>1</v>
-      </c>
-      <c r="D37" s="8" t="b">
-        <v>1</v>
       </c>
       <c r="E37" s="8"/>
       <c r="F37" s="8"/>
@@ -1702,16 +1708,16 @@
     </row>
     <row r="38" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="8" t="s">
-        <v>61</v>
+        <v>38</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C38" s="8">
-        <v>-0.5</v>
-      </c>
-      <c r="D38" s="8">
-        <v>-0.5</v>
+        <v>11</v>
+      </c>
+      <c r="C38" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="D38" s="8" t="b">
+        <v>1</v>
       </c>
       <c r="E38" s="8"/>
       <c r="F38" s="8"/>
@@ -1730,10 +1736,18 @@
       <c r="S38" s="8"/>
     </row>
     <row r="39" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="8"/>
-      <c r="B39" s="3"/>
-      <c r="C39" s="8"/>
-      <c r="D39" s="8"/>
+      <c r="A39" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="B39" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C39" s="8">
+        <v>-0.5</v>
+      </c>
+      <c r="D39" s="8">
+        <v>-0.5</v>
+      </c>
       <c r="E39" s="8"/>
       <c r="F39" s="8"/>
       <c r="G39" s="8"/>
@@ -1750,32 +1764,31 @@
       <c r="R39" s="8"/>
       <c r="S39" s="8"/>
     </row>
-    <row r="40" spans="1:19" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="15"/>
-      <c r="C40" s="15"/>
-      <c r="D40" s="15"/>
-      <c r="E40" s="14"/>
-      <c r="F40" s="14"/>
-      <c r="G40" s="14"/>
-      <c r="H40" s="14"/>
-      <c r="I40" s="14"/>
-      <c r="J40" s="14"/>
-      <c r="K40" s="14"/>
-      <c r="L40" s="14"/>
-      <c r="M40" s="14"/>
-      <c r="N40" s="14"/>
-      <c r="O40" s="14"/>
-      <c r="P40" s="14"/>
-      <c r="Q40" s="14"/>
-      <c r="R40" s="14"/>
-      <c r="S40" s="14"/>
-    </row>
-    <row r="41" spans="1:19" s="12" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A41" s="20" t="s">
-        <v>7</v>
-      </c>
-      <c r="C41" s="14"/>
-      <c r="D41" s="14"/>
+    <row r="40" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="8"/>
+      <c r="B40" s="3"/>
+      <c r="C40" s="8"/>
+      <c r="D40" s="8"/>
+      <c r="E40" s="8"/>
+      <c r="F40" s="8"/>
+      <c r="G40" s="8"/>
+      <c r="H40" s="8"/>
+      <c r="I40" s="8"/>
+      <c r="J40" s="8"/>
+      <c r="K40" s="8"/>
+      <c r="L40" s="8"/>
+      <c r="M40" s="8"/>
+      <c r="N40" s="8"/>
+      <c r="O40" s="8"/>
+      <c r="P40" s="8"/>
+      <c r="Q40" s="8"/>
+      <c r="R40" s="8"/>
+      <c r="S40" s="8"/>
+    </row>
+    <row r="41" spans="1:19" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="15"/>
+      <c r="C41" s="15"/>
+      <c r="D41" s="15"/>
       <c r="E41" s="14"/>
       <c r="F41" s="14"/>
       <c r="G41" s="14"/>
@@ -1792,38 +1805,31 @@
       <c r="R41" s="14"/>
       <c r="S41" s="14"/>
     </row>
-    <row r="42" spans="1:19" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A42" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="B42" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="C42" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="D42" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="E42" s="8"/>
-      <c r="F42" s="8"/>
-      <c r="G42" s="8"/>
-      <c r="H42" s="8"/>
-      <c r="I42" s="8"/>
-      <c r="J42" s="8"/>
-      <c r="K42" s="8"/>
-      <c r="L42" s="8"/>
-      <c r="M42" s="8"/>
-      <c r="N42" s="8"/>
-      <c r="O42" s="8"/>
-      <c r="P42" s="8"/>
-      <c r="Q42" s="8"/>
-      <c r="R42" s="8"/>
-      <c r="S42" s="8"/>
+    <row r="42" spans="1:19" s="12" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A42" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="C42" s="14"/>
+      <c r="D42" s="14"/>
+      <c r="E42" s="14"/>
+      <c r="F42" s="14"/>
+      <c r="G42" s="14"/>
+      <c r="H42" s="14"/>
+      <c r="I42" s="14"/>
+      <c r="J42" s="14"/>
+      <c r="K42" s="14"/>
+      <c r="L42" s="14"/>
+      <c r="M42" s="14"/>
+      <c r="N42" s="14"/>
+      <c r="O42" s="14"/>
+      <c r="P42" s="14"/>
+      <c r="Q42" s="14"/>
+      <c r="R42" s="14"/>
+      <c r="S42" s="14"/>
     </row>
     <row r="43" spans="1:19" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A43" s="10" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B43" s="3" t="s">
         <v>22</v>
@@ -1850,11 +1856,19 @@
       <c r="R43" s="8"/>
       <c r="S43" s="8"/>
     </row>
-    <row r="44" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="8"/>
-      <c r="B44" s="3"/>
-      <c r="C44" s="8"/>
-      <c r="D44" s="8"/>
+    <row r="44" spans="1:19" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A44" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="B44" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C44" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="D44" s="8" t="s">
+        <v>27</v>
+      </c>
       <c r="E44" s="8"/>
       <c r="F44" s="8"/>
       <c r="G44" s="8"/>
@@ -1871,6 +1885,27 @@
       <c r="R44" s="8"/>
       <c r="S44" s="8"/>
     </row>
+    <row r="45" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="8"/>
+      <c r="B45" s="3"/>
+      <c r="C45" s="8"/>
+      <c r="D45" s="8"/>
+      <c r="E45" s="8"/>
+      <c r="F45" s="8"/>
+      <c r="G45" s="8"/>
+      <c r="H45" s="8"/>
+      <c r="I45" s="8"/>
+      <c r="J45" s="8"/>
+      <c r="K45" s="8"/>
+      <c r="L45" s="8"/>
+      <c r="M45" s="8"/>
+      <c r="N45" s="8"/>
+      <c r="O45" s="8"/>
+      <c r="P45" s="8"/>
+      <c r="Q45" s="8"/>
+      <c r="R45" s="8"/>
+      <c r="S45" s="8"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Changing "Fixed" and "Dynamic" to "fixed" and "dynamic" in the stock/postproc settings of the batch process.
</commit_message>
<xml_diff>
--- a/input_samples/multiple_session_batch.xlsx
+++ b/input_samples/multiple_session_batch.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\GitHub\EPA_OMEGA_Model\input_samples\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TSHERWOO\Documents\GitHub\EPA_OMEGA_Model\input_samples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B668B380-DDB0-44B8-9189-8A2DBA1B7F76}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D91821BD-782B-4AA5-A65F-E78B558B43D5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="405" yWindow="735" windowWidth="17625" windowHeight="16530" tabRatio="151" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" tabRatio="151" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sessions" sheetId="5" r:id="rId1"/>
@@ -104,10 +104,6 @@
     <t>GHG Standards File</t>
   </si>
   <si>
-    <t>Fixed
-Dynamic</t>
-  </si>
-  <si>
     <t>Stock Deregistration</t>
   </si>
   <si>
@@ -120,9 +116,6 @@
     <t>Allow Backsliding</t>
   </si>
   <si>
-    <t>Fixed</t>
-  </si>
-  <si>
     <t>Cost Curve Frontier Affinity Factor</t>
   </si>
   <si>
@@ -229,6 +222,13 @@
   </si>
   <si>
     <t>input_samples/context_fuel_upstream.csv</t>
+  </si>
+  <si>
+    <t>fixed</t>
+  </si>
+  <si>
+    <t>fixed
+dynamic</t>
   </si>
 </sst>
 </file>
@@ -723,24 +723,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AG45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="10" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C19" sqref="C19"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane ySplit="10" topLeftCell="A42" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B45" sqref="B45"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="42" style="11" customWidth="1"/>
-    <col min="2" max="2" width="17.28515625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="17.33203125" style="1" customWidth="1"/>
     <col min="3" max="4" width="48" style="11" bestFit="1" customWidth="1"/>
-    <col min="5" max="17" width="21.28515625" style="11" customWidth="1"/>
-    <col min="18" max="18" width="16.7109375" style="1" customWidth="1"/>
+    <col min="5" max="17" width="21.33203125" style="11" customWidth="1"/>
+    <col min="18" max="18" width="16.6640625" style="1" customWidth="1"/>
     <col min="19" max="19" width="18" style="1" customWidth="1"/>
-    <col min="20" max="20" width="16.42578125" style="1" customWidth="1"/>
-    <col min="21" max="16384" width="8.7109375" style="1"/>
+    <col min="20" max="20" width="16.44140625" style="1" customWidth="1"/>
+    <col min="21" max="16384" width="8.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" s="18" customFormat="1" ht="21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:33" s="18" customFormat="1" ht="21" x14ac:dyDescent="0.3">
       <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
@@ -781,7 +781,7 @@
       <c r="AF1" s="17"/>
       <c r="AG1" s="17"/>
     </row>
-    <row r="2" spans="1:33" s="12" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:33" s="12" customFormat="1" ht="18" x14ac:dyDescent="0.3">
       <c r="A2" s="19" t="s">
         <v>10</v>
       </c>
@@ -801,7 +801,7 @@
       <c r="P2" s="14"/>
       <c r="Q2" s="14"/>
     </row>
-    <row r="3" spans="1:33" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:33" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
         <v>4</v>
       </c>
@@ -809,7 +809,7 @@
         <v>3</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D3" s="14"/>
       <c r="E3" s="14"/>
@@ -826,9 +826,9 @@
       <c r="P3" s="14"/>
       <c r="Q3" s="14"/>
     </row>
-    <row r="4" spans="1:33" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:33" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B4" s="6" t="s">
         <v>3</v>
@@ -849,29 +849,29 @@
       <c r="P4" s="14"/>
       <c r="Q4" s="14"/>
     </row>
-    <row r="5" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B5" s="6" t="s">
         <v>3</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="6" spans="1:33" x14ac:dyDescent="0.25">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="6" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B6" s="6" t="s">
         <v>3</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="7" spans="1:33" s="12" customFormat="1" x14ac:dyDescent="0.25">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="7" spans="1:33" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="14"/>
       <c r="C7" s="14"/>
       <c r="D7" s="14"/>
@@ -889,7 +889,7 @@
       <c r="P7" s="14"/>
       <c r="Q7" s="14"/>
     </row>
-    <row r="8" spans="1:33" s="12" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:33" s="12" customFormat="1" ht="18" x14ac:dyDescent="0.3">
       <c r="A8" s="20" t="s">
         <v>9</v>
       </c>
@@ -909,7 +909,7 @@
       <c r="P8" s="14"/>
       <c r="Q8" s="14"/>
     </row>
-    <row r="9" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="8" t="s">
         <v>5</v>
       </c>
@@ -938,7 +938,7 @@
       <c r="R9" s="8"/>
       <c r="S9" s="8"/>
     </row>
-    <row r="10" spans="1:33" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:33" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A10" s="9" t="s">
         <v>2</v>
       </c>
@@ -946,10 +946,10 @@
         <v>3</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E10" s="9"/>
       <c r="F10" s="9"/>
@@ -967,7 +967,7 @@
       <c r="R10" s="9"/>
       <c r="S10" s="9"/>
     </row>
-    <row r="11" spans="1:33" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:33" s="16" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A11" s="15"/>
       <c r="C11" s="15"/>
       <c r="D11" s="15"/>
@@ -987,7 +987,7 @@
       <c r="R11" s="14"/>
       <c r="S11" s="14"/>
     </row>
-    <row r="12" spans="1:33" s="12" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:33" s="12" customFormat="1" ht="18" x14ac:dyDescent="0.3">
       <c r="A12" s="13" t="s">
         <v>6</v>
       </c>
@@ -1009,7 +1009,7 @@
       <c r="R12" s="14"/>
       <c r="S12" s="14"/>
     </row>
-    <row r="13" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A13" s="8" t="s">
         <v>14</v>
       </c>
@@ -1017,10 +1017,10 @@
         <v>3</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="E13" s="8"/>
       <c r="F13" s="8"/>
@@ -1038,7 +1038,7 @@
       <c r="R13" s="8"/>
       <c r="S13" s="8"/>
     </row>
-    <row r="14" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A14" s="8" t="s">
         <v>16</v>
       </c>
@@ -1046,10 +1046,10 @@
         <v>3</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E14" s="8"/>
       <c r="F14" s="8"/>
@@ -1067,7 +1067,7 @@
       <c r="R14" s="8"/>
       <c r="S14" s="8"/>
     </row>
-    <row r="15" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A15" s="8" t="s">
         <v>17</v>
       </c>
@@ -1075,10 +1075,10 @@
         <v>3</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E15" s="8"/>
       <c r="F15" s="8"/>
@@ -1096,18 +1096,18 @@
       <c r="R15" s="8"/>
       <c r="S15" s="8"/>
     </row>
-    <row r="16" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A16" s="8" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>3</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E16" s="8"/>
       <c r="F16" s="8"/>
@@ -1125,7 +1125,7 @@
       <c r="R16" s="8"/>
       <c r="S16" s="8"/>
     </row>
-    <row r="17" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A17" s="8" t="s">
         <v>19</v>
       </c>
@@ -1133,10 +1133,10 @@
         <v>3</v>
       </c>
       <c r="C17" s="8" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E17" s="8"/>
       <c r="F17" s="8"/>
@@ -1154,18 +1154,18 @@
       <c r="R17" s="8"/>
       <c r="S17" s="8"/>
     </row>
-    <row r="18" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A18" s="8" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>3</v>
       </c>
       <c r="C18" s="8" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D18" s="8" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E18" s="8"/>
       <c r="F18" s="8"/>
@@ -1183,18 +1183,18 @@
       <c r="R18" s="8"/>
       <c r="S18" s="8"/>
     </row>
-    <row r="19" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A19" s="8" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>3</v>
       </c>
       <c r="C19" s="8" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D19" s="8" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E19" s="8"/>
       <c r="F19" s="8"/>
@@ -1212,18 +1212,18 @@
       <c r="R19" s="8"/>
       <c r="S19" s="8"/>
     </row>
-    <row r="20" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A20" s="8" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>3</v>
       </c>
       <c r="C20" s="8" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D20" s="8" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E20" s="8"/>
       <c r="F20" s="8"/>
@@ -1241,7 +1241,7 @@
       <c r="R20" s="8"/>
       <c r="S20" s="8"/>
     </row>
-    <row r="21" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A21" s="8" t="s">
         <v>18</v>
       </c>
@@ -1249,10 +1249,10 @@
         <v>3</v>
       </c>
       <c r="C21" s="8" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D21" s="8" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E21" s="8"/>
       <c r="F21" s="8"/>
@@ -1270,7 +1270,7 @@
       <c r="R21" s="8"/>
       <c r="S21" s="8"/>
     </row>
-    <row r="22" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A22" s="8" t="s">
         <v>20</v>
       </c>
@@ -1278,10 +1278,10 @@
         <v>3</v>
       </c>
       <c r="C22" s="8" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D22" s="8" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E22" s="8"/>
       <c r="F22" s="8"/>
@@ -1299,7 +1299,7 @@
       <c r="R22" s="8"/>
       <c r="S22" s="8"/>
     </row>
-    <row r="23" spans="1:19" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:19" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A23" s="10" t="s">
         <v>21</v>
       </c>
@@ -1307,10 +1307,10 @@
         <v>3</v>
       </c>
       <c r="C23" s="10" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D23" s="10" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E23" s="10"/>
       <c r="F23" s="10"/>
@@ -1328,18 +1328,18 @@
       <c r="R23" s="10"/>
       <c r="S23" s="10"/>
     </row>
-    <row r="24" spans="1:19" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:19" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A24" s="8" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>3</v>
       </c>
       <c r="C24" s="8" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D24" s="8" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E24" s="10"/>
       <c r="F24" s="10"/>
@@ -1357,18 +1357,18 @@
       <c r="R24" s="10"/>
       <c r="S24" s="10"/>
     </row>
-    <row r="25" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A25" s="8" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B25" s="2" t="s">
         <v>3</v>
       </c>
       <c r="C25" s="8" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D25" s="8" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E25" s="8"/>
       <c r="F25" s="8"/>
@@ -1386,7 +1386,7 @@
       <c r="R25" s="8"/>
       <c r="S25" s="8"/>
     </row>
-    <row r="26" spans="1:19" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:19" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A26" s="10" t="s">
         <v>15</v>
       </c>
@@ -1415,9 +1415,9 @@
       <c r="R26" s="10"/>
       <c r="S26" s="10"/>
     </row>
-    <row r="27" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A27" s="10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B27" s="3" t="s">
         <v>11</v>
@@ -1444,7 +1444,7 @@
       <c r="R27" s="8"/>
       <c r="S27" s="8"/>
     </row>
-    <row r="28" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="E28" s="8"/>
       <c r="F28" s="8"/>
       <c r="G28" s="8"/>
@@ -1461,7 +1461,7 @@
       <c r="R28" s="8"/>
       <c r="S28" s="8"/>
     </row>
-    <row r="29" spans="1:19" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:19" s="16" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A29" s="15"/>
       <c r="C29" s="15"/>
       <c r="D29" s="15"/>
@@ -1481,7 +1481,7 @@
       <c r="R29" s="14"/>
       <c r="S29" s="14"/>
     </row>
-    <row r="30" spans="1:19" s="12" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:19" s="12" customFormat="1" ht="18" x14ac:dyDescent="0.3">
       <c r="A30" s="20" t="s">
         <v>8</v>
       </c>
@@ -1503,9 +1503,9 @@
       <c r="R30" s="14"/>
       <c r="S30" s="14"/>
     </row>
-    <row r="31" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A31" s="8" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B31" s="3" t="s">
         <v>13</v>
@@ -1532,9 +1532,9 @@
       <c r="R31" s="8"/>
       <c r="S31" s="8"/>
     </row>
-    <row r="32" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A32" s="8" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B32" s="3" t="s">
         <v>13</v>
@@ -1561,9 +1561,9 @@
       <c r="R32" s="8"/>
       <c r="S32" s="8"/>
     </row>
-    <row r="33" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A33" s="8" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B33" s="3" t="s">
         <v>13</v>
@@ -1590,9 +1590,9 @@
       <c r="R33" s="8"/>
       <c r="S33" s="8"/>
     </row>
-    <row r="34" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A34" s="8" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B34" s="3" t="s">
         <v>13</v>
@@ -1619,9 +1619,9 @@
       <c r="R34" s="8"/>
       <c r="S34" s="8"/>
     </row>
-    <row r="35" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A35" s="8" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B35" s="3" t="s">
         <v>13</v>
@@ -1648,9 +1648,9 @@
       <c r="R35" s="8"/>
       <c r="S35" s="8"/>
     </row>
-    <row r="36" spans="1:19" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:19" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A36" s="10" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B36" s="3" t="s">
         <v>11</v>
@@ -1659,7 +1659,7 @@
         <v>0</v>
       </c>
       <c r="D36" s="10" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E36" s="10"/>
       <c r="F36" s="10"/>
@@ -1677,9 +1677,9 @@
       <c r="R36" s="10"/>
       <c r="S36" s="10"/>
     </row>
-    <row r="37" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A37" s="10" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B37" s="4" t="s">
         <v>13</v>
@@ -1706,9 +1706,9 @@
       <c r="R37" s="8"/>
       <c r="S37" s="8"/>
     </row>
-    <row r="38" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A38" s="8" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B38" s="3" t="s">
         <v>11</v>
@@ -1735,9 +1735,9 @@
       <c r="R38" s="8"/>
       <c r="S38" s="8"/>
     </row>
-    <row r="39" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A39" s="8" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B39" s="3" t="s">
         <v>13</v>
@@ -1764,7 +1764,7 @@
       <c r="R39" s="8"/>
       <c r="S39" s="8"/>
     </row>
-    <row r="40" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A40" s="8"/>
       <c r="B40" s="3"/>
       <c r="C40" s="8"/>
@@ -1785,7 +1785,7 @@
       <c r="R40" s="8"/>
       <c r="S40" s="8"/>
     </row>
-    <row r="41" spans="1:19" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:19" s="16" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A41" s="15"/>
       <c r="C41" s="15"/>
       <c r="D41" s="15"/>
@@ -1805,7 +1805,7 @@
       <c r="R41" s="14"/>
       <c r="S41" s="14"/>
     </row>
-    <row r="42" spans="1:19" s="12" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:19" s="12" customFormat="1" ht="18" x14ac:dyDescent="0.3">
       <c r="A42" s="20" t="s">
         <v>7</v>
       </c>
@@ -1827,18 +1827,18 @@
       <c r="R42" s="14"/>
       <c r="S42" s="14"/>
     </row>
-    <row r="43" spans="1:19" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:19" s="2" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A43" s="10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>22</v>
+        <v>63</v>
       </c>
       <c r="C43" s="8" t="s">
-        <v>27</v>
+        <v>62</v>
       </c>
       <c r="D43" s="8" t="s">
-        <v>27</v>
+        <v>62</v>
       </c>
       <c r="E43" s="8"/>
       <c r="F43" s="8"/>
@@ -1856,18 +1856,18 @@
       <c r="R43" s="8"/>
       <c r="S43" s="8"/>
     </row>
-    <row r="44" spans="1:19" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:19" s="2" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A44" s="10" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>22</v>
+        <v>63</v>
       </c>
       <c r="C44" s="8" t="s">
-        <v>27</v>
+        <v>62</v>
       </c>
       <c r="D44" s="8" t="s">
-        <v>27</v>
+        <v>62</v>
       </c>
       <c r="E44" s="8"/>
       <c r="F44" s="8"/>
@@ -1885,7 +1885,7 @@
       <c r="R44" s="8"/>
       <c r="S44" s="8"/>
     </row>
-    <row r="45" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A45" s="8"/>
       <c r="B45" s="3"/>
       <c r="C45" s="8"/>

</xml_diff>

<commit_message>
New batch files with Stock files (VMT & registration) now part of I/O rather than postproc. Context cost & emission factor input files now part of postproc. The CSV files get copied into the bundle output, but the DB tables are not dumped (I need help).
</commit_message>
<xml_diff>
--- a/input_samples/multiple_session_batch.xlsx
+++ b/input_samples/multiple_session_batch.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TSHERWOO\Documents\GitHub\EPA_OMEGA_Model\input_samples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D91821BD-782B-4AA5-A65F-E78B558B43D5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{679DC5D9-7A81-49E7-A92B-3A7DFA4C5B16}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" tabRatio="151" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="6252" windowWidth="23040" windowHeight="6252" tabRatio="151" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sessions" sheetId="5" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="78">
   <si>
     <t>Parameter</t>
   </si>
@@ -104,12 +104,6 @@
     <t>GHG Standards File</t>
   </si>
   <si>
-    <t>Stock Deregistration</t>
-  </si>
-  <si>
-    <t>Stock VMT</t>
-  </si>
-  <si>
     <t>Slice Tech Combo Tables</t>
   </si>
   <si>
@@ -224,11 +218,58 @@
     <t>input_samples/context_fuel_upstream.csv</t>
   </si>
   <si>
-    <t>fixed</t>
-  </si>
-  <si>
-    <t>fixed
-dynamic</t>
+    <t>Stock Deregistration File</t>
+  </si>
+  <si>
+    <t>input_samples/reregistration_fixed_by_age.csv</t>
+  </si>
+  <si>
+    <t>Stock VMT File</t>
+  </si>
+  <si>
+    <t>input_samples/annual_vmt_fixed_by_age.csv</t>
+  </si>
+  <si>
+    <t>Context Criteria Cost Factors File</t>
+  </si>
+  <si>
+    <t>input_samples/context_cost_factors-criteria.csv</t>
+  </si>
+  <si>
+    <t>Context SCC Cost Factors File</t>
+  </si>
+  <si>
+    <t>input_samples/context_cost_factors-scc.csv</t>
+  </si>
+  <si>
+    <t>Context Powersector Emission Factors File</t>
+  </si>
+  <si>
+    <t>input_samples/context_emission_factors-powersector.csv</t>
+  </si>
+  <si>
+    <t>Context Refinery Emission Factors File</t>
+  </si>
+  <si>
+    <t>input_samples/context_emission_factors-refinery.csv</t>
+  </si>
+  <si>
+    <t>Context Vehicle Emission Factors File</t>
+  </si>
+  <si>
+    <t>input_samples/context_emission_factors-vehicles.csv</t>
+  </si>
+  <si>
+    <t>Context Implicit Price Deflators File</t>
+  </si>
+  <si>
+    <t>input_samples/context_implicit_price_deflators.csv</t>
+  </si>
+  <si>
+    <t>Context Consumer Price Index File</t>
+  </si>
+  <si>
+    <t>input_samples/context_cpi_price_deflators.csv</t>
   </si>
 </sst>
 </file>
@@ -351,7 +392,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -411,6 +452,33 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -721,11 +789,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AG45"/>
+  <dimension ref="A1:AG51"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="10" topLeftCell="A42" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B45" sqref="B45"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane ySplit="10" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D50" sqref="D50:D51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -809,7 +877,7 @@
         <v>3</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D3" s="14"/>
       <c r="E3" s="14"/>
@@ -828,7 +896,7 @@
     </row>
     <row r="4" spans="1:33" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B4" s="6" t="s">
         <v>3</v>
@@ -851,24 +919,24 @@
     </row>
     <row r="5" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B5" s="6" t="s">
         <v>3</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="6" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B6" s="6" t="s">
         <v>3</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="7" spans="1:33" s="12" customFormat="1" x14ac:dyDescent="0.3">
@@ -946,10 +1014,10 @@
         <v>3</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E10" s="9"/>
       <c r="F10" s="9"/>
@@ -1017,10 +1085,10 @@
         <v>3</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E13" s="8"/>
       <c r="F13" s="8"/>
@@ -1046,10 +1114,10 @@
         <v>3</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E14" s="8"/>
       <c r="F14" s="8"/>
@@ -1075,10 +1143,10 @@
         <v>3</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E15" s="8"/>
       <c r="F15" s="8"/>
@@ -1098,16 +1166,16 @@
     </row>
     <row r="16" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A16" s="8" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>3</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E16" s="8"/>
       <c r="F16" s="8"/>
@@ -1133,10 +1201,10 @@
         <v>3</v>
       </c>
       <c r="C17" s="8" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E17" s="8"/>
       <c r="F17" s="8"/>
@@ -1156,16 +1224,16 @@
     </row>
     <row r="18" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A18" s="8" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>3</v>
       </c>
       <c r="C18" s="8" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D18" s="8" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E18" s="8"/>
       <c r="F18" s="8"/>
@@ -1185,16 +1253,16 @@
     </row>
     <row r="19" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A19" s="8" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>3</v>
       </c>
       <c r="C19" s="8" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D19" s="8" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E19" s="8"/>
       <c r="F19" s="8"/>
@@ -1214,16 +1282,16 @@
     </row>
     <row r="20" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A20" s="8" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>3</v>
       </c>
       <c r="C20" s="8" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D20" s="8" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E20" s="8"/>
       <c r="F20" s="8"/>
@@ -1249,10 +1317,10 @@
         <v>3</v>
       </c>
       <c r="C21" s="8" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D21" s="8" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E21" s="8"/>
       <c r="F21" s="8"/>
@@ -1278,10 +1346,10 @@
         <v>3</v>
       </c>
       <c r="C22" s="8" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D22" s="8" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E22" s="8"/>
       <c r="F22" s="8"/>
@@ -1307,10 +1375,10 @@
         <v>3</v>
       </c>
       <c r="C23" s="10" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D23" s="10" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E23" s="10"/>
       <c r="F23" s="10"/>
@@ -1330,16 +1398,16 @@
     </row>
     <row r="24" spans="1:19" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A24" s="8" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>3</v>
       </c>
       <c r="C24" s="8" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D24" s="8" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E24" s="10"/>
       <c r="F24" s="10"/>
@@ -1359,16 +1427,16 @@
     </row>
     <row r="25" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A25" s="8" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B25" s="2" t="s">
         <v>3</v>
       </c>
       <c r="C25" s="8" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D25" s="8" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E25" s="8"/>
       <c r="F25" s="8"/>
@@ -1386,47 +1454,47 @@
       <c r="R25" s="8"/>
       <c r="S25" s="8"/>
     </row>
-    <row r="26" spans="1:19" s="4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="B26" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C26" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="D26" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="E26" s="10"/>
-      <c r="F26" s="10"/>
-      <c r="G26" s="10"/>
-      <c r="H26" s="10"/>
-      <c r="I26" s="10"/>
-      <c r="J26" s="10"/>
-      <c r="K26" s="10"/>
-      <c r="L26" s="10"/>
-      <c r="M26" s="10"/>
-      <c r="N26" s="10"/>
-      <c r="O26" s="10"/>
-      <c r="P26" s="10"/>
-      <c r="Q26" s="10"/>
-      <c r="R26" s="10"/>
-      <c r="S26" s="10"/>
+    <row r="26" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="23" t="s">
+        <v>60</v>
+      </c>
+      <c r="B26" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="C26" s="22" t="s">
+        <v>61</v>
+      </c>
+      <c r="D26" s="22" t="s">
+        <v>61</v>
+      </c>
+      <c r="E26" s="8"/>
+      <c r="F26" s="8"/>
+      <c r="G26" s="8"/>
+      <c r="H26" s="8"/>
+      <c r="I26" s="8"/>
+      <c r="J26" s="8"/>
+      <c r="K26" s="8"/>
+      <c r="L26" s="8"/>
+      <c r="M26" s="8"/>
+      <c r="N26" s="8"/>
+      <c r="O26" s="8"/>
+      <c r="P26" s="8"/>
+      <c r="Q26" s="8"/>
+      <c r="R26" s="8"/>
+      <c r="S26" s="8"/>
     </row>
     <row r="27" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="B27" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C27" s="8" t="b">
-        <v>1</v>
-      </c>
-      <c r="D27" s="8" t="b">
-        <v>1</v>
+      <c r="A27" s="23" t="s">
+        <v>62</v>
+      </c>
+      <c r="B27" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="C27" s="22" t="s">
+        <v>63</v>
+      </c>
+      <c r="D27" s="22" t="s">
+        <v>63</v>
       </c>
       <c r="E27" s="8"/>
       <c r="F27" s="8"/>
@@ -1444,135 +1512,135 @@
       <c r="R27" s="8"/>
       <c r="S27" s="8"/>
     </row>
-    <row r="28" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="E28" s="8"/>
-      <c r="F28" s="8"/>
-      <c r="G28" s="8"/>
-      <c r="H28" s="8"/>
-      <c r="I28" s="8"/>
-      <c r="J28" s="8"/>
-      <c r="K28" s="8"/>
-      <c r="L28" s="8"/>
-      <c r="M28" s="8"/>
-      <c r="N28" s="8"/>
-      <c r="O28" s="8"/>
-      <c r="P28" s="8"/>
-      <c r="Q28" s="8"/>
-      <c r="R28" s="8"/>
-      <c r="S28" s="8"/>
-    </row>
-    <row r="29" spans="1:19" s="16" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="15"/>
-      <c r="C29" s="15"/>
-      <c r="D29" s="15"/>
-      <c r="E29" s="14"/>
-      <c r="F29" s="14"/>
-      <c r="G29" s="14"/>
-      <c r="H29" s="14"/>
-      <c r="I29" s="14"/>
-      <c r="J29" s="14"/>
-      <c r="K29" s="14"/>
-      <c r="L29" s="14"/>
-      <c r="M29" s="14"/>
-      <c r="N29" s="14"/>
-      <c r="O29" s="14"/>
-      <c r="P29" s="14"/>
-      <c r="Q29" s="14"/>
-      <c r="R29" s="14"/>
-      <c r="S29" s="14"/>
-    </row>
-    <row r="30" spans="1:19" s="12" customFormat="1" ht="18" x14ac:dyDescent="0.3">
-      <c r="A30" s="20" t="s">
+    <row r="28" spans="1:19" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C28" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="D28" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="E28" s="10"/>
+      <c r="F28" s="10"/>
+      <c r="G28" s="10"/>
+      <c r="H28" s="10"/>
+      <c r="I28" s="10"/>
+      <c r="J28" s="10"/>
+      <c r="K28" s="10"/>
+      <c r="L28" s="10"/>
+      <c r="M28" s="10"/>
+      <c r="N28" s="10"/>
+      <c r="O28" s="10"/>
+      <c r="P28" s="10"/>
+      <c r="Q28" s="10"/>
+      <c r="R28" s="10"/>
+      <c r="S28" s="10"/>
+    </row>
+    <row r="29" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C29" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="D29" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="E29" s="8"/>
+      <c r="F29" s="8"/>
+      <c r="G29" s="8"/>
+      <c r="H29" s="8"/>
+      <c r="I29" s="8"/>
+      <c r="J29" s="8"/>
+      <c r="K29" s="8"/>
+      <c r="L29" s="8"/>
+      <c r="M29" s="8"/>
+      <c r="N29" s="8"/>
+      <c r="O29" s="8"/>
+      <c r="P29" s="8"/>
+      <c r="Q29" s="8"/>
+      <c r="R29" s="8"/>
+      <c r="S29" s="8"/>
+    </row>
+    <row r="30" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="E30" s="8"/>
+      <c r="F30" s="8"/>
+      <c r="G30" s="8"/>
+      <c r="H30" s="8"/>
+      <c r="I30" s="8"/>
+      <c r="J30" s="8"/>
+      <c r="K30" s="8"/>
+      <c r="L30" s="8"/>
+      <c r="M30" s="8"/>
+      <c r="N30" s="8"/>
+      <c r="O30" s="8"/>
+      <c r="P30" s="8"/>
+      <c r="Q30" s="8"/>
+      <c r="R30" s="8"/>
+      <c r="S30" s="8"/>
+    </row>
+    <row r="31" spans="1:19" s="16" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="15"/>
+      <c r="C31" s="15"/>
+      <c r="D31" s="15"/>
+      <c r="E31" s="14"/>
+      <c r="F31" s="14"/>
+      <c r="G31" s="14"/>
+      <c r="H31" s="14"/>
+      <c r="I31" s="14"/>
+      <c r="J31" s="14"/>
+      <c r="K31" s="14"/>
+      <c r="L31" s="14"/>
+      <c r="M31" s="14"/>
+      <c r="N31" s="14"/>
+      <c r="O31" s="14"/>
+      <c r="P31" s="14"/>
+      <c r="Q31" s="14"/>
+      <c r="R31" s="14"/>
+      <c r="S31" s="14"/>
+    </row>
+    <row r="32" spans="1:19" s="12" customFormat="1" ht="18" x14ac:dyDescent="0.3">
+      <c r="A32" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="C30" s="14"/>
-      <c r="D30" s="14"/>
-      <c r="E30" s="14"/>
-      <c r="F30" s="14"/>
-      <c r="G30" s="14"/>
-      <c r="H30" s="14"/>
-      <c r="I30" s="14"/>
-      <c r="J30" s="14"/>
-      <c r="K30" s="14"/>
-      <c r="L30" s="14"/>
-      <c r="M30" s="14"/>
-      <c r="N30" s="14"/>
-      <c r="O30" s="14"/>
-      <c r="P30" s="14"/>
-      <c r="Q30" s="14"/>
-      <c r="R30" s="14"/>
-      <c r="S30" s="14"/>
-    </row>
-    <row r="31" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="B31" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C31" s="8">
-        <v>15</v>
-      </c>
-      <c r="D31" s="8">
-        <v>15</v>
-      </c>
-      <c r="E31" s="8"/>
-      <c r="F31" s="8"/>
-      <c r="G31" s="8"/>
-      <c r="H31" s="8"/>
-      <c r="I31" s="8"/>
-      <c r="J31" s="8"/>
-      <c r="K31" s="8"/>
-      <c r="L31" s="8"/>
-      <c r="M31" s="8"/>
-      <c r="N31" s="8"/>
-      <c r="O31" s="8"/>
-      <c r="P31" s="8"/>
-      <c r="Q31" s="8"/>
-      <c r="R31" s="8"/>
-      <c r="S31" s="8"/>
-    </row>
-    <row r="32" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="B32" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C32" s="8">
-        <v>15</v>
-      </c>
-      <c r="D32" s="8">
-        <v>5</v>
-      </c>
-      <c r="E32" s="8"/>
-      <c r="F32" s="8"/>
-      <c r="G32" s="8"/>
-      <c r="H32" s="8"/>
-      <c r="I32" s="8"/>
-      <c r="J32" s="8"/>
-      <c r="K32" s="8"/>
-      <c r="L32" s="8"/>
-      <c r="M32" s="8"/>
-      <c r="N32" s="8"/>
-      <c r="O32" s="8"/>
-      <c r="P32" s="8"/>
-      <c r="Q32" s="8"/>
-      <c r="R32" s="8"/>
-      <c r="S32" s="8"/>
+      <c r="C32" s="14"/>
+      <c r="D32" s="14"/>
+      <c r="E32" s="14"/>
+      <c r="F32" s="14"/>
+      <c r="G32" s="14"/>
+      <c r="H32" s="14"/>
+      <c r="I32" s="14"/>
+      <c r="J32" s="14"/>
+      <c r="K32" s="14"/>
+      <c r="L32" s="14"/>
+      <c r="M32" s="14"/>
+      <c r="N32" s="14"/>
+      <c r="O32" s="14"/>
+      <c r="P32" s="14"/>
+      <c r="Q32" s="14"/>
+      <c r="R32" s="14"/>
+      <c r="S32" s="14"/>
     </row>
     <row r="33" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A33" s="8" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B33" s="3" t="s">
         <v>13</v>
       </c>
       <c r="C33" s="8">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="D33" s="8">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="E33" s="8"/>
       <c r="F33" s="8"/>
@@ -1648,47 +1716,47 @@
       <c r="R35" s="8"/>
       <c r="S35" s="8"/>
     </row>
-    <row r="36" spans="1:19" s="4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="10" t="s">
-        <v>25</v>
+    <row r="36" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="8" t="s">
+        <v>45</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C36" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="D36" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="E36" s="10"/>
-      <c r="F36" s="10"/>
-      <c r="G36" s="10"/>
-      <c r="H36" s="10"/>
-      <c r="I36" s="10"/>
-      <c r="J36" s="10"/>
-      <c r="K36" s="10"/>
-      <c r="L36" s="10"/>
-      <c r="M36" s="10"/>
-      <c r="N36" s="10"/>
-      <c r="O36" s="10"/>
-      <c r="P36" s="10"/>
-      <c r="Q36" s="10"/>
-      <c r="R36" s="10"/>
-      <c r="S36" s="10"/>
+        <v>13</v>
+      </c>
+      <c r="C36" s="8">
+        <v>15</v>
+      </c>
+      <c r="D36" s="8">
+        <v>5</v>
+      </c>
+      <c r="E36" s="8"/>
+      <c r="F36" s="8"/>
+      <c r="G36" s="8"/>
+      <c r="H36" s="8"/>
+      <c r="I36" s="8"/>
+      <c r="J36" s="8"/>
+      <c r="K36" s="8"/>
+      <c r="L36" s="8"/>
+      <c r="M36" s="8"/>
+      <c r="N36" s="8"/>
+      <c r="O36" s="8"/>
+      <c r="P36" s="8"/>
+      <c r="Q36" s="8"/>
+      <c r="R36" s="8"/>
+      <c r="S36" s="8"/>
     </row>
     <row r="37" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="B37" s="4" t="s">
+      <c r="A37" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="B37" s="3" t="s">
         <v>13</v>
       </c>
       <c r="C37" s="8">
-        <v>0.75</v>
+        <v>2</v>
       </c>
       <c r="D37" s="8">
-        <v>0.75</v>
+        <v>5</v>
       </c>
       <c r="E37" s="8"/>
       <c r="F37" s="8"/>
@@ -1706,47 +1774,47 @@
       <c r="R37" s="8"/>
       <c r="S37" s="8"/>
     </row>
-    <row r="38" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="8" t="s">
-        <v>36</v>
+    <row r="38" spans="1:19" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="10" t="s">
+        <v>23</v>
       </c>
       <c r="B38" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C38" s="8" t="b">
-        <v>1</v>
-      </c>
-      <c r="D38" s="8" t="b">
-        <v>1</v>
-      </c>
-      <c r="E38" s="8"/>
-      <c r="F38" s="8"/>
-      <c r="G38" s="8"/>
-      <c r="H38" s="8"/>
-      <c r="I38" s="8"/>
-      <c r="J38" s="8"/>
-      <c r="K38" s="8"/>
-      <c r="L38" s="8"/>
-      <c r="M38" s="8"/>
-      <c r="N38" s="8"/>
-      <c r="O38" s="8"/>
-      <c r="P38" s="8"/>
-      <c r="Q38" s="8"/>
-      <c r="R38" s="8"/>
-      <c r="S38" s="8"/>
+      <c r="C38" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="D38" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="E38" s="10"/>
+      <c r="F38" s="10"/>
+      <c r="G38" s="10"/>
+      <c r="H38" s="10"/>
+      <c r="I38" s="10"/>
+      <c r="J38" s="10"/>
+      <c r="K38" s="10"/>
+      <c r="L38" s="10"/>
+      <c r="M38" s="10"/>
+      <c r="N38" s="10"/>
+      <c r="O38" s="10"/>
+      <c r="P38" s="10"/>
+      <c r="Q38" s="10"/>
+      <c r="R38" s="10"/>
+      <c r="S38" s="10"/>
     </row>
     <row r="39" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="8" t="s">
-        <v>59</v>
-      </c>
-      <c r="B39" s="3" t="s">
+      <c r="A39" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="B39" s="4" t="s">
         <v>13</v>
       </c>
       <c r="C39" s="8">
-        <v>-0.5</v>
+        <v>0.75</v>
       </c>
       <c r="D39" s="8">
-        <v>-0.5</v>
+        <v>0.75</v>
       </c>
       <c r="E39" s="8"/>
       <c r="F39" s="8"/>
@@ -1765,10 +1833,18 @@
       <c r="S39" s="8"/>
     </row>
     <row r="40" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="8"/>
-      <c r="B40" s="3"/>
-      <c r="C40" s="8"/>
-      <c r="D40" s="8"/>
+      <c r="A40" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="B40" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C40" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="D40" s="8" t="b">
+        <v>1</v>
+      </c>
       <c r="E40" s="8"/>
       <c r="F40" s="8"/>
       <c r="G40" s="8"/>
@@ -1785,111 +1861,111 @@
       <c r="R40" s="8"/>
       <c r="S40" s="8"/>
     </row>
-    <row r="41" spans="1:19" s="16" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="15"/>
-      <c r="C41" s="15"/>
-      <c r="D41" s="15"/>
-      <c r="E41" s="14"/>
-      <c r="F41" s="14"/>
-      <c r="G41" s="14"/>
-      <c r="H41" s="14"/>
-      <c r="I41" s="14"/>
-      <c r="J41" s="14"/>
-      <c r="K41" s="14"/>
-      <c r="L41" s="14"/>
-      <c r="M41" s="14"/>
-      <c r="N41" s="14"/>
-      <c r="O41" s="14"/>
-      <c r="P41" s="14"/>
-      <c r="Q41" s="14"/>
-      <c r="R41" s="14"/>
-      <c r="S41" s="14"/>
-    </row>
-    <row r="42" spans="1:19" s="12" customFormat="1" ht="18" x14ac:dyDescent="0.3">
-      <c r="A42" s="20" t="s">
+    <row r="41" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="B41" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C41" s="8">
+        <v>-0.5</v>
+      </c>
+      <c r="D41" s="8">
+        <v>-0.5</v>
+      </c>
+      <c r="E41" s="8"/>
+      <c r="F41" s="8"/>
+      <c r="G41" s="8"/>
+      <c r="H41" s="8"/>
+      <c r="I41" s="8"/>
+      <c r="J41" s="8"/>
+      <c r="K41" s="8"/>
+      <c r="L41" s="8"/>
+      <c r="M41" s="8"/>
+      <c r="N41" s="8"/>
+      <c r="O41" s="8"/>
+      <c r="P41" s="8"/>
+      <c r="Q41" s="8"/>
+      <c r="R41" s="8"/>
+      <c r="S41" s="8"/>
+    </row>
+    <row r="42" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="8"/>
+      <c r="B42" s="3"/>
+      <c r="C42" s="8"/>
+      <c r="D42" s="8"/>
+      <c r="E42" s="8"/>
+      <c r="F42" s="8"/>
+      <c r="G42" s="8"/>
+      <c r="H42" s="8"/>
+      <c r="I42" s="8"/>
+      <c r="J42" s="8"/>
+      <c r="K42" s="8"/>
+      <c r="L42" s="8"/>
+      <c r="M42" s="8"/>
+      <c r="N42" s="8"/>
+      <c r="O42" s="8"/>
+      <c r="P42" s="8"/>
+      <c r="Q42" s="8"/>
+      <c r="R42" s="8"/>
+      <c r="S42" s="8"/>
+    </row>
+    <row r="43" spans="1:19" s="16" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="15"/>
+      <c r="C43" s="15"/>
+      <c r="D43" s="15"/>
+      <c r="E43" s="14"/>
+      <c r="F43" s="14"/>
+      <c r="G43" s="14"/>
+      <c r="H43" s="14"/>
+      <c r="I43" s="14"/>
+      <c r="J43" s="14"/>
+      <c r="K43" s="14"/>
+      <c r="L43" s="14"/>
+      <c r="M43" s="14"/>
+      <c r="N43" s="14"/>
+      <c r="O43" s="14"/>
+      <c r="P43" s="14"/>
+      <c r="Q43" s="14"/>
+      <c r="R43" s="14"/>
+      <c r="S43" s="14"/>
+    </row>
+    <row r="44" spans="1:19" s="12" customFormat="1" ht="18" x14ac:dyDescent="0.3">
+      <c r="A44" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="C42" s="14"/>
-      <c r="D42" s="14"/>
-      <c r="E42" s="14"/>
-      <c r="F42" s="14"/>
-      <c r="G42" s="14"/>
-      <c r="H42" s="14"/>
-      <c r="I42" s="14"/>
-      <c r="J42" s="14"/>
-      <c r="K42" s="14"/>
-      <c r="L42" s="14"/>
-      <c r="M42" s="14"/>
-      <c r="N42" s="14"/>
-      <c r="O42" s="14"/>
-      <c r="P42" s="14"/>
-      <c r="Q42" s="14"/>
-      <c r="R42" s="14"/>
-      <c r="S42" s="14"/>
-    </row>
-    <row r="43" spans="1:19" s="2" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A43" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="B43" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="C43" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="D43" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="E43" s="8"/>
-      <c r="F43" s="8"/>
-      <c r="G43" s="8"/>
-      <c r="H43" s="8"/>
-      <c r="I43" s="8"/>
-      <c r="J43" s="8"/>
-      <c r="K43" s="8"/>
-      <c r="L43" s="8"/>
-      <c r="M43" s="8"/>
-      <c r="N43" s="8"/>
-      <c r="O43" s="8"/>
-      <c r="P43" s="8"/>
-      <c r="Q43" s="8"/>
-      <c r="R43" s="8"/>
-      <c r="S43" s="8"/>
-    </row>
-    <row r="44" spans="1:19" s="2" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A44" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="B44" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="C44" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="D44" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="E44" s="8"/>
-      <c r="F44" s="8"/>
-      <c r="G44" s="8"/>
-      <c r="H44" s="8"/>
-      <c r="I44" s="8"/>
-      <c r="J44" s="8"/>
-      <c r="K44" s="8"/>
-      <c r="L44" s="8"/>
-      <c r="M44" s="8"/>
-      <c r="N44" s="8"/>
-      <c r="O44" s="8"/>
-      <c r="P44" s="8"/>
-      <c r="Q44" s="8"/>
-      <c r="R44" s="8"/>
-      <c r="S44" s="8"/>
+      <c r="C44" s="14"/>
+      <c r="D44" s="14"/>
+      <c r="E44" s="14"/>
+      <c r="F44" s="14"/>
+      <c r="G44" s="14"/>
+      <c r="H44" s="14"/>
+      <c r="I44" s="14"/>
+      <c r="J44" s="14"/>
+      <c r="K44" s="14"/>
+      <c r="L44" s="14"/>
+      <c r="M44" s="14"/>
+      <c r="N44" s="14"/>
+      <c r="O44" s="14"/>
+      <c r="P44" s="14"/>
+      <c r="Q44" s="14"/>
+      <c r="R44" s="14"/>
+      <c r="S44" s="14"/>
     </row>
     <row r="45" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="8"/>
-      <c r="B45" s="3"/>
-      <c r="C45" s="8"/>
-      <c r="D45" s="8"/>
+      <c r="A45" s="26" t="s">
+        <v>64</v>
+      </c>
+      <c r="B45" s="24" t="s">
+        <v>3</v>
+      </c>
+      <c r="C45" s="25" t="s">
+        <v>65</v>
+      </c>
+      <c r="D45" s="25" t="s">
+        <v>65</v>
+      </c>
       <c r="E45" s="8"/>
       <c r="F45" s="8"/>
       <c r="G45" s="8"/>
@@ -1906,6 +1982,180 @@
       <c r="R45" s="8"/>
       <c r="S45" s="8"/>
     </row>
+    <row r="46" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="26" t="s">
+        <v>66</v>
+      </c>
+      <c r="B46" s="24" t="s">
+        <v>3</v>
+      </c>
+      <c r="C46" s="25" t="s">
+        <v>67</v>
+      </c>
+      <c r="D46" s="25" t="s">
+        <v>67</v>
+      </c>
+      <c r="E46" s="8"/>
+      <c r="F46" s="8"/>
+      <c r="G46" s="8"/>
+      <c r="H46" s="8"/>
+      <c r="I46" s="8"/>
+      <c r="J46" s="8"/>
+      <c r="K46" s="8"/>
+      <c r="L46" s="8"/>
+      <c r="M46" s="8"/>
+      <c r="N46" s="8"/>
+      <c r="O46" s="8"/>
+      <c r="P46" s="8"/>
+      <c r="Q46" s="8"/>
+      <c r="R46" s="8"/>
+      <c r="S46" s="8"/>
+    </row>
+    <row r="47" spans="1:19" s="21" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="26" t="s">
+        <v>68</v>
+      </c>
+      <c r="B47" s="24" t="s">
+        <v>3</v>
+      </c>
+      <c r="C47" s="25" t="s">
+        <v>69</v>
+      </c>
+      <c r="D47" s="25" t="s">
+        <v>69</v>
+      </c>
+      <c r="E47" s="22"/>
+      <c r="F47" s="22"/>
+      <c r="G47" s="22"/>
+      <c r="H47" s="22"/>
+      <c r="I47" s="22"/>
+      <c r="J47" s="22"/>
+      <c r="K47" s="22"/>
+      <c r="L47" s="22"/>
+      <c r="M47" s="22"/>
+      <c r="N47" s="22"/>
+      <c r="O47" s="22"/>
+      <c r="P47" s="22"/>
+      <c r="Q47" s="22"/>
+      <c r="R47" s="22"/>
+      <c r="S47" s="22"/>
+    </row>
+    <row r="48" spans="1:19" s="21" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="26" t="s">
+        <v>70</v>
+      </c>
+      <c r="B48" s="24" t="s">
+        <v>3</v>
+      </c>
+      <c r="C48" s="25" t="s">
+        <v>71</v>
+      </c>
+      <c r="D48" s="25" t="s">
+        <v>71</v>
+      </c>
+      <c r="E48" s="22"/>
+      <c r="F48" s="22"/>
+      <c r="G48" s="22"/>
+      <c r="H48" s="22"/>
+      <c r="I48" s="22"/>
+      <c r="J48" s="22"/>
+      <c r="K48" s="22"/>
+      <c r="L48" s="22"/>
+      <c r="M48" s="22"/>
+      <c r="N48" s="22"/>
+      <c r="O48" s="22"/>
+      <c r="P48" s="22"/>
+      <c r="Q48" s="22"/>
+      <c r="R48" s="22"/>
+      <c r="S48" s="22"/>
+    </row>
+    <row r="49" spans="1:19" s="21" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="26" t="s">
+        <v>72</v>
+      </c>
+      <c r="B49" s="24" t="s">
+        <v>3</v>
+      </c>
+      <c r="C49" s="25" t="s">
+        <v>73</v>
+      </c>
+      <c r="D49" s="25" t="s">
+        <v>73</v>
+      </c>
+      <c r="E49" s="22"/>
+      <c r="F49" s="22"/>
+      <c r="G49" s="22"/>
+      <c r="H49" s="22"/>
+      <c r="I49" s="22"/>
+      <c r="J49" s="22"/>
+      <c r="K49" s="22"/>
+      <c r="L49" s="22"/>
+      <c r="M49" s="22"/>
+      <c r="N49" s="22"/>
+      <c r="O49" s="22"/>
+      <c r="P49" s="22"/>
+      <c r="Q49" s="22"/>
+      <c r="R49" s="22"/>
+      <c r="S49" s="22"/>
+    </row>
+    <row r="50" spans="1:19" s="21" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A50" s="29" t="s">
+        <v>74</v>
+      </c>
+      <c r="B50" s="27" t="s">
+        <v>3</v>
+      </c>
+      <c r="C50" s="28" t="s">
+        <v>75</v>
+      </c>
+      <c r="D50" s="28" t="s">
+        <v>75</v>
+      </c>
+      <c r="E50" s="22"/>
+      <c r="F50" s="22"/>
+      <c r="G50" s="22"/>
+      <c r="H50" s="22"/>
+      <c r="I50" s="22"/>
+      <c r="J50" s="22"/>
+      <c r="K50" s="22"/>
+      <c r="L50" s="22"/>
+      <c r="M50" s="22"/>
+      <c r="N50" s="22"/>
+      <c r="O50" s="22"/>
+      <c r="P50" s="22"/>
+      <c r="Q50" s="22"/>
+      <c r="R50" s="22"/>
+      <c r="S50" s="22"/>
+    </row>
+    <row r="51" spans="1:19" s="21" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A51" s="28" t="s">
+        <v>76</v>
+      </c>
+      <c r="B51" s="27" t="s">
+        <v>3</v>
+      </c>
+      <c r="C51" s="28" t="s">
+        <v>77</v>
+      </c>
+      <c r="D51" s="28" t="s">
+        <v>77</v>
+      </c>
+      <c r="E51" s="22"/>
+      <c r="F51" s="22"/>
+      <c r="G51" s="22"/>
+      <c r="H51" s="22"/>
+      <c r="I51" s="22"/>
+      <c r="J51" s="22"/>
+      <c r="K51" s="22"/>
+      <c r="L51" s="22"/>
+      <c r="M51" s="22"/>
+      <c r="N51" s="22"/>
+      <c r="O51" s="22"/>
+      <c r="P51" s="22"/>
+      <c r="Q51" s="22"/>
+      <c r="R51" s="22"/>
+      <c r="S51" s="22"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
BATCH FILE FORMAT CHANGE : no more 'First Pass...' and 'Iteration...'
Signed-off-by: kevinanewman <newman.kevin@epa.gov>
</commit_message>
<xml_diff>
--- a/input_samples/multiple_session_batch.xlsx
+++ b/input_samples/multiple_session_batch.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TSHERWOO\Documents\GitHub\EPA_OMEGA_Model\input_samples\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\GitHub\EPA_OMEGA_Model\input_samples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{679DC5D9-7A81-49E7-A92B-3A7DFA4C5B16}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99E7EA19-F9C6-4433-B7F8-EAADE84C9399}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="6252" windowWidth="23040" windowHeight="6252" tabRatio="151" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8445" yWindow="2520" windowWidth="16635" windowHeight="13275" tabRatio="151" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sessions" sheetId="5" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="76">
   <si>
     <t>Parameter</t>
   </si>
@@ -173,21 +173,6 @@
     <t>input_samples/manufacturers.csv</t>
   </si>
   <si>
-    <t>Iteration Num Tech Options per ICE Vehicle</t>
-  </si>
-  <si>
-    <t>Iteration Num Tech Options per BEV Vehicle</t>
-  </si>
-  <si>
-    <t>First Pass Num Tech Options per ICE Vehicle</t>
-  </si>
-  <si>
-    <t>First Pass Num Tech Options per BEV Vehicle</t>
-  </si>
-  <si>
-    <t>First Pass Num Market Share Options</t>
-  </si>
-  <si>
     <t>input_samples/context_fuel_prices.csv</t>
   </si>
   <si>
@@ -270,6 +255,15 @@
   </si>
   <si>
     <t>input_samples/context_cpi_price_deflators.csv</t>
+  </si>
+  <si>
+    <t>Num Market Share Options</t>
+  </si>
+  <si>
+    <t>Num Tech Options per ICE Vehicle</t>
+  </si>
+  <si>
+    <t>Num Tech Options per BEV Vehicle</t>
   </si>
 </sst>
 </file>
@@ -789,26 +783,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AG51"/>
+  <dimension ref="A1:AG49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="10" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D50" sqref="D50:D51"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane ySplit="10" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="42" style="11" customWidth="1"/>
-    <col min="2" max="2" width="17.33203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="17.28515625" style="1" customWidth="1"/>
     <col min="3" max="4" width="48" style="11" bestFit="1" customWidth="1"/>
-    <col min="5" max="17" width="21.33203125" style="11" customWidth="1"/>
-    <col min="18" max="18" width="16.6640625" style="1" customWidth="1"/>
+    <col min="5" max="17" width="21.28515625" style="11" customWidth="1"/>
+    <col min="18" max="18" width="16.7109375" style="1" customWidth="1"/>
     <col min="19" max="19" width="18" style="1" customWidth="1"/>
-    <col min="20" max="20" width="16.44140625" style="1" customWidth="1"/>
-    <col min="21" max="16384" width="8.6640625" style="1"/>
+    <col min="20" max="20" width="16.42578125" style="1" customWidth="1"/>
+    <col min="21" max="16384" width="8.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" s="18" customFormat="1" ht="21" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:33" s="18" customFormat="1" ht="21" x14ac:dyDescent="0.25">
       <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
@@ -849,7 +843,7 @@
       <c r="AF1" s="17"/>
       <c r="AG1" s="17"/>
     </row>
-    <row r="2" spans="1:33" s="12" customFormat="1" ht="18" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:33" s="12" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A2" s="19" t="s">
         <v>10</v>
       </c>
@@ -869,7 +863,7 @@
       <c r="P2" s="14"/>
       <c r="Q2" s="14"/>
     </row>
-    <row r="3" spans="1:33" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:33" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>4</v>
       </c>
@@ -894,7 +888,7 @@
       <c r="P3" s="14"/>
       <c r="Q3" s="14"/>
     </row>
-    <row r="4" spans="1:33" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:33" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>31</v>
       </c>
@@ -917,7 +911,7 @@
       <c r="P4" s="14"/>
       <c r="Q4" s="14"/>
     </row>
-    <row r="5" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>30</v>
       </c>
@@ -925,21 +919,21 @@
         <v>3</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="6" spans="1:33" x14ac:dyDescent="0.3">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="6" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="B6" s="6" t="s">
         <v>3</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="7" spans="1:33" s="12" customFormat="1" x14ac:dyDescent="0.3">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="7" spans="1:33" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="14"/>
       <c r="C7" s="14"/>
       <c r="D7" s="14"/>
@@ -957,7 +951,7 @@
       <c r="P7" s="14"/>
       <c r="Q7" s="14"/>
     </row>
-    <row r="8" spans="1:33" s="12" customFormat="1" ht="18" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:33" s="12" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A8" s="20" t="s">
         <v>9</v>
       </c>
@@ -977,7 +971,7 @@
       <c r="P8" s="14"/>
       <c r="Q8" s="14"/>
     </row>
-    <row r="9" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
         <v>5</v>
       </c>
@@ -1006,7 +1000,7 @@
       <c r="R9" s="8"/>
       <c r="S9" s="8"/>
     </row>
-    <row r="10" spans="1:33" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:33" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
         <v>2</v>
       </c>
@@ -1035,7 +1029,7 @@
       <c r="R10" s="9"/>
       <c r="S10" s="9"/>
     </row>
-    <row r="11" spans="1:33" s="16" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:33" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="15"/>
       <c r="C11" s="15"/>
       <c r="D11" s="15"/>
@@ -1055,7 +1049,7 @@
       <c r="R11" s="14"/>
       <c r="S11" s="14"/>
     </row>
-    <row r="12" spans="1:33" s="12" customFormat="1" ht="18" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:33" s="12" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A12" s="13" t="s">
         <v>6</v>
       </c>
@@ -1077,7 +1071,7 @@
       <c r="R12" s="14"/>
       <c r="S12" s="14"/>
     </row>
-    <row r="13" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
         <v>14</v>
       </c>
@@ -1106,7 +1100,7 @@
       <c r="R13" s="8"/>
       <c r="S13" s="8"/>
     </row>
-    <row r="14" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="8" t="s">
         <v>16</v>
       </c>
@@ -1135,7 +1129,7 @@
       <c r="R14" s="8"/>
       <c r="S14" s="8"/>
     </row>
-    <row r="15" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="8" t="s">
         <v>17</v>
       </c>
@@ -1164,7 +1158,7 @@
       <c r="R15" s="8"/>
       <c r="S15" s="8"/>
     </row>
-    <row r="16" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="8" t="s">
         <v>27</v>
       </c>
@@ -1193,7 +1187,7 @@
       <c r="R16" s="8"/>
       <c r="S16" s="8"/>
     </row>
-    <row r="17" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="8" t="s">
         <v>19</v>
       </c>
@@ -1222,18 +1216,18 @@
       <c r="R17" s="8"/>
       <c r="S17" s="8"/>
     </row>
-    <row r="18" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="8" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>3</v>
       </c>
       <c r="C18" s="8" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="D18" s="8" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="E18" s="8"/>
       <c r="F18" s="8"/>
@@ -1251,18 +1245,18 @@
       <c r="R18" s="8"/>
       <c r="S18" s="8"/>
     </row>
-    <row r="19" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="8" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>3</v>
       </c>
       <c r="C19" s="8" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="D19" s="8" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="E19" s="8"/>
       <c r="F19" s="8"/>
@@ -1280,18 +1274,18 @@
       <c r="R19" s="8"/>
       <c r="S19" s="8"/>
     </row>
-    <row r="20" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="8" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>3</v>
       </c>
       <c r="C20" s="8" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="D20" s="8" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="E20" s="8"/>
       <c r="F20" s="8"/>
@@ -1309,7 +1303,7 @@
       <c r="R20" s="8"/>
       <c r="S20" s="8"/>
     </row>
-    <row r="21" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="8" t="s">
         <v>18</v>
       </c>
@@ -1317,10 +1311,10 @@
         <v>3</v>
       </c>
       <c r="C21" s="8" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="D21" s="8" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="E21" s="8"/>
       <c r="F21" s="8"/>
@@ -1338,7 +1332,7 @@
       <c r="R21" s="8"/>
       <c r="S21" s="8"/>
     </row>
-    <row r="22" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="8" t="s">
         <v>20</v>
       </c>
@@ -1367,7 +1361,7 @@
       <c r="R22" s="8"/>
       <c r="S22" s="8"/>
     </row>
-    <row r="23" spans="1:19" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:19" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="10" t="s">
         <v>21</v>
       </c>
@@ -1396,7 +1390,7 @@
       <c r="R23" s="10"/>
       <c r="S23" s="10"/>
     </row>
-    <row r="24" spans="1:19" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:19" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="8" t="s">
         <v>32</v>
       </c>
@@ -1425,7 +1419,7 @@
       <c r="R24" s="10"/>
       <c r="S24" s="10"/>
     </row>
-    <row r="25" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="8" t="s">
         <v>33</v>
       </c>
@@ -1454,18 +1448,18 @@
       <c r="R25" s="8"/>
       <c r="S25" s="8"/>
     </row>
-    <row r="26" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="23" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="B26" s="21" t="s">
         <v>3</v>
       </c>
       <c r="C26" s="22" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="D26" s="22" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="E26" s="8"/>
       <c r="F26" s="8"/>
@@ -1483,18 +1477,18 @@
       <c r="R26" s="8"/>
       <c r="S26" s="8"/>
     </row>
-    <row r="27" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="23" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="B27" s="21" t="s">
         <v>3</v>
       </c>
       <c r="C27" s="22" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="D27" s="22" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="E27" s="8"/>
       <c r="F27" s="8"/>
@@ -1512,7 +1506,7 @@
       <c r="R27" s="8"/>
       <c r="S27" s="8"/>
     </row>
-    <row r="28" spans="1:19" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:19" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="10" t="s">
         <v>15</v>
       </c>
@@ -1541,7 +1535,7 @@
       <c r="R28" s="10"/>
       <c r="S28" s="10"/>
     </row>
-    <row r="29" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="10" t="s">
         <v>22</v>
       </c>
@@ -1570,7 +1564,7 @@
       <c r="R29" s="8"/>
       <c r="S29" s="8"/>
     </row>
-    <row r="30" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E30" s="8"/>
       <c r="F30" s="8"/>
       <c r="G30" s="8"/>
@@ -1587,7 +1581,7 @@
       <c r="R30" s="8"/>
       <c r="S30" s="8"/>
     </row>
-    <row r="31" spans="1:19" s="16" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:19" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="15"/>
       <c r="C31" s="15"/>
       <c r="D31" s="15"/>
@@ -1607,7 +1601,7 @@
       <c r="R31" s="14"/>
       <c r="S31" s="14"/>
     </row>
-    <row r="32" spans="1:19" s="12" customFormat="1" ht="18" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:19" s="12" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A32" s="20" t="s">
         <v>8</v>
       </c>
@@ -1629,18 +1623,18 @@
       <c r="R32" s="14"/>
       <c r="S32" s="14"/>
     </row>
-    <row r="33" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="8" t="s">
-        <v>49</v>
+        <v>73</v>
       </c>
       <c r="B33" s="3" t="s">
         <v>13</v>
       </c>
       <c r="C33" s="8">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="D33" s="8">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="E33" s="8"/>
       <c r="F33" s="8"/>
@@ -1658,18 +1652,18 @@
       <c r="R33" s="8"/>
       <c r="S33" s="8"/>
     </row>
-    <row r="34" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="8" t="s">
-        <v>47</v>
+        <v>74</v>
       </c>
       <c r="B34" s="3" t="s">
         <v>13</v>
       </c>
       <c r="C34" s="8">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="D34" s="8">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E34" s="8"/>
       <c r="F34" s="8"/>
@@ -1687,18 +1681,18 @@
       <c r="R34" s="8"/>
       <c r="S34" s="8"/>
     </row>
-    <row r="35" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="8" t="s">
-        <v>48</v>
+        <v>75</v>
       </c>
       <c r="B35" s="3" t="s">
         <v>13</v>
       </c>
       <c r="C35" s="8">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D35" s="8">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E35" s="8"/>
       <c r="F35" s="8"/>
@@ -1716,47 +1710,47 @@
       <c r="R35" s="8"/>
       <c r="S35" s="8"/>
     </row>
-    <row r="36" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="8" t="s">
-        <v>45</v>
+    <row r="36" spans="1:19" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="10" t="s">
+        <v>23</v>
       </c>
       <c r="B36" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C36" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="D36" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="E36" s="10"/>
+      <c r="F36" s="10"/>
+      <c r="G36" s="10"/>
+      <c r="H36" s="10"/>
+      <c r="I36" s="10"/>
+      <c r="J36" s="10"/>
+      <c r="K36" s="10"/>
+      <c r="L36" s="10"/>
+      <c r="M36" s="10"/>
+      <c r="N36" s="10"/>
+      <c r="O36" s="10"/>
+      <c r="P36" s="10"/>
+      <c r="Q36" s="10"/>
+      <c r="R36" s="10"/>
+      <c r="S36" s="10"/>
+    </row>
+    <row r="37" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="B37" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C36" s="8">
-        <v>15</v>
-      </c>
-      <c r="D36" s="8">
-        <v>5</v>
-      </c>
-      <c r="E36" s="8"/>
-      <c r="F36" s="8"/>
-      <c r="G36" s="8"/>
-      <c r="H36" s="8"/>
-      <c r="I36" s="8"/>
-      <c r="J36" s="8"/>
-      <c r="K36" s="8"/>
-      <c r="L36" s="8"/>
-      <c r="M36" s="8"/>
-      <c r="N36" s="8"/>
-      <c r="O36" s="8"/>
-      <c r="P36" s="8"/>
-      <c r="Q36" s="8"/>
-      <c r="R36" s="8"/>
-      <c r="S36" s="8"/>
-    </row>
-    <row r="37" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="B37" s="3" t="s">
-        <v>13</v>
-      </c>
       <c r="C37" s="8">
-        <v>2</v>
+        <v>0.75</v>
       </c>
       <c r="D37" s="8">
-        <v>5</v>
+        <v>0.75</v>
       </c>
       <c r="E37" s="8"/>
       <c r="F37" s="8"/>
@@ -1774,47 +1768,47 @@
       <c r="R37" s="8"/>
       <c r="S37" s="8"/>
     </row>
-    <row r="38" spans="1:19" s="4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="10" t="s">
-        <v>23</v>
+    <row r="38" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="8" t="s">
+        <v>34</v>
       </c>
       <c r="B38" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C38" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="D38" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="E38" s="10"/>
-      <c r="F38" s="10"/>
-      <c r="G38" s="10"/>
-      <c r="H38" s="10"/>
-      <c r="I38" s="10"/>
-      <c r="J38" s="10"/>
-      <c r="K38" s="10"/>
-      <c r="L38" s="10"/>
-      <c r="M38" s="10"/>
-      <c r="N38" s="10"/>
-      <c r="O38" s="10"/>
-      <c r="P38" s="10"/>
-      <c r="Q38" s="10"/>
-      <c r="R38" s="10"/>
-      <c r="S38" s="10"/>
-    </row>
-    <row r="39" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="B39" s="4" t="s">
+      <c r="C38" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="D38" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="E38" s="8"/>
+      <c r="F38" s="8"/>
+      <c r="G38" s="8"/>
+      <c r="H38" s="8"/>
+      <c r="I38" s="8"/>
+      <c r="J38" s="8"/>
+      <c r="K38" s="8"/>
+      <c r="L38" s="8"/>
+      <c r="M38" s="8"/>
+      <c r="N38" s="8"/>
+      <c r="O38" s="8"/>
+      <c r="P38" s="8"/>
+      <c r="Q38" s="8"/>
+      <c r="R38" s="8"/>
+      <c r="S38" s="8"/>
+    </row>
+    <row r="39" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="B39" s="3" t="s">
         <v>13</v>
       </c>
       <c r="C39" s="8">
-        <v>0.75</v>
+        <v>-0.5</v>
       </c>
       <c r="D39" s="8">
-        <v>0.75</v>
+        <v>-0.5</v>
       </c>
       <c r="E39" s="8"/>
       <c r="F39" s="8"/>
@@ -1832,19 +1826,11 @@
       <c r="R39" s="8"/>
       <c r="S39" s="8"/>
     </row>
-    <row r="40" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="B40" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C40" s="8" t="b">
-        <v>1</v>
-      </c>
-      <c r="D40" s="8" t="b">
-        <v>1</v>
-      </c>
+    <row r="40" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="8"/>
+      <c r="B40" s="3"/>
+      <c r="C40" s="8"/>
+      <c r="D40" s="8"/>
       <c r="E40" s="8"/>
       <c r="F40" s="8"/>
       <c r="G40" s="8"/>
@@ -1861,168 +1847,176 @@
       <c r="R40" s="8"/>
       <c r="S40" s="8"/>
     </row>
-    <row r="41" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="8" t="s">
-        <v>57</v>
-      </c>
-      <c r="B41" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C41" s="8">
-        <v>-0.5</v>
-      </c>
-      <c r="D41" s="8">
-        <v>-0.5</v>
-      </c>
-      <c r="E41" s="8"/>
-      <c r="F41" s="8"/>
-      <c r="G41" s="8"/>
-      <c r="H41" s="8"/>
-      <c r="I41" s="8"/>
-      <c r="J41" s="8"/>
-      <c r="K41" s="8"/>
-      <c r="L41" s="8"/>
-      <c r="M41" s="8"/>
-      <c r="N41" s="8"/>
-      <c r="O41" s="8"/>
-      <c r="P41" s="8"/>
-      <c r="Q41" s="8"/>
-      <c r="R41" s="8"/>
-      <c r="S41" s="8"/>
-    </row>
-    <row r="42" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="8"/>
-      <c r="B42" s="3"/>
-      <c r="C42" s="8"/>
-      <c r="D42" s="8"/>
-      <c r="E42" s="8"/>
-      <c r="F42" s="8"/>
-      <c r="G42" s="8"/>
-      <c r="H42" s="8"/>
-      <c r="I42" s="8"/>
-      <c r="J42" s="8"/>
-      <c r="K42" s="8"/>
-      <c r="L42" s="8"/>
-      <c r="M42" s="8"/>
-      <c r="N42" s="8"/>
-      <c r="O42" s="8"/>
-      <c r="P42" s="8"/>
-      <c r="Q42" s="8"/>
-      <c r="R42" s="8"/>
-      <c r="S42" s="8"/>
-    </row>
-    <row r="43" spans="1:19" s="16" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="15"/>
-      <c r="C43" s="15"/>
-      <c r="D43" s="15"/>
-      <c r="E43" s="14"/>
-      <c r="F43" s="14"/>
-      <c r="G43" s="14"/>
-      <c r="H43" s="14"/>
-      <c r="I43" s="14"/>
-      <c r="J43" s="14"/>
-      <c r="K43" s="14"/>
-      <c r="L43" s="14"/>
-      <c r="M43" s="14"/>
-      <c r="N43" s="14"/>
-      <c r="O43" s="14"/>
-      <c r="P43" s="14"/>
-      <c r="Q43" s="14"/>
-      <c r="R43" s="14"/>
-      <c r="S43" s="14"/>
-    </row>
-    <row r="44" spans="1:19" s="12" customFormat="1" ht="18" x14ac:dyDescent="0.3">
-      <c r="A44" s="20" t="s">
+    <row r="41" spans="1:19" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="15"/>
+      <c r="C41" s="15"/>
+      <c r="D41" s="15"/>
+      <c r="E41" s="14"/>
+      <c r="F41" s="14"/>
+      <c r="G41" s="14"/>
+      <c r="H41" s="14"/>
+      <c r="I41" s="14"/>
+      <c r="J41" s="14"/>
+      <c r="K41" s="14"/>
+      <c r="L41" s="14"/>
+      <c r="M41" s="14"/>
+      <c r="N41" s="14"/>
+      <c r="O41" s="14"/>
+      <c r="P41" s="14"/>
+      <c r="Q41" s="14"/>
+      <c r="R41" s="14"/>
+      <c r="S41" s="14"/>
+    </row>
+    <row r="42" spans="1:19" s="12" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A42" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="C44" s="14"/>
-      <c r="D44" s="14"/>
-      <c r="E44" s="14"/>
-      <c r="F44" s="14"/>
-      <c r="G44" s="14"/>
-      <c r="H44" s="14"/>
-      <c r="I44" s="14"/>
-      <c r="J44" s="14"/>
-      <c r="K44" s="14"/>
-      <c r="L44" s="14"/>
-      <c r="M44" s="14"/>
-      <c r="N44" s="14"/>
-      <c r="O44" s="14"/>
-      <c r="P44" s="14"/>
-      <c r="Q44" s="14"/>
-      <c r="R44" s="14"/>
-      <c r="S44" s="14"/>
-    </row>
-    <row r="45" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C42" s="14"/>
+      <c r="D42" s="14"/>
+      <c r="E42" s="14"/>
+      <c r="F42" s="14"/>
+      <c r="G42" s="14"/>
+      <c r="H42" s="14"/>
+      <c r="I42" s="14"/>
+      <c r="J42" s="14"/>
+      <c r="K42" s="14"/>
+      <c r="L42" s="14"/>
+      <c r="M42" s="14"/>
+      <c r="N42" s="14"/>
+      <c r="O42" s="14"/>
+      <c r="P42" s="14"/>
+      <c r="Q42" s="14"/>
+      <c r="R42" s="14"/>
+      <c r="S42" s="14"/>
+    </row>
+    <row r="43" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="26" t="s">
+        <v>59</v>
+      </c>
+      <c r="B43" s="24" t="s">
+        <v>3</v>
+      </c>
+      <c r="C43" s="25" t="s">
+        <v>60</v>
+      </c>
+      <c r="D43" s="25" t="s">
+        <v>60</v>
+      </c>
+      <c r="E43" s="8"/>
+      <c r="F43" s="8"/>
+      <c r="G43" s="8"/>
+      <c r="H43" s="8"/>
+      <c r="I43" s="8"/>
+      <c r="J43" s="8"/>
+      <c r="K43" s="8"/>
+      <c r="L43" s="8"/>
+      <c r="M43" s="8"/>
+      <c r="N43" s="8"/>
+      <c r="O43" s="8"/>
+      <c r="P43" s="8"/>
+      <c r="Q43" s="8"/>
+      <c r="R43" s="8"/>
+      <c r="S43" s="8"/>
+    </row>
+    <row r="44" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="26" t="s">
+        <v>61</v>
+      </c>
+      <c r="B44" s="24" t="s">
+        <v>3</v>
+      </c>
+      <c r="C44" s="25" t="s">
+        <v>62</v>
+      </c>
+      <c r="D44" s="25" t="s">
+        <v>62</v>
+      </c>
+      <c r="E44" s="8"/>
+      <c r="F44" s="8"/>
+      <c r="G44" s="8"/>
+      <c r="H44" s="8"/>
+      <c r="I44" s="8"/>
+      <c r="J44" s="8"/>
+      <c r="K44" s="8"/>
+      <c r="L44" s="8"/>
+      <c r="M44" s="8"/>
+      <c r="N44" s="8"/>
+      <c r="O44" s="8"/>
+      <c r="P44" s="8"/>
+      <c r="Q44" s="8"/>
+      <c r="R44" s="8"/>
+      <c r="S44" s="8"/>
+    </row>
+    <row r="45" spans="1:19" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45" s="26" t="s">
+        <v>63</v>
+      </c>
+      <c r="B45" s="24" t="s">
+        <v>3</v>
+      </c>
+      <c r="C45" s="25" t="s">
         <v>64</v>
       </c>
-      <c r="B45" s="24" t="s">
-        <v>3</v>
-      </c>
-      <c r="C45" s="25" t="s">
+      <c r="D45" s="25" t="s">
+        <v>64</v>
+      </c>
+      <c r="E45" s="22"/>
+      <c r="F45" s="22"/>
+      <c r="G45" s="22"/>
+      <c r="H45" s="22"/>
+      <c r="I45" s="22"/>
+      <c r="J45" s="22"/>
+      <c r="K45" s="22"/>
+      <c r="L45" s="22"/>
+      <c r="M45" s="22"/>
+      <c r="N45" s="22"/>
+      <c r="O45" s="22"/>
+      <c r="P45" s="22"/>
+      <c r="Q45" s="22"/>
+      <c r="R45" s="22"/>
+      <c r="S45" s="22"/>
+    </row>
+    <row r="46" spans="1:19" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="26" t="s">
         <v>65</v>
       </c>
-      <c r="D45" s="25" t="s">
-        <v>65</v>
-      </c>
-      <c r="E45" s="8"/>
-      <c r="F45" s="8"/>
-      <c r="G45" s="8"/>
-      <c r="H45" s="8"/>
-      <c r="I45" s="8"/>
-      <c r="J45" s="8"/>
-      <c r="K45" s="8"/>
-      <c r="L45" s="8"/>
-      <c r="M45" s="8"/>
-      <c r="N45" s="8"/>
-      <c r="O45" s="8"/>
-      <c r="P45" s="8"/>
-      <c r="Q45" s="8"/>
-      <c r="R45" s="8"/>
-      <c r="S45" s="8"/>
-    </row>
-    <row r="46" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="26" t="s">
+      <c r="B46" s="24" t="s">
+        <v>3</v>
+      </c>
+      <c r="C46" s="25" t="s">
         <v>66</v>
       </c>
-      <c r="B46" s="24" t="s">
-        <v>3</v>
-      </c>
-      <c r="C46" s="25" t="s">
+      <c r="D46" s="25" t="s">
+        <v>66</v>
+      </c>
+      <c r="E46" s="22"/>
+      <c r="F46" s="22"/>
+      <c r="G46" s="22"/>
+      <c r="H46" s="22"/>
+      <c r="I46" s="22"/>
+      <c r="J46" s="22"/>
+      <c r="K46" s="22"/>
+      <c r="L46" s="22"/>
+      <c r="M46" s="22"/>
+      <c r="N46" s="22"/>
+      <c r="O46" s="22"/>
+      <c r="P46" s="22"/>
+      <c r="Q46" s="22"/>
+      <c r="R46" s="22"/>
+      <c r="S46" s="22"/>
+    </row>
+    <row r="47" spans="1:19" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="26" t="s">
         <v>67</v>
       </c>
-      <c r="D46" s="25" t="s">
-        <v>67</v>
-      </c>
-      <c r="E46" s="8"/>
-      <c r="F46" s="8"/>
-      <c r="G46" s="8"/>
-      <c r="H46" s="8"/>
-      <c r="I46" s="8"/>
-      <c r="J46" s="8"/>
-      <c r="K46" s="8"/>
-      <c r="L46" s="8"/>
-      <c r="M46" s="8"/>
-      <c r="N46" s="8"/>
-      <c r="O46" s="8"/>
-      <c r="P46" s="8"/>
-      <c r="Q46" s="8"/>
-      <c r="R46" s="8"/>
-      <c r="S46" s="8"/>
-    </row>
-    <row r="47" spans="1:19" s="21" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="26" t="s">
+      <c r="B47" s="24" t="s">
+        <v>3</v>
+      </c>
+      <c r="C47" s="25" t="s">
         <v>68</v>
       </c>
-      <c r="B47" s="24" t="s">
-        <v>3</v>
-      </c>
-      <c r="C47" s="25" t="s">
-        <v>69</v>
-      </c>
       <c r="D47" s="25" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E47" s="22"/>
       <c r="F47" s="22"/>
@@ -2040,18 +2034,18 @@
       <c r="R47" s="22"/>
       <c r="S47" s="22"/>
     </row>
-    <row r="48" spans="1:19" s="21" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="26" t="s">
+    <row r="48" spans="1:19" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="29" t="s">
+        <v>69</v>
+      </c>
+      <c r="B48" s="27" t="s">
+        <v>3</v>
+      </c>
+      <c r="C48" s="28" t="s">
         <v>70</v>
       </c>
-      <c r="B48" s="24" t="s">
-        <v>3</v>
-      </c>
-      <c r="C48" s="25" t="s">
-        <v>71</v>
-      </c>
-      <c r="D48" s="25" t="s">
-        <v>71</v>
+      <c r="D48" s="28" t="s">
+        <v>70</v>
       </c>
       <c r="E48" s="22"/>
       <c r="F48" s="22"/>
@@ -2069,18 +2063,18 @@
       <c r="R48" s="22"/>
       <c r="S48" s="22"/>
     </row>
-    <row r="49" spans="1:19" s="21" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="26" t="s">
+    <row r="49" spans="1:19" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="28" t="s">
+        <v>71</v>
+      </c>
+      <c r="B49" s="27" t="s">
+        <v>3</v>
+      </c>
+      <c r="C49" s="28" t="s">
         <v>72</v>
       </c>
-      <c r="B49" s="24" t="s">
-        <v>3</v>
-      </c>
-      <c r="C49" s="25" t="s">
-        <v>73</v>
-      </c>
-      <c r="D49" s="25" t="s">
-        <v>73</v>
+      <c r="D49" s="28" t="s">
+        <v>72</v>
       </c>
       <c r="E49" s="22"/>
       <c r="F49" s="22"/>
@@ -2098,64 +2092,6 @@
       <c r="R49" s="22"/>
       <c r="S49" s="22"/>
     </row>
-    <row r="50" spans="1:19" s="21" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="29" t="s">
-        <v>74</v>
-      </c>
-      <c r="B50" s="27" t="s">
-        <v>3</v>
-      </c>
-      <c r="C50" s="28" t="s">
-        <v>75</v>
-      </c>
-      <c r="D50" s="28" t="s">
-        <v>75</v>
-      </c>
-      <c r="E50" s="22"/>
-      <c r="F50" s="22"/>
-      <c r="G50" s="22"/>
-      <c r="H50" s="22"/>
-      <c r="I50" s="22"/>
-      <c r="J50" s="22"/>
-      <c r="K50" s="22"/>
-      <c r="L50" s="22"/>
-      <c r="M50" s="22"/>
-      <c r="N50" s="22"/>
-      <c r="O50" s="22"/>
-      <c r="P50" s="22"/>
-      <c r="Q50" s="22"/>
-      <c r="R50" s="22"/>
-      <c r="S50" s="22"/>
-    </row>
-    <row r="51" spans="1:19" s="21" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="28" t="s">
-        <v>76</v>
-      </c>
-      <c r="B51" s="27" t="s">
-        <v>3</v>
-      </c>
-      <c r="C51" s="28" t="s">
-        <v>77</v>
-      </c>
-      <c r="D51" s="28" t="s">
-        <v>77</v>
-      </c>
-      <c r="E51" s="22"/>
-      <c r="F51" s="22"/>
-      <c r="G51" s="22"/>
-      <c r="H51" s="22"/>
-      <c r="I51" s="22"/>
-      <c r="J51" s="22"/>
-      <c r="K51" s="22"/>
-      <c r="L51" s="22"/>
-      <c r="M51" s="22"/>
-      <c r="N51" s="22"/>
-      <c r="O51" s="22"/>
-      <c r="P51" s="22"/>
-      <c r="Q51" s="22"/>
-      <c r="R51" s="22"/>
-      <c r="S51" s="22"/>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
gcam performance improvements console output improvements
Signed-off-by: kevinanewman <newman.kevin@epa.gov>
</commit_message>
<xml_diff>
--- a/input_samples/multiple_session_batch.xlsx
+++ b/input_samples/multiple_session_batch.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\GitHub\EPA_OMEGA_Model\input_samples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99E7EA19-F9C6-4433-B7F8-EAADE84C9399}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{759324E0-4D82-4B30-A2C1-7F007DE3FA33}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8445" yWindow="2520" windowWidth="16635" windowHeight="13275" tabRatio="151" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3810" yWindow="1485" windowWidth="20325" windowHeight="15885" tabRatio="151" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sessions" sheetId="5" r:id="rId1"/>
@@ -787,7 +787,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="10" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A36" sqref="A36"/>
+      <selection pane="bottomLeft" activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1660,10 +1660,10 @@
         <v>13</v>
       </c>
       <c r="C34" s="8">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D34" s="8">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E34" s="8"/>
       <c r="F34" s="8"/>

</xml_diff>

<commit_message>
batch fix for Energy Security Cost Factors File
Signed-off-by: kevinanewman <newman.kevin@epa.gov>
</commit_message>
<xml_diff>
--- a/input_samples/multiple_session_batch.xlsx
+++ b/input_samples/multiple_session_batch.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\GitHub\EPA_OMEGA_Model\input_samples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{759324E0-4D82-4B30-A2C1-7F007DE3FA33}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38E8DA31-A063-421A-BB92-D3AE5CF6027E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3810" yWindow="1485" windowWidth="20325" windowHeight="15885" tabRatio="151" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2250" yWindow="570" windowWidth="15690" windowHeight="19695" tabRatio="151" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sessions" sheetId="5" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="78">
   <si>
     <t>Parameter</t>
   </si>
@@ -264,6 +264,12 @@
   </si>
   <si>
     <t>Num Tech Options per BEV Vehicle</t>
+  </si>
+  <si>
+    <t>Context Energy Security Cost Factors File</t>
+  </si>
+  <si>
+    <t>input_samples/context_cost_factors-energysecurity.csv</t>
   </si>
 </sst>
 </file>
@@ -783,11 +789,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AG49"/>
+  <dimension ref="A1:AG50"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="10" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D35" sqref="D35"/>
+      <selection pane="bottomLeft" activeCell="A50" sqref="A50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2092,6 +2098,35 @@
       <c r="R49" s="22"/>
       <c r="S49" s="22"/>
     </row>
+    <row r="50" spans="1:19" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="29" t="s">
+        <v>76</v>
+      </c>
+      <c r="B50" s="27" t="s">
+        <v>3</v>
+      </c>
+      <c r="C50" s="28" t="s">
+        <v>77</v>
+      </c>
+      <c r="D50" s="28" t="s">
+        <v>77</v>
+      </c>
+      <c r="E50" s="28"/>
+      <c r="F50" s="28"/>
+      <c r="G50" s="28"/>
+      <c r="H50" s="28"/>
+      <c r="I50" s="28"/>
+      <c r="J50" s="28"/>
+      <c r="K50" s="28"/>
+      <c r="L50" s="28"/>
+      <c r="M50" s="28"/>
+      <c r="N50" s="28"/>
+      <c r="O50" s="28"/>
+      <c r="P50" s="28"/>
+      <c r="Q50" s="28"/>
+      <c r="R50" s="28"/>
+      <c r="S50" s="28"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Adding cost_factors_congestion_noise.py and context_cost_factors-congestion-noise.csv. Adding congestion and noise calcs to social_costs.py. Adding oil_import_fraction to energy security calcs. I think I made all needed changes to __init__.py, omega2.py, run_omega_batch.py and batch input files.
</commit_message>
<xml_diff>
--- a/input_samples/multiple_session_batch.xlsx
+++ b/input_samples/multiple_session_batch.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\GitHub\EPA_OMEGA_Model\input_samples\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TSHERWOO\Documents\GitHub\EPA_OMEGA_Model\input_samples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38E8DA31-A063-421A-BB92-D3AE5CF6027E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C36D698B-BCDA-4D5F-B204-535E994DAB96}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2250" yWindow="570" windowWidth="15690" windowHeight="19695" tabRatio="151" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" tabRatio="151" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sessions" sheetId="5" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="80">
   <si>
     <t>Parameter</t>
   </si>
@@ -116,9 +116,6 @@
     <t>ActionAlternative</t>
   </si>
   <si>
-    <t>FALSE, TRUE</t>
-  </si>
-  <si>
     <t>Demanded Shares File</t>
   </si>
   <si>
@@ -270,6 +267,15 @@
   </si>
   <si>
     <t>input_samples/context_cost_factors-energysecurity.csv</t>
+  </si>
+  <si>
+    <t>Context Congestion-Noise Cost Factors File</t>
+  </si>
+  <si>
+    <t>input_samples/context_cost_factors-congestion-noise.csv</t>
+  </si>
+  <si>
+    <t>TRUE, FALSE</t>
   </si>
 </sst>
 </file>
@@ -789,26 +795,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AG50"/>
+  <dimension ref="A1:AG51"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="10" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A50" sqref="A50"/>
+      <pane ySplit="10" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C39" sqref="C39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="42" style="11" customWidth="1"/>
-    <col min="2" max="2" width="17.28515625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="17.33203125" style="1" customWidth="1"/>
     <col min="3" max="4" width="48" style="11" bestFit="1" customWidth="1"/>
-    <col min="5" max="17" width="21.28515625" style="11" customWidth="1"/>
-    <col min="18" max="18" width="16.7109375" style="1" customWidth="1"/>
+    <col min="5" max="17" width="21.33203125" style="11" customWidth="1"/>
+    <col min="18" max="18" width="16.6640625" style="1" customWidth="1"/>
     <col min="19" max="19" width="18" style="1" customWidth="1"/>
-    <col min="20" max="20" width="16.42578125" style="1" customWidth="1"/>
-    <col min="21" max="16384" width="8.7109375" style="1"/>
+    <col min="20" max="20" width="16.44140625" style="1" customWidth="1"/>
+    <col min="21" max="16384" width="8.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" s="18" customFormat="1" ht="21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:33" s="18" customFormat="1" ht="21" x14ac:dyDescent="0.3">
       <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
@@ -849,7 +855,7 @@
       <c r="AF1" s="17"/>
       <c r="AG1" s="17"/>
     </row>
-    <row r="2" spans="1:33" s="12" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:33" s="12" customFormat="1" ht="18" x14ac:dyDescent="0.3">
       <c r="A2" s="19" t="s">
         <v>10</v>
       </c>
@@ -869,7 +875,7 @@
       <c r="P2" s="14"/>
       <c r="Q2" s="14"/>
     </row>
-    <row r="3" spans="1:33" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:33" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
         <v>4</v>
       </c>
@@ -877,7 +883,7 @@
         <v>3</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D3" s="14"/>
       <c r="E3" s="14"/>
@@ -894,9 +900,9 @@
       <c r="P3" s="14"/>
       <c r="Q3" s="14"/>
     </row>
-    <row r="4" spans="1:33" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:33" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B4" s="6" t="s">
         <v>3</v>
@@ -917,29 +923,29 @@
       <c r="P4" s="14"/>
       <c r="Q4" s="14"/>
     </row>
-    <row r="5" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B5" s="6" t="s">
         <v>3</v>
       </c>
       <c r="C5" s="7" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="6" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="A6" s="7" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="6" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A6" s="7" t="s">
+      <c r="B6" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="B6" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="7" spans="1:33" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:33" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="14"/>
       <c r="C7" s="14"/>
       <c r="D7" s="14"/>
@@ -957,7 +963,7 @@
       <c r="P7" s="14"/>
       <c r="Q7" s="14"/>
     </row>
-    <row r="8" spans="1:33" s="12" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:33" s="12" customFormat="1" ht="18" x14ac:dyDescent="0.3">
       <c r="A8" s="20" t="s">
         <v>9</v>
       </c>
@@ -977,7 +983,7 @@
       <c r="P8" s="14"/>
       <c r="Q8" s="14"/>
     </row>
-    <row r="9" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="8" t="s">
         <v>5</v>
       </c>
@@ -988,7 +994,7 @@
         <v>1</v>
       </c>
       <c r="D9" s="8" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E9" s="8"/>
       <c r="F9" s="8"/>
@@ -1006,7 +1012,7 @@
       <c r="R9" s="8"/>
       <c r="S9" s="8"/>
     </row>
-    <row r="10" spans="1:33" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:33" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A10" s="9" t="s">
         <v>2</v>
       </c>
@@ -1014,7 +1020,7 @@
         <v>3</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D10" s="9" t="s">
         <v>25</v>
@@ -1035,7 +1041,7 @@
       <c r="R10" s="9"/>
       <c r="S10" s="9"/>
     </row>
-    <row r="11" spans="1:33" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:33" s="16" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A11" s="15"/>
       <c r="C11" s="15"/>
       <c r="D11" s="15"/>
@@ -1055,7 +1061,7 @@
       <c r="R11" s="14"/>
       <c r="S11" s="14"/>
     </row>
-    <row r="12" spans="1:33" s="12" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:33" s="12" customFormat="1" ht="18" x14ac:dyDescent="0.3">
       <c r="A12" s="13" t="s">
         <v>6</v>
       </c>
@@ -1077,7 +1083,7 @@
       <c r="R12" s="14"/>
       <c r="S12" s="14"/>
     </row>
-    <row r="13" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A13" s="8" t="s">
         <v>14</v>
       </c>
@@ -1085,10 +1091,10 @@
         <v>3</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E13" s="8"/>
       <c r="F13" s="8"/>
@@ -1106,7 +1112,7 @@
       <c r="R13" s="8"/>
       <c r="S13" s="8"/>
     </row>
-    <row r="14" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A14" s="8" t="s">
         <v>16</v>
       </c>
@@ -1114,10 +1120,10 @@
         <v>3</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E14" s="8"/>
       <c r="F14" s="8"/>
@@ -1135,7 +1141,7 @@
       <c r="R14" s="8"/>
       <c r="S14" s="8"/>
     </row>
-    <row r="15" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A15" s="8" t="s">
         <v>17</v>
       </c>
@@ -1143,10 +1149,10 @@
         <v>3</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E15" s="8"/>
       <c r="F15" s="8"/>
@@ -1164,18 +1170,18 @@
       <c r="R15" s="8"/>
       <c r="S15" s="8"/>
     </row>
-    <row r="16" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A16" s="8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>3</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E16" s="8"/>
       <c r="F16" s="8"/>
@@ -1193,7 +1199,7 @@
       <c r="R16" s="8"/>
       <c r="S16" s="8"/>
     </row>
-    <row r="17" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A17" s="8" t="s">
         <v>19</v>
       </c>
@@ -1201,10 +1207,10 @@
         <v>3</v>
       </c>
       <c r="C17" s="8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E17" s="8"/>
       <c r="F17" s="8"/>
@@ -1222,18 +1228,18 @@
       <c r="R17" s="8"/>
       <c r="S17" s="8"/>
     </row>
-    <row r="18" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A18" s="8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>3</v>
       </c>
       <c r="C18" s="8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D18" s="8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E18" s="8"/>
       <c r="F18" s="8"/>
@@ -1251,18 +1257,18 @@
       <c r="R18" s="8"/>
       <c r="S18" s="8"/>
     </row>
-    <row r="19" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A19" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C19" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="B19" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C19" s="8" t="s">
-        <v>54</v>
-      </c>
       <c r="D19" s="8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E19" s="8"/>
       <c r="F19" s="8"/>
@@ -1280,18 +1286,18 @@
       <c r="R19" s="8"/>
       <c r="S19" s="8"/>
     </row>
-    <row r="20" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A20" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C20" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="B20" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C20" s="8" t="s">
-        <v>48</v>
-      </c>
       <c r="D20" s="8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E20" s="8"/>
       <c r="F20" s="8"/>
@@ -1309,7 +1315,7 @@
       <c r="R20" s="8"/>
       <c r="S20" s="8"/>
     </row>
-    <row r="21" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A21" s="8" t="s">
         <v>18</v>
       </c>
@@ -1317,10 +1323,10 @@
         <v>3</v>
       </c>
       <c r="C21" s="8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D21" s="8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E21" s="8"/>
       <c r="F21" s="8"/>
@@ -1338,7 +1344,7 @@
       <c r="R21" s="8"/>
       <c r="S21" s="8"/>
     </row>
-    <row r="22" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A22" s="8" t="s">
         <v>20</v>
       </c>
@@ -1346,10 +1352,10 @@
         <v>3</v>
       </c>
       <c r="C22" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D22" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E22" s="8"/>
       <c r="F22" s="8"/>
@@ -1367,7 +1373,7 @@
       <c r="R22" s="8"/>
       <c r="S22" s="8"/>
     </row>
-    <row r="23" spans="1:19" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:19" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A23" s="10" t="s">
         <v>21</v>
       </c>
@@ -1375,10 +1381,10 @@
         <v>3</v>
       </c>
       <c r="C23" s="10" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D23" s="10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E23" s="10"/>
       <c r="F23" s="10"/>
@@ -1396,18 +1402,18 @@
       <c r="R23" s="10"/>
       <c r="S23" s="10"/>
     </row>
-    <row r="24" spans="1:19" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:19" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A24" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>3</v>
       </c>
       <c r="C24" s="8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D24" s="8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E24" s="10"/>
       <c r="F24" s="10"/>
@@ -1425,18 +1431,18 @@
       <c r="R24" s="10"/>
       <c r="S24" s="10"/>
     </row>
-    <row r="25" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A25" s="8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B25" s="2" t="s">
         <v>3</v>
       </c>
       <c r="C25" s="8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D25" s="8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E25" s="8"/>
       <c r="F25" s="8"/>
@@ -1454,18 +1460,18 @@
       <c r="R25" s="8"/>
       <c r="S25" s="8"/>
     </row>
-    <row r="26" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A26" s="23" t="s">
+        <v>54</v>
+      </c>
+      <c r="B26" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="C26" s="22" t="s">
         <v>55</v>
       </c>
-      <c r="B26" s="21" t="s">
-        <v>3</v>
-      </c>
-      <c r="C26" s="22" t="s">
-        <v>56</v>
-      </c>
       <c r="D26" s="22" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E26" s="8"/>
       <c r="F26" s="8"/>
@@ -1483,18 +1489,18 @@
       <c r="R26" s="8"/>
       <c r="S26" s="8"/>
     </row>
-    <row r="27" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A27" s="23" t="s">
+        <v>56</v>
+      </c>
+      <c r="B27" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="C27" s="22" t="s">
         <v>57</v>
       </c>
-      <c r="B27" s="21" t="s">
-        <v>3</v>
-      </c>
-      <c r="C27" s="22" t="s">
-        <v>58</v>
-      </c>
       <c r="D27" s="22" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E27" s="8"/>
       <c r="F27" s="8"/>
@@ -1512,7 +1518,7 @@
       <c r="R27" s="8"/>
       <c r="S27" s="8"/>
     </row>
-    <row r="28" spans="1:19" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:19" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A28" s="10" t="s">
         <v>15</v>
       </c>
@@ -1541,7 +1547,7 @@
       <c r="R28" s="10"/>
       <c r="S28" s="10"/>
     </row>
-    <row r="29" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A29" s="10" t="s">
         <v>22</v>
       </c>
@@ -1570,7 +1576,7 @@
       <c r="R29" s="8"/>
       <c r="S29" s="8"/>
     </row>
-    <row r="30" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="E30" s="8"/>
       <c r="F30" s="8"/>
       <c r="G30" s="8"/>
@@ -1587,7 +1593,7 @@
       <c r="R30" s="8"/>
       <c r="S30" s="8"/>
     </row>
-    <row r="31" spans="1:19" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:19" s="16" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A31" s="15"/>
       <c r="C31" s="15"/>
       <c r="D31" s="15"/>
@@ -1607,7 +1613,7 @@
       <c r="R31" s="14"/>
       <c r="S31" s="14"/>
     </row>
-    <row r="32" spans="1:19" s="12" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:19" s="12" customFormat="1" ht="18" x14ac:dyDescent="0.3">
       <c r="A32" s="20" t="s">
         <v>8</v>
       </c>
@@ -1629,9 +1635,9 @@
       <c r="R32" s="14"/>
       <c r="S32" s="14"/>
     </row>
-    <row r="33" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A33" s="8" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B33" s="3" t="s">
         <v>13</v>
@@ -1658,9 +1664,9 @@
       <c r="R33" s="8"/>
       <c r="S33" s="8"/>
     </row>
-    <row r="34" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A34" s="8" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B34" s="3" t="s">
         <v>13</v>
@@ -1687,9 +1693,9 @@
       <c r="R34" s="8"/>
       <c r="S34" s="8"/>
     </row>
-    <row r="35" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A35" s="8" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B35" s="3" t="s">
         <v>13</v>
@@ -1716,7 +1722,7 @@
       <c r="R35" s="8"/>
       <c r="S35" s="8"/>
     </row>
-    <row r="36" spans="1:19" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:19" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A36" s="10" t="s">
         <v>23</v>
       </c>
@@ -1727,7 +1733,7 @@
         <v>0</v>
       </c>
       <c r="D36" s="10" t="s">
-        <v>26</v>
+        <v>79</v>
       </c>
       <c r="E36" s="10"/>
       <c r="F36" s="10"/>
@@ -1745,7 +1751,7 @@
       <c r="R36" s="10"/>
       <c r="S36" s="10"/>
     </row>
-    <row r="37" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A37" s="10" t="s">
         <v>24</v>
       </c>
@@ -1774,15 +1780,15 @@
       <c r="R37" s="8"/>
       <c r="S37" s="8"/>
     </row>
-    <row r="38" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A38" s="8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B38" s="3" t="s">
         <v>11</v>
       </c>
       <c r="C38" s="8" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D38" s="8" t="b">
         <v>1</v>
@@ -1803,9 +1809,9 @@
       <c r="R38" s="8"/>
       <c r="S38" s="8"/>
     </row>
-    <row r="39" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A39" s="8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B39" s="3" t="s">
         <v>13</v>
@@ -1832,7 +1838,7 @@
       <c r="R39" s="8"/>
       <c r="S39" s="8"/>
     </row>
-    <row r="40" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A40" s="8"/>
       <c r="B40" s="3"/>
       <c r="C40" s="8"/>
@@ -1853,7 +1859,7 @@
       <c r="R40" s="8"/>
       <c r="S40" s="8"/>
     </row>
-    <row r="41" spans="1:19" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:19" s="16" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A41" s="15"/>
       <c r="C41" s="15"/>
       <c r="D41" s="15"/>
@@ -1873,7 +1879,7 @@
       <c r="R41" s="14"/>
       <c r="S41" s="14"/>
     </row>
-    <row r="42" spans="1:19" s="12" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:19" s="12" customFormat="1" ht="18" x14ac:dyDescent="0.3">
       <c r="A42" s="20" t="s">
         <v>7</v>
       </c>
@@ -1895,18 +1901,18 @@
       <c r="R42" s="14"/>
       <c r="S42" s="14"/>
     </row>
-    <row r="43" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A43" s="26" t="s">
+        <v>58</v>
+      </c>
+      <c r="B43" s="24" t="s">
+        <v>3</v>
+      </c>
+      <c r="C43" s="25" t="s">
         <v>59</v>
       </c>
-      <c r="B43" s="24" t="s">
-        <v>3</v>
-      </c>
-      <c r="C43" s="25" t="s">
-        <v>60</v>
-      </c>
       <c r="D43" s="25" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E43" s="8"/>
       <c r="F43" s="8"/>
@@ -1924,18 +1930,18 @@
       <c r="R43" s="8"/>
       <c r="S43" s="8"/>
     </row>
-    <row r="44" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A44" s="26" t="s">
+        <v>60</v>
+      </c>
+      <c r="B44" s="24" t="s">
+        <v>3</v>
+      </c>
+      <c r="C44" s="25" t="s">
         <v>61</v>
       </c>
-      <c r="B44" s="24" t="s">
-        <v>3</v>
-      </c>
-      <c r="C44" s="25" t="s">
-        <v>62</v>
-      </c>
       <c r="D44" s="25" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E44" s="8"/>
       <c r="F44" s="8"/>
@@ -1953,76 +1959,76 @@
       <c r="R44" s="8"/>
       <c r="S44" s="8"/>
     </row>
-    <row r="45" spans="1:19" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="26" t="s">
+    <row r="45" spans="1:19" s="21" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="29" t="s">
+        <v>75</v>
+      </c>
+      <c r="B45" s="27" t="s">
+        <v>3</v>
+      </c>
+      <c r="C45" s="28" t="s">
+        <v>76</v>
+      </c>
+      <c r="D45" s="28" t="s">
+        <v>76</v>
+      </c>
+      <c r="E45" s="28"/>
+      <c r="F45" s="28"/>
+      <c r="G45" s="28"/>
+      <c r="H45" s="28"/>
+      <c r="I45" s="28"/>
+      <c r="J45" s="28"/>
+      <c r="K45" s="28"/>
+      <c r="L45" s="28"/>
+      <c r="M45" s="28"/>
+      <c r="N45" s="28"/>
+      <c r="O45" s="28"/>
+      <c r="P45" s="28"/>
+      <c r="Q45" s="28"/>
+      <c r="R45" s="28"/>
+      <c r="S45" s="28"/>
+    </row>
+    <row r="46" spans="1:19" s="21" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="29" t="s">
+        <v>77</v>
+      </c>
+      <c r="B46" s="27" t="s">
+        <v>3</v>
+      </c>
+      <c r="C46" s="28" t="s">
+        <v>78</v>
+      </c>
+      <c r="D46" s="28" t="s">
+        <v>78</v>
+      </c>
+      <c r="E46" s="28"/>
+      <c r="F46" s="28"/>
+      <c r="G46" s="28"/>
+      <c r="H46" s="28"/>
+      <c r="I46" s="28"/>
+      <c r="J46" s="28"/>
+      <c r="K46" s="28"/>
+      <c r="L46" s="28"/>
+      <c r="M46" s="28"/>
+      <c r="N46" s="28"/>
+      <c r="O46" s="28"/>
+      <c r="P46" s="28"/>
+      <c r="Q46" s="28"/>
+      <c r="R46" s="28"/>
+      <c r="S46" s="28"/>
+    </row>
+    <row r="47" spans="1:19" s="21" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="26" t="s">
+        <v>62</v>
+      </c>
+      <c r="B47" s="24" t="s">
+        <v>3</v>
+      </c>
+      <c r="C47" s="25" t="s">
         <v>63</v>
       </c>
-      <c r="B45" s="24" t="s">
-        <v>3</v>
-      </c>
-      <c r="C45" s="25" t="s">
-        <v>64</v>
-      </c>
-      <c r="D45" s="25" t="s">
-        <v>64</v>
-      </c>
-      <c r="E45" s="22"/>
-      <c r="F45" s="22"/>
-      <c r="G45" s="22"/>
-      <c r="H45" s="22"/>
-      <c r="I45" s="22"/>
-      <c r="J45" s="22"/>
-      <c r="K45" s="22"/>
-      <c r="L45" s="22"/>
-      <c r="M45" s="22"/>
-      <c r="N45" s="22"/>
-      <c r="O45" s="22"/>
-      <c r="P45" s="22"/>
-      <c r="Q45" s="22"/>
-      <c r="R45" s="22"/>
-      <c r="S45" s="22"/>
-    </row>
-    <row r="46" spans="1:19" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="26" t="s">
-        <v>65</v>
-      </c>
-      <c r="B46" s="24" t="s">
-        <v>3</v>
-      </c>
-      <c r="C46" s="25" t="s">
-        <v>66</v>
-      </c>
-      <c r="D46" s="25" t="s">
-        <v>66</v>
-      </c>
-      <c r="E46" s="22"/>
-      <c r="F46" s="22"/>
-      <c r="G46" s="22"/>
-      <c r="H46" s="22"/>
-      <c r="I46" s="22"/>
-      <c r="J46" s="22"/>
-      <c r="K46" s="22"/>
-      <c r="L46" s="22"/>
-      <c r="M46" s="22"/>
-      <c r="N46" s="22"/>
-      <c r="O46" s="22"/>
-      <c r="P46" s="22"/>
-      <c r="Q46" s="22"/>
-      <c r="R46" s="22"/>
-      <c r="S46" s="22"/>
-    </row>
-    <row r="47" spans="1:19" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="26" t="s">
-        <v>67</v>
-      </c>
-      <c r="B47" s="24" t="s">
-        <v>3</v>
-      </c>
-      <c r="C47" s="25" t="s">
-        <v>68</v>
-      </c>
       <c r="D47" s="25" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="E47" s="22"/>
       <c r="F47" s="22"/>
@@ -2040,18 +2046,18 @@
       <c r="R47" s="22"/>
       <c r="S47" s="22"/>
     </row>
-    <row r="48" spans="1:19" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="29" t="s">
-        <v>69</v>
-      </c>
-      <c r="B48" s="27" t="s">
-        <v>3</v>
-      </c>
-      <c r="C48" s="28" t="s">
-        <v>70</v>
-      </c>
-      <c r="D48" s="28" t="s">
-        <v>70</v>
+    <row r="48" spans="1:19" s="21" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="26" t="s">
+        <v>64</v>
+      </c>
+      <c r="B48" s="24" t="s">
+        <v>3</v>
+      </c>
+      <c r="C48" s="25" t="s">
+        <v>65</v>
+      </c>
+      <c r="D48" s="25" t="s">
+        <v>65</v>
       </c>
       <c r="E48" s="22"/>
       <c r="F48" s="22"/>
@@ -2069,18 +2075,18 @@
       <c r="R48" s="22"/>
       <c r="S48" s="22"/>
     </row>
-    <row r="49" spans="1:19" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="28" t="s">
-        <v>71</v>
-      </c>
-      <c r="B49" s="27" t="s">
-        <v>3</v>
-      </c>
-      <c r="C49" s="28" t="s">
-        <v>72</v>
-      </c>
-      <c r="D49" s="28" t="s">
-        <v>72</v>
+    <row r="49" spans="1:19" s="21" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="26" t="s">
+        <v>66</v>
+      </c>
+      <c r="B49" s="24" t="s">
+        <v>3</v>
+      </c>
+      <c r="C49" s="25" t="s">
+        <v>67</v>
+      </c>
+      <c r="D49" s="25" t="s">
+        <v>67</v>
       </c>
       <c r="E49" s="22"/>
       <c r="F49" s="22"/>
@@ -2098,34 +2104,63 @@
       <c r="R49" s="22"/>
       <c r="S49" s="22"/>
     </row>
-    <row r="50" spans="1:19" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:19" s="21" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A50" s="29" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="B50" s="27" t="s">
         <v>3</v>
       </c>
       <c r="C50" s="28" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="D50" s="28" t="s">
-        <v>77</v>
-      </c>
-      <c r="E50" s="28"/>
-      <c r="F50" s="28"/>
-      <c r="G50" s="28"/>
-      <c r="H50" s="28"/>
-      <c r="I50" s="28"/>
-      <c r="J50" s="28"/>
-      <c r="K50" s="28"/>
-      <c r="L50" s="28"/>
-      <c r="M50" s="28"/>
-      <c r="N50" s="28"/>
-      <c r="O50" s="28"/>
-      <c r="P50" s="28"/>
-      <c r="Q50" s="28"/>
-      <c r="R50" s="28"/>
-      <c r="S50" s="28"/>
+        <v>69</v>
+      </c>
+      <c r="E50" s="22"/>
+      <c r="F50" s="22"/>
+      <c r="G50" s="22"/>
+      <c r="H50" s="22"/>
+      <c r="I50" s="22"/>
+      <c r="J50" s="22"/>
+      <c r="K50" s="22"/>
+      <c r="L50" s="22"/>
+      <c r="M50" s="22"/>
+      <c r="N50" s="22"/>
+      <c r="O50" s="22"/>
+      <c r="P50" s="22"/>
+      <c r="Q50" s="22"/>
+      <c r="R50" s="22"/>
+      <c r="S50" s="22"/>
+    </row>
+    <row r="51" spans="1:19" s="21" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A51" s="28" t="s">
+        <v>70</v>
+      </c>
+      <c r="B51" s="27" t="s">
+        <v>3</v>
+      </c>
+      <c r="C51" s="28" t="s">
+        <v>71</v>
+      </c>
+      <c r="D51" s="28" t="s">
+        <v>71</v>
+      </c>
+      <c r="E51" s="22"/>
+      <c r="F51" s="22"/>
+      <c r="G51" s="22"/>
+      <c r="H51" s="22"/>
+      <c r="I51" s="22"/>
+      <c r="J51" s="22"/>
+      <c r="K51" s="22"/>
+      <c r="L51" s="22"/>
+      <c r="M51" s="22"/>
+      <c r="N51" s="22"/>
+      <c r="O51" s="22"/>
+      <c r="P51" s="22"/>
+      <c r="Q51" s="22"/>
+      <c r="R51" s="22"/>
+      <c r="S51" s="22"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Update GUI Plotting for Multiple Scenarios
</commit_message>
<xml_diff>
--- a/input_samples/multiple_session_batch.xlsx
+++ b/input_samples/multiple_session_batch.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TSHERWOO\Documents\GitHub\EPA_OMEGA_Model\input_samples\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jcherr01\OneDrive - Environmental Protection Agency (EPA)\Documents\Jeff Documents\GitHub\EPA_OMEGA_Model\input_samples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C36D698B-BCDA-4D5F-B204-535E994DAB96}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{C36D698B-BCDA-4D5F-B204-535E994DAB96}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{07C7DCEA-BDC2-4CF2-8A9F-5A1B2A5BC804}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" tabRatio="151" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="151" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sessions" sheetId="5" r:id="rId1"/>
@@ -799,22 +799,22 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="10" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C39" sqref="C39"/>
+      <selection pane="bottomLeft" activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="42" style="11" customWidth="1"/>
-    <col min="2" max="2" width="17.33203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="17.28515625" style="1" customWidth="1"/>
     <col min="3" max="4" width="48" style="11" bestFit="1" customWidth="1"/>
-    <col min="5" max="17" width="21.33203125" style="11" customWidth="1"/>
-    <col min="18" max="18" width="16.6640625" style="1" customWidth="1"/>
+    <col min="5" max="17" width="21.28515625" style="11" customWidth="1"/>
+    <col min="18" max="18" width="16.7109375" style="1" customWidth="1"/>
     <col min="19" max="19" width="18" style="1" customWidth="1"/>
-    <col min="20" max="20" width="16.44140625" style="1" customWidth="1"/>
-    <col min="21" max="16384" width="8.6640625" style="1"/>
+    <col min="20" max="20" width="16.42578125" style="1" customWidth="1"/>
+    <col min="21" max="16384" width="8.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" s="18" customFormat="1" ht="21" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:33" s="18" customFormat="1" ht="21" x14ac:dyDescent="0.25">
       <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
@@ -855,7 +855,7 @@
       <c r="AF1" s="17"/>
       <c r="AG1" s="17"/>
     </row>
-    <row r="2" spans="1:33" s="12" customFormat="1" ht="18" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:33" s="12" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A2" s="19" t="s">
         <v>10</v>
       </c>
@@ -875,7 +875,7 @@
       <c r="P2" s="14"/>
       <c r="Q2" s="14"/>
     </row>
-    <row r="3" spans="1:33" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:33" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>4</v>
       </c>
@@ -900,7 +900,7 @@
       <c r="P3" s="14"/>
       <c r="Q3" s="14"/>
     </row>
-    <row r="4" spans="1:33" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:33" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>30</v>
       </c>
@@ -923,7 +923,7 @@
       <c r="P4" s="14"/>
       <c r="Q4" s="14"/>
     </row>
-    <row r="5" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>29</v>
       </c>
@@ -934,7 +934,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="6" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>49</v>
       </c>
@@ -945,7 +945,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="7" spans="1:33" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:33" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="14"/>
       <c r="C7" s="14"/>
       <c r="D7" s="14"/>
@@ -963,7 +963,7 @@
       <c r="P7" s="14"/>
       <c r="Q7" s="14"/>
     </row>
-    <row r="8" spans="1:33" s="12" customFormat="1" ht="18" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:33" s="12" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A8" s="20" t="s">
         <v>9</v>
       </c>
@@ -983,7 +983,7 @@
       <c r="P8" s="14"/>
       <c r="Q8" s="14"/>
     </row>
-    <row r="9" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
         <v>5</v>
       </c>
@@ -1012,7 +1012,7 @@
       <c r="R9" s="8"/>
       <c r="S9" s="8"/>
     </row>
-    <row r="10" spans="1:33" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:33" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
         <v>2</v>
       </c>
@@ -1041,7 +1041,7 @@
       <c r="R10" s="9"/>
       <c r="S10" s="9"/>
     </row>
-    <row r="11" spans="1:33" s="16" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:33" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="15"/>
       <c r="C11" s="15"/>
       <c r="D11" s="15"/>
@@ -1061,7 +1061,7 @@
       <c r="R11" s="14"/>
       <c r="S11" s="14"/>
     </row>
-    <row r="12" spans="1:33" s="12" customFormat="1" ht="18" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:33" s="12" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A12" s="13" t="s">
         <v>6</v>
       </c>
@@ -1083,7 +1083,7 @@
       <c r="R12" s="14"/>
       <c r="S12" s="14"/>
     </row>
-    <row r="13" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
         <v>14</v>
       </c>
@@ -1112,7 +1112,7 @@
       <c r="R13" s="8"/>
       <c r="S13" s="8"/>
     </row>
-    <row r="14" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="8" t="s">
         <v>16</v>
       </c>
@@ -1141,7 +1141,7 @@
       <c r="R14" s="8"/>
       <c r="S14" s="8"/>
     </row>
-    <row r="15" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="8" t="s">
         <v>17</v>
       </c>
@@ -1170,7 +1170,7 @@
       <c r="R15" s="8"/>
       <c r="S15" s="8"/>
     </row>
-    <row r="16" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="8" t="s">
         <v>26</v>
       </c>
@@ -1199,7 +1199,7 @@
       <c r="R16" s="8"/>
       <c r="S16" s="8"/>
     </row>
-    <row r="17" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="8" t="s">
         <v>19</v>
       </c>
@@ -1228,7 +1228,7 @@
       <c r="R17" s="8"/>
       <c r="S17" s="8"/>
     </row>
-    <row r="18" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="8" t="s">
         <v>45</v>
       </c>
@@ -1257,7 +1257,7 @@
       <c r="R18" s="8"/>
       <c r="S18" s="8"/>
     </row>
-    <row r="19" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="8" t="s">
         <v>52</v>
       </c>
@@ -1286,7 +1286,7 @@
       <c r="R19" s="8"/>
       <c r="S19" s="8"/>
     </row>
-    <row r="20" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="8" t="s">
         <v>46</v>
       </c>
@@ -1315,7 +1315,7 @@
       <c r="R20" s="8"/>
       <c r="S20" s="8"/>
     </row>
-    <row r="21" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="8" t="s">
         <v>18</v>
       </c>
@@ -1344,7 +1344,7 @@
       <c r="R21" s="8"/>
       <c r="S21" s="8"/>
     </row>
-    <row r="22" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="8" t="s">
         <v>20</v>
       </c>
@@ -1373,7 +1373,7 @@
       <c r="R22" s="8"/>
       <c r="S22" s="8"/>
     </row>
-    <row r="23" spans="1:19" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:19" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="10" t="s">
         <v>21</v>
       </c>
@@ -1402,7 +1402,7 @@
       <c r="R23" s="10"/>
       <c r="S23" s="10"/>
     </row>
-    <row r="24" spans="1:19" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:19" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="8" t="s">
         <v>31</v>
       </c>
@@ -1431,7 +1431,7 @@
       <c r="R24" s="10"/>
       <c r="S24" s="10"/>
     </row>
-    <row r="25" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="8" t="s">
         <v>32</v>
       </c>
@@ -1460,7 +1460,7 @@
       <c r="R25" s="8"/>
       <c r="S25" s="8"/>
     </row>
-    <row r="26" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="23" t="s">
         <v>54</v>
       </c>
@@ -1489,7 +1489,7 @@
       <c r="R26" s="8"/>
       <c r="S26" s="8"/>
     </row>
-    <row r="27" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="23" t="s">
         <v>56</v>
       </c>
@@ -1518,7 +1518,7 @@
       <c r="R27" s="8"/>
       <c r="S27" s="8"/>
     </row>
-    <row r="28" spans="1:19" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:19" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="10" t="s">
         <v>15</v>
       </c>
@@ -1547,7 +1547,7 @@
       <c r="R28" s="10"/>
       <c r="S28" s="10"/>
     </row>
-    <row r="29" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="10" t="s">
         <v>22</v>
       </c>
@@ -1576,7 +1576,7 @@
       <c r="R29" s="8"/>
       <c r="S29" s="8"/>
     </row>
-    <row r="30" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E30" s="8"/>
       <c r="F30" s="8"/>
       <c r="G30" s="8"/>
@@ -1593,7 +1593,7 @@
       <c r="R30" s="8"/>
       <c r="S30" s="8"/>
     </row>
-    <row r="31" spans="1:19" s="16" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:19" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="15"/>
       <c r="C31" s="15"/>
       <c r="D31" s="15"/>
@@ -1613,7 +1613,7 @@
       <c r="R31" s="14"/>
       <c r="S31" s="14"/>
     </row>
-    <row r="32" spans="1:19" s="12" customFormat="1" ht="18" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:19" s="12" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A32" s="20" t="s">
         <v>8</v>
       </c>
@@ -1635,7 +1635,7 @@
       <c r="R32" s="14"/>
       <c r="S32" s="14"/>
     </row>
-    <row r="33" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="8" t="s">
         <v>72</v>
       </c>
@@ -1664,7 +1664,7 @@
       <c r="R33" s="8"/>
       <c r="S33" s="8"/>
     </row>
-    <row r="34" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="8" t="s">
         <v>73</v>
       </c>
@@ -1693,7 +1693,7 @@
       <c r="R34" s="8"/>
       <c r="S34" s="8"/>
     </row>
-    <row r="35" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="8" t="s">
         <v>74</v>
       </c>
@@ -1722,7 +1722,7 @@
       <c r="R35" s="8"/>
       <c r="S35" s="8"/>
     </row>
-    <row r="36" spans="1:19" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:19" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="10" t="s">
         <v>23</v>
       </c>
@@ -1751,7 +1751,7 @@
       <c r="R36" s="10"/>
       <c r="S36" s="10"/>
     </row>
-    <row r="37" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="10" t="s">
         <v>24</v>
       </c>
@@ -1780,7 +1780,7 @@
       <c r="R37" s="8"/>
       <c r="S37" s="8"/>
     </row>
-    <row r="38" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="8" t="s">
         <v>33</v>
       </c>
@@ -1809,7 +1809,7 @@
       <c r="R38" s="8"/>
       <c r="S38" s="8"/>
     </row>
-    <row r="39" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="8" t="s">
         <v>51</v>
       </c>
@@ -1838,7 +1838,7 @@
       <c r="R39" s="8"/>
       <c r="S39" s="8"/>
     </row>
-    <row r="40" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="8"/>
       <c r="B40" s="3"/>
       <c r="C40" s="8"/>
@@ -1859,7 +1859,7 @@
       <c r="R40" s="8"/>
       <c r="S40" s="8"/>
     </row>
-    <row r="41" spans="1:19" s="16" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:19" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="15"/>
       <c r="C41" s="15"/>
       <c r="D41" s="15"/>
@@ -1879,7 +1879,7 @@
       <c r="R41" s="14"/>
       <c r="S41" s="14"/>
     </row>
-    <row r="42" spans="1:19" s="12" customFormat="1" ht="18" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:19" s="12" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A42" s="20" t="s">
         <v>7</v>
       </c>
@@ -1901,7 +1901,7 @@
       <c r="R42" s="14"/>
       <c r="S42" s="14"/>
     </row>
-    <row r="43" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="26" t="s">
         <v>58</v>
       </c>
@@ -1930,7 +1930,7 @@
       <c r="R43" s="8"/>
       <c r="S43" s="8"/>
     </row>
-    <row r="44" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44" s="26" t="s">
         <v>60</v>
       </c>
@@ -1959,7 +1959,7 @@
       <c r="R44" s="8"/>
       <c r="S44" s="8"/>
     </row>
-    <row r="45" spans="1:19" s="21" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:19" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45" s="29" t="s">
         <v>75</v>
       </c>
@@ -1988,7 +1988,7 @@
       <c r="R45" s="28"/>
       <c r="S45" s="28"/>
     </row>
-    <row r="46" spans="1:19" s="21" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:19" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A46" s="29" t="s">
         <v>77</v>
       </c>
@@ -2017,7 +2017,7 @@
       <c r="R46" s="28"/>
       <c r="S46" s="28"/>
     </row>
-    <row r="47" spans="1:19" s="21" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:19" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47" s="26" t="s">
         <v>62</v>
       </c>
@@ -2046,7 +2046,7 @@
       <c r="R47" s="22"/>
       <c r="S47" s="22"/>
     </row>
-    <row r="48" spans="1:19" s="21" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:19" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" s="26" t="s">
         <v>64</v>
       </c>
@@ -2075,7 +2075,7 @@
       <c r="R48" s="22"/>
       <c r="S48" s="22"/>
     </row>
-    <row r="49" spans="1:19" s="21" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:19" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A49" s="26" t="s">
         <v>66</v>
       </c>
@@ -2104,7 +2104,7 @@
       <c r="R49" s="22"/>
       <c r="S49" s="22"/>
     </row>
-    <row r="50" spans="1:19" s="21" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:19" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A50" s="29" t="s">
         <v>68</v>
       </c>
@@ -2133,7 +2133,7 @@
       <c r="R50" s="22"/>
       <c r="S50" s="22"/>
     </row>
-    <row r="51" spans="1:19" s="21" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:19" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A51" s="28" t="s">
         <v>70</v>
       </c>

</xml_diff>